<commit_message>
Made changes to other files, reverting changes done.
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -4,32 +4,30 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="8985" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="8985" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
     <sheet name="S205014" sheetId="2" r:id="rId2"/>
-    <sheet name="EMV_LOAD_BALANCE_AGENCY_FUNDED" sheetId="16" r:id="rId3"/>
-    <sheet name="EMV_LOAD_BALANCE_AGENCY_NONFUND" sheetId="17" r:id="rId4"/>
-    <sheet name="S205000" sheetId="3" r:id="rId5"/>
-    <sheet name="S205009" sheetId="6" r:id="rId6"/>
-    <sheet name="AccountMaster_S205195" sheetId="7" r:id="rId7"/>
-    <sheet name="AccounHeadMapping_S205175" sheetId="8" r:id="rId8"/>
-    <sheet name="AccountHead_S205168" sheetId="9" r:id="rId9"/>
-    <sheet name="SuspenseAccount_S205193" sheetId="10" r:id="rId10"/>
-    <sheet name="Institute" sheetId="5" r:id="rId11"/>
-    <sheet name="ApplicationUpload" sheetId="11" r:id="rId12"/>
-    <sheet name="AmlockDownloads" sheetId="15" r:id="rId13"/>
-    <sheet name="CurrencyExchangeRates" sheetId="12" r:id="rId14"/>
-    <sheet name="CurrencyExchangeRateUpload" sheetId="13" r:id="rId15"/>
-    <sheet name="CurrencyExchangeRateMapping" sheetId="14" r:id="rId16"/>
+    <sheet name="S205000" sheetId="3" r:id="rId3"/>
+    <sheet name="S205009" sheetId="6" r:id="rId4"/>
+    <sheet name="AccountMaster_S205195" sheetId="7" r:id="rId5"/>
+    <sheet name="AccounHeadMapping_S205175" sheetId="8" r:id="rId6"/>
+    <sheet name="AccountHead_S205168" sheetId="9" r:id="rId7"/>
+    <sheet name="SuspenseAccount_S205193" sheetId="10" r:id="rId8"/>
+    <sheet name="Institute" sheetId="5" r:id="rId9"/>
+    <sheet name="ApplicationUpload" sheetId="11" r:id="rId10"/>
+    <sheet name="AmlockDownloads" sheetId="15" r:id="rId11"/>
+    <sheet name="CurrencyExchangeRates" sheetId="12" r:id="rId12"/>
+    <sheet name="CurrencyExchangeRateUpload" sheetId="13" r:id="rId13"/>
+    <sheet name="CurrencyExchangeRateMapping" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1938" uniqueCount="711">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="457">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1400,768 +1398,6 @@
   </si>
   <si>
     <t>March/10/2050</t>
-  </si>
-  <si>
-    <t>Field Name</t>
-  </si>
-  <si>
-    <t>Values</t>
-  </si>
-  <si>
-    <t>TRANSACTION_DETAILS</t>
-  </si>
-  <si>
-    <t>INR [356]:10.00:INR [356],USD [840]:5.00:USD [840]</t>
-  </si>
-  <si>
-    <t>WalletCurrency:Amount:TransactionCurrency, &lt;next values&gt;</t>
-  </si>
-  <si>
-    <t>PAYMENT_MODE</t>
-  </si>
-  <si>
-    <t>Cash</t>
-  </si>
-  <si>
-    <t>DOCUMENTS_VERIFIED</t>
-  </si>
-  <si>
-    <t>Passport</t>
-  </si>
-  <si>
-    <t>ACTIVATION_CODE</t>
-  </si>
-  <si>
-    <t>Manual</t>
-  </si>
-  <si>
-    <t>ADVANCE_RENEWAL_REPORT</t>
-  </si>
-  <si>
-    <t>AGENCY</t>
-  </si>
-  <si>
-    <t>AUTOAGNC001 [AGNC001]</t>
-  </si>
-  <si>
-    <t>AGENCY_ID</t>
-  </si>
-  <si>
-    <t>AUTOAGNC001</t>
-  </si>
-  <si>
-    <t>AGENT_ID</t>
-  </si>
-  <si>
-    <t>AUTOAGNT007 [AGNT007]</t>
-  </si>
-  <si>
-    <t>APPLICATION_TYPE</t>
-  </si>
-  <si>
-    <t>ASSOCIATION</t>
-  </si>
-  <si>
-    <t>MASTERCARD [02]</t>
-  </si>
-  <si>
-    <t>AUTO_RENEWAL_DAYS</t>
-  </si>
-  <si>
-    <t>BRANCH</t>
-  </si>
-  <si>
-    <t>auto branch [1000]</t>
-  </si>
-  <si>
-    <t>BRANCH_ID</t>
-  </si>
-  <si>
-    <t>AUTOBRNCH001 [BRNCH001]</t>
-  </si>
-  <si>
-    <t>CALENDAR_START_MONTH</t>
-  </si>
-  <si>
-    <t>Mar [03]</t>
-  </si>
-  <si>
-    <t>CARD_PACKID_GENERATION_TEMPLATE</t>
-  </si>
-  <si>
-    <t>AUTOMATION [PAN042]</t>
-  </si>
-  <si>
-    <t>CARD_PRODUCTION</t>
-  </si>
-  <si>
-    <t>enable</t>
-  </si>
-  <si>
-    <t>CEILING_AMOUNT</t>
-  </si>
-  <si>
-    <t>CEILING_RESPONSE</t>
-  </si>
-  <si>
-    <t>Decline [1]</t>
-  </si>
-  <si>
-    <t>CHIP_TYPE</t>
-  </si>
-  <si>
-    <t>MChip [02]</t>
-  </si>
-  <si>
-    <t>CORPORATE_CLIENT_CODE</t>
-  </si>
-  <si>
-    <t>Automation [12121217222000002]</t>
-  </si>
-  <si>
-    <t>COUNTRY</t>
-  </si>
-  <si>
-    <t>COURIER_AGENCY</t>
-  </si>
-  <si>
-    <t>DTDC [C0000005]</t>
-  </si>
-  <si>
-    <t>CREATE_OPEN_BATCH</t>
-  </si>
-  <si>
-    <t>CURRENCY</t>
-  </si>
-  <si>
-    <t>CURRENCY_CONVERSION_BY</t>
-  </si>
-  <si>
-    <t>CURRENT_ADDRESS_LINE_1</t>
-  </si>
-  <si>
-    <t>Current Address</t>
-  </si>
-  <si>
-    <t>CUSTOMER_TYPE</t>
-  </si>
-  <si>
-    <t>DAILY_AMOUNT</t>
-  </si>
-  <si>
-    <t>DAILY_RESPONSE</t>
-  </si>
-  <si>
-    <t>DELIVERY_MODE</t>
-  </si>
-  <si>
-    <t>Branch [0]</t>
-  </si>
-  <si>
-    <t>DEVICE_CUSTOMER_TYPE</t>
-  </si>
-  <si>
-    <t>DEVICE_ID_GENERATION_TEMPLATE</t>
-  </si>
-  <si>
-    <t>AUTOMATION [PAN019]</t>
-  </si>
-  <si>
-    <t>DEVICE_PLAN_CODE</t>
-  </si>
-  <si>
-    <t>Corp Multicurrency travel card [CMTC01]</t>
-  </si>
-  <si>
-    <t>DEVICE_TYPE</t>
-  </si>
-  <si>
-    <t>DJMP_FEE_TYPE</t>
-  </si>
-  <si>
-    <t>Joining/Issuance Fee [I]</t>
-  </si>
-  <si>
-    <t>DJMP_POST_ISSUANCE_FEE_ON</t>
-  </si>
-  <si>
-    <t>Sale [S]</t>
-  </si>
-  <si>
-    <t>DR_STATUS</t>
-  </si>
-  <si>
-    <t>EMBOSSING_VENDOR</t>
-  </si>
-  <si>
-    <t>AUTOMATION PERS BUREAU [AUTOBU]</t>
-  </si>
-  <si>
-    <t>EMV_ABOVE_ATC_RANGE</t>
-  </si>
-  <si>
-    <t>EMV_BELOW_ATC_RANGE</t>
-  </si>
-  <si>
-    <t>EMV_PLAN_RESPONSE</t>
-  </si>
-  <si>
-    <t>END_POINT_MODE</t>
-  </si>
-  <si>
-    <t>Host [H]</t>
-  </si>
-  <si>
-    <t>EXPIRY_FLAG</t>
-  </si>
-  <si>
-    <t>Variable [V]</t>
-  </si>
-  <si>
-    <t>FEE_TYPE</t>
-  </si>
-  <si>
-    <t>Maintenance [A]</t>
-  </si>
-  <si>
-    <t>FIELD_NAME</t>
-  </si>
-  <si>
-    <t>Maiden Name [MAIDEN_NAME]</t>
-  </si>
-  <si>
-    <t>FILL_EMV_PLAN</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>FILL_RENEWAL_SECTION</t>
-  </si>
-  <si>
-    <t>FILL_REPLACEMENT_SECTION</t>
-  </si>
-  <si>
-    <t>FLOOR_AMOUNT</t>
-  </si>
-  <si>
-    <t>FLOOR_RESPONSE</t>
-  </si>
-  <si>
-    <t>GENDER</t>
-  </si>
-  <si>
-    <t>Male [M]</t>
-  </si>
-  <si>
-    <t>INTERCHANGE</t>
-  </si>
-  <si>
-    <t>INTERFACE_NAME</t>
-  </si>
-  <si>
-    <t>CBS1 [CBS1]</t>
-  </si>
-  <si>
-    <t>ISSUER_BIN</t>
-  </si>
-  <si>
-    <t>automation prepaid card [588765]</t>
-  </si>
-  <si>
-    <t>LANGUAGE_PREFERENCE</t>
-  </si>
-  <si>
-    <t>LEGAL_ID</t>
-  </si>
-  <si>
-    <t>MARITAL_STATUS</t>
-  </si>
-  <si>
-    <t>MEMBERSHIP_FEE_POSTING</t>
-  </si>
-  <si>
-    <t>Monthly [M]</t>
-  </si>
-  <si>
-    <t>MOBILE_NUMBER</t>
-  </si>
-  <si>
-    <t>PAYMENT_DATE</t>
-  </si>
-  <si>
-    <t>Next Month [8]</t>
-  </si>
-  <si>
-    <t>PICTURE_CODE</t>
-  </si>
-  <si>
-    <t>AUTOMATION PICTURE CODE [AUT]</t>
-  </si>
-  <si>
-    <t>PIN_DATA_TRANSMISSION</t>
-  </si>
-  <si>
-    <t>File [F]</t>
-  </si>
-  <si>
-    <t>PIN_GENERATION_OPTION</t>
-  </si>
-  <si>
-    <t>Random PIN [1]</t>
-  </si>
-  <si>
-    <t>PIN_LENGTH</t>
-  </si>
-  <si>
-    <t>PIN_RETRY_LIMIT</t>
-  </si>
-  <si>
-    <t>PLAN_TYPE</t>
-  </si>
-  <si>
-    <t>PLASTIC_ID</t>
-  </si>
-  <si>
-    <t>AUTOMATION PLASTIC CODE [AUT]</t>
-  </si>
-  <si>
-    <t>PREFERRED_MAILING_ADDRESS</t>
-  </si>
-  <si>
-    <t>Current [C]</t>
-  </si>
-  <si>
-    <t>PRODUCT_TYPE</t>
-  </si>
-  <si>
-    <t>PROGRAM</t>
-  </si>
-  <si>
-    <t>Multi currency Mastercard [CMCM01]</t>
-  </si>
-  <si>
-    <t>PROGRAM_TYPE</t>
-  </si>
-  <si>
-    <t>Retail Travel Card - Multi Currency [2]</t>
-  </si>
-  <si>
-    <t>PSP_PERIOD</t>
-  </si>
-  <si>
-    <t>PSP_SUPPRESS_IF_NO_ACTIVITY</t>
-  </si>
-  <si>
-    <t>PSPD_BILLING_DAY</t>
-  </si>
-  <si>
-    <t>PSPD_GENERATION_STATUS</t>
-  </si>
-  <si>
-    <t>Active [0]</t>
-  </si>
-  <si>
-    <t>PSPD_PRINT_DAY</t>
-  </si>
-  <si>
-    <t>PSPD_TO_LOT</t>
-  </si>
-  <si>
-    <t>QUANTITY_ORDERED</t>
-  </si>
-  <si>
-    <t>QUANTITY_TO_DISPATCH</t>
-  </si>
-  <si>
-    <t>REFUND_IN_CURRENCY</t>
-  </si>
-  <si>
-    <t>Program [P]</t>
-  </si>
-  <si>
-    <t>RENEWAL_ACTIVATION_MODE</t>
-  </si>
-  <si>
-    <t>REPLACEMENT_DEVICE_TECHNOLOGY</t>
-  </si>
-  <si>
-    <t>REPLACEMENT_NO_OF_DAYS</t>
-  </si>
-  <si>
-    <t>ROUTING_TYPE</t>
-  </si>
-  <si>
-    <t>Device Range Based [D]</t>
-  </si>
-  <si>
-    <t>SELECT_ALL_CAVV</t>
-  </si>
-  <si>
-    <t>SELECT_ALL_CVCCVV</t>
-  </si>
-  <si>
-    <t>SELECT_ALL_PIN_VALIDATION</t>
-  </si>
-  <si>
-    <t>SEQUENTIAL_INDICATOR</t>
-  </si>
-  <si>
-    <t>Sequential</t>
-  </si>
-  <si>
-    <t>SERVICE_CODE</t>
-  </si>
-  <si>
-    <t>STAND_IN_AMOUNT</t>
-  </si>
-  <si>
-    <t>STAND_IN_RESPONSE</t>
-  </si>
-  <si>
-    <t>START_MONTH_FOR_YEARLY_LIMITS</t>
-  </si>
-  <si>
-    <t>SUB_APPLICATION_TYPE</t>
-  </si>
-  <si>
-    <t>TABLE_FIRST_RECORD_FIELD</t>
-  </si>
-  <si>
-    <t>BIN [1]</t>
-  </si>
-  <si>
-    <t>TABLE_FIRST_RECORD_FIELD_CARDPACKID_TEMPLATE</t>
-  </si>
-  <si>
-    <t>Program Code [8]</t>
-  </si>
-  <si>
-    <t>TABLE_FIRST_RECORD_LENGTH</t>
-  </si>
-  <si>
-    <t>TABLE_LAST_RECORD_CUSTOM_FIELD_VALUE_1</t>
-  </si>
-  <si>
-    <t>0000000000</t>
-  </si>
-  <si>
-    <t>TABLE_LAST_RECORD_CUSTOM_FIELD_VALUE_2</t>
-  </si>
-  <si>
-    <t>TABLE_LAST_RECORD_LENGTH</t>
-  </si>
-  <si>
-    <t>TABLE_SECOND_RECORD_FIELD</t>
-  </si>
-  <si>
-    <t>Sequence number [4]</t>
-  </si>
-  <si>
-    <t>TABLE_SECOND_RECORD_LENGTH</t>
-  </si>
-  <si>
-    <t>TEMPLATE_LENGTH</t>
-  </si>
-  <si>
-    <t>TEMPLATE_TYPE_CARDPACKID</t>
-  </si>
-  <si>
-    <t>Card Pack ID Template [C]</t>
-  </si>
-  <si>
-    <t>TEMPLATE_TYPE_DEVICE</t>
-  </si>
-  <si>
-    <t>Device Template [D]</t>
-  </si>
-  <si>
-    <t>TEMPLATE_TYPE_PRIORITY_PASSID</t>
-  </si>
-  <si>
-    <t>Priority Pass ID [P]</t>
-  </si>
-  <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>Mr. [1]</t>
-  </si>
-  <si>
-    <t>TP_ASSIGNED_TRANSACTIONS</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>TRANSACTION_AMOUNT</t>
-  </si>
-  <si>
-    <t>TRANSACTION_CHANNEL</t>
-  </si>
-  <si>
-    <t>All [~]</t>
-  </si>
-  <si>
-    <t>TRANSACTION_LIMIT_PLAN</t>
-  </si>
-  <si>
-    <t>test field [TESTF]</t>
-  </si>
-  <si>
-    <t>TRANSACTION_ORIGIN</t>
-  </si>
-  <si>
-    <t>Both [~]</t>
-  </si>
-  <si>
-    <t>TRANSACTION_SOURCE</t>
-  </si>
-  <si>
-    <t>TRANSACTION_TYPE</t>
-  </si>
-  <si>
-    <t>Account Funding [AF]</t>
-  </si>
-  <si>
-    <t>UNPAID_DATE</t>
-  </si>
-  <si>
-    <t>USAGE</t>
-  </si>
-  <si>
-    <t>USER_INSTITUTION_DEFAULT</t>
-  </si>
-  <si>
-    <t>AUTO [121212]</t>
-  </si>
-  <si>
-    <t>VALIDITY_ON_INITIAL_MONTHS</t>
-  </si>
-  <si>
-    <t>VALIDITY_ON_RENEWAL_MONTHS</t>
-  </si>
-  <si>
-    <t>VALIDITY_ON_REPLACEMENT_MONTHS</t>
-  </si>
-  <si>
-    <t>POSTAL_CODE</t>
-  </si>
-  <si>
-    <t>DOCUMENT_1_TYPE</t>
-  </si>
-  <si>
-    <t>CS_SERVICE_CODE</t>
-  </si>
-  <si>
-    <t>Activate Device [108]</t>
-  </si>
-  <si>
-    <t>APPLICANT_PROFESSION</t>
-  </si>
-  <si>
-    <t>Architect [0]</t>
-  </si>
-  <si>
-    <t>MANDATORY_FIELDS</t>
-  </si>
-  <si>
-    <t>APPLICANT_PROF</t>
-  </si>
-  <si>
-    <t>CBS_CLIENT_ID</t>
-  </si>
-  <si>
-    <t>NO_OF_CURRENCY_ALLOWED</t>
-  </si>
-  <si>
-    <t>WALLET_TO_WALLET_TRANSFER_TYPE</t>
-  </si>
-  <si>
-    <t>Direct [D]</t>
-  </si>
-  <si>
-    <t>Reference Currency [R]</t>
-  </si>
-  <si>
-    <t>REFERENCE_CURRENCY</t>
-  </si>
-  <si>
-    <t>CURRENCY_WITH_PRIORITY</t>
-  </si>
-  <si>
-    <t>USD:02,EUR:03</t>
-  </si>
-  <si>
-    <t>Currency:Priority - To send muliple values use comma to separate data - example - USD:02,EUR:03</t>
-  </si>
-  <si>
-    <t>BDR_CORPORATE_CLIENT_CODE</t>
-  </si>
-  <si>
-    <t>Test Auto [12121217222000001]</t>
-  </si>
-  <si>
-    <t>BDR_DEVICE_PROMOTION_PLAN</t>
-  </si>
-  <si>
-    <t>BDR_DUMMY_ACCOUNT_NUMBER</t>
-  </si>
-  <si>
-    <t>BDR_EMBOSSING_LINE_4</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>BDR_EMBOSSING_NAME</t>
-  </si>
-  <si>
-    <t>BDR_QUANTITY_REQUESTED</t>
-  </si>
-  <si>
-    <t>BDR_WALLET_PROMOTION_PLAN1</t>
-  </si>
-  <si>
-    <t>CURRENCY_SETUP_SERVICE_CODE</t>
-  </si>
-  <si>
-    <t>Currency Setup [312]</t>
-  </si>
-  <si>
-    <t>HD_CURRENCY_WITH_PRIORITY</t>
-  </si>
-  <si>
-    <t>USD [840]:2 [2],EUR [978]:3 [3]</t>
-  </si>
-  <si>
-    <t>PGM_CALENDER_START_MONTH</t>
-  </si>
-  <si>
-    <t>PGM_KYC_LIMITS_MAX_BAL_WO_KYC</t>
-  </si>
-  <si>
-    <t>PGM_KYC_LIMITS_NO_OF_LOADS_ALLOWED_WO_KYC</t>
-  </si>
-  <si>
-    <t>ND_OTHERINFO_FAX_NO</t>
-  </si>
-  <si>
-    <t>ND_OTHERINFO_STATEMENT_PREFERENCE</t>
-  </si>
-  <si>
-    <t>Email [E]</t>
-  </si>
-  <si>
-    <t>ND_VIP</t>
-  </si>
-  <si>
-    <t>Normal [0]</t>
-  </si>
-  <si>
-    <t>ND_MIDDLE_NAME_2</t>
-  </si>
-  <si>
-    <t>ND_ENCODED_NAME</t>
-  </si>
-  <si>
-    <t>FINSIM_CARD_LENGTH</t>
-  </si>
-  <si>
-    <t>FINSIM_PAD</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>FINSIM_PIN_LENGHT</t>
-  </si>
-  <si>
-    <t>FINSIM_VALIDATION_DATA_START</t>
-  </si>
-  <si>
-    <t>ADJUSTMENT_TYPE</t>
-  </si>
-  <si>
-    <t>Miscellaneous Credit [71]</t>
-  </si>
-  <si>
-    <t>MANDATORY_FIELDS_FIELD_NAME</t>
-  </si>
-  <si>
-    <t>DATE_TYPE</t>
-  </si>
-  <si>
-    <t>Transaction Date [T]</t>
-  </si>
-  <si>
-    <t>INITIAL_LOAD_TXN_DETAILS</t>
-  </si>
-  <si>
-    <t>INR [356]:10.00:INR [356]</t>
-  </si>
-  <si>
-    <t>PROGRAM_WISE_BALANCE_SUMMARY</t>
-  </si>
-  <si>
-    <t>Program Wise Balance Summary Report</t>
-  </si>
-  <si>
-    <t>BATCH_NAME</t>
-  </si>
-  <si>
-    <t>Transaction Upload [TRANSACTION_UPLOAD]</t>
-  </si>
-  <si>
-    <t>BATCH_TYPE</t>
-  </si>
-  <si>
-    <t>UPLOAD [U]</t>
-  </si>
-  <si>
-    <t>BATCH_NAME_PRE_CLEARING</t>
-  </si>
-  <si>
-    <t>Pre-clearing</t>
-  </si>
-  <si>
-    <t>BATCH_NAME_PREPAID_EOD</t>
-  </si>
-  <si>
-    <t>EOD-Prepaid</t>
-  </si>
-  <si>
-    <t>PREPAID_PRODUCT_TYPE</t>
-  </si>
-  <si>
-    <t>ALL_TRANSACTIONS_REPORT</t>
-  </si>
-  <si>
-    <t>All Transactions Report</t>
-  </si>
-  <si>
-    <t>FILE_TYPE_REPORT</t>
-  </si>
-  <si>
-    <t>Excel Format [xlsDump]</t>
-  </si>
-  <si>
-    <t>PROGRAM_TRANSACTION_SUMMARY</t>
-  </si>
-  <si>
-    <t>Authorization Report</t>
-  </si>
-  <si>
-    <t>AUTOAGNC002 [AGNC002]</t>
-  </si>
-  <si>
-    <t>AUTOAGNC002</t>
-  </si>
-  <si>
-    <t>AUTOAGNT008 [AGNT008]</t>
-  </si>
-  <si>
-    <t>AUTOBRNCH002 [BRNCH002]</t>
   </si>
 </sst>
 </file>
@@ -2171,7 +1407,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\-yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2195,20 +1431,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2221,38 +1445,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF66FFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2EFDA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -2336,64 +1530,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2462,38 +1604,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3379,438 +2489,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA2"/>
-  <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="28.5703125" customWidth="1"/>
-    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:53" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="2" spans="1:53" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>357</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>377</v>
-      </c>
-      <c r="D2" s="9">
-        <v>8520</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>378</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="U2" s="9">
-        <v>16</v>
-      </c>
-      <c r="V2" s="9">
-        <v>16</v>
-      </c>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="32" t="s">
-        <v>379</v>
-      </c>
-      <c r="Z2" s="33" t="s">
-        <v>232</v>
-      </c>
-      <c r="AA2" s="9">
-        <v>45665456</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD2" s="9">
-        <v>1113332</v>
-      </c>
-      <c r="AE2" s="9">
-        <v>23564589</v>
-      </c>
-      <c r="AF2" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="AG2" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="AH2" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="AI2" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="AJ2" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL2" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="AM2" s="9">
-        <v>411006</v>
-      </c>
-      <c r="AN2" s="9">
-        <v>124421</v>
-      </c>
-      <c r="AO2" s="9" t="s">
-        <v>389</v>
-      </c>
-      <c r="AP2" s="9" t="s">
-        <v>388</v>
-      </c>
-      <c r="AQ2" s="9" t="s">
-        <v>380</v>
-      </c>
-      <c r="AR2" s="9" t="s">
-        <v>381</v>
-      </c>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="9"/>
-      <c r="AU2" s="9" t="s">
-        <v>382</v>
-      </c>
-      <c r="AV2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AW2" s="32" t="s">
-        <v>383</v>
-      </c>
-      <c r="AX2" s="9" t="s">
-        <v>384</v>
-      </c>
-      <c r="AY2" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="AZ2" s="9" t="s">
-        <v>387</v>
-      </c>
-      <c r="BA2" s="9" t="s">
-        <v>386</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="Y2" r:id="rId1" display="auto@mail.com"/>
-    <hyperlink ref="S2" r:id="rId2" display="auto12@mail.com"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4146,7 +2824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -4330,7 +3008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q13"/>
   <sheetViews>
@@ -4468,7 +3146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
@@ -4627,7 +3305,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -7646,2971 +6324,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C166"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
-        <v>457</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>459</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>460</v>
-      </c>
-      <c r="C2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>462</v>
-      </c>
-      <c r="B3" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>464</v>
-      </c>
-      <c r="B4" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="B6" s="2">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>470</v>
-      </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="B12" s="2">
-        <v>20</v>
-      </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="B18" s="2">
-        <v>100000</v>
-      </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="B29" s="2">
-        <v>500000</v>
-      </c>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>506</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="B40" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C40" s="2"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="B41" s="2">
-        <v>100</v>
-      </c>
-      <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="C42" s="2"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="C43" s="2"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="C44" s="2"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="C45" s="2"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="B50" s="2">
-        <v>100</v>
-      </c>
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="C54" s="2"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="C55" s="2"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="B57" s="2">
-        <v>1234</v>
-      </c>
-      <c r="C57" s="2"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C58" s="2"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="C59" s="2"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="B60" s="2">
-        <v>9999999999</v>
-      </c>
-      <c r="C60" s="2"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="C61" s="2"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="C62" s="2"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="C63" s="2"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="C64" s="2"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="B65" s="2">
-        <v>4</v>
-      </c>
-      <c r="C65" s="2"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="B66" s="2">
-        <v>3</v>
-      </c>
-      <c r="C66" s="2"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C67" s="2"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="C68" s="2"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="C69" s="2"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C70" s="2"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="C71" s="2"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="C72" s="2"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="C73" s="2"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="B74" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C74" s="2"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="B75" s="2">
-        <v>1</v>
-      </c>
-      <c r="C75" s="2"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>576</v>
-      </c>
-      <c r="C76" s="2"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="B77" s="2">
-        <v>5</v>
-      </c>
-      <c r="C77" s="2"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="B78" s="2">
-        <v>5</v>
-      </c>
-      <c r="C78" s="2"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="B79" s="2">
-        <v>1</v>
-      </c>
-      <c r="C79" s="2"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="B80" s="2">
-        <v>1</v>
-      </c>
-      <c r="C80" s="2"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="C81" s="2"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="B82" s="2">
-        <v>110</v>
-      </c>
-      <c r="C82" s="2"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="B84" s="2">
-        <v>25</v>
-      </c>
-      <c r="C84" s="2"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="C85" s="2"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C86" s="2"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>589</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C87" s="2"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>590</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C88" s="2"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="C89" s="2"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>593</v>
-      </c>
-      <c r="B90" s="2">
-        <v>201</v>
-      </c>
-      <c r="C90" s="2"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>594</v>
-      </c>
-      <c r="B91" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C91" s="2"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="C92" s="2"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C93" s="2"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C94" s="2"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>598</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>599</v>
-      </c>
-      <c r="C95" s="2"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="C96" s="2"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="B97" s="2">
-        <v>6</v>
-      </c>
-      <c r="C97" s="2"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="C98" s="2"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="B99" s="2">
-        <v>9999999999</v>
-      </c>
-      <c r="C99" s="2"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="B100" s="2">
-        <v>10</v>
-      </c>
-      <c r="C100" s="2"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="C101" s="2"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>609</v>
-      </c>
-      <c r="B102" s="2">
-        <v>9</v>
-      </c>
-      <c r="C102" s="2"/>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="B103" s="2">
-        <v>16</v>
-      </c>
-      <c r="C103" s="2"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="C104" s="2"/>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="C105" s="2"/>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="C106" s="2"/>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="C107" s="2"/>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>619</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>620</v>
-      </c>
-      <c r="C108" s="2"/>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="B109" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C109" s="2"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="C110" s="2"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>624</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>625</v>
-      </c>
-      <c r="C111" s="2"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>627</v>
-      </c>
-      <c r="C112" s="2"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="C113" s="2"/>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>629</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>630</v>
-      </c>
-      <c r="C114" s="2"/>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>631</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="C115" s="2"/>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C116" s="2"/>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="C117" s="2"/>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="B118" s="2">
-        <v>5</v>
-      </c>
-      <c r="C118" s="2"/>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>636</v>
-      </c>
-      <c r="B119" s="2">
-        <v>5</v>
-      </c>
-      <c r="C119" s="2"/>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>637</v>
-      </c>
-      <c r="B120" s="2">
-        <v>5</v>
-      </c>
-      <c r="C120" s="2"/>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
-        <v>638</v>
-      </c>
-      <c r="B121" s="2">
-        <v>411006</v>
-      </c>
-      <c r="C121" s="2"/>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
-        <v>639</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C122" s="2"/>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
-        <v>640</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>641</v>
-      </c>
-      <c r="C123" s="2"/>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>642</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="C124" s="2"/>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
-        <v>644</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="B126" s="2">
-        <v>5</v>
-      </c>
-      <c r="C126" s="2"/>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="C127" s="2"/>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="s">
-        <v>648</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C129" s="2"/>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>652</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>653</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>656</v>
-      </c>
-      <c r="C131" s="2"/>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>657</v>
-      </c>
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="B133" s="2">
-        <v>12345678</v>
-      </c>
-      <c r="C133" s="2"/>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>660</v>
-      </c>
-      <c r="C134" s="2"/>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
-        <v>661</v>
-      </c>
-      <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="B136" s="2">
-        <v>3</v>
-      </c>
-      <c r="C136" s="2"/>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>663</v>
-      </c>
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>664</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>666</v>
-      </c>
-      <c r="B139" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>668</v>
-      </c>
-      <c r="B140" s="40" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>669</v>
-      </c>
-      <c r="B141">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>670</v>
-      </c>
-      <c r="B142">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="41" t="s">
-        <v>671</v>
-      </c>
-      <c r="B143" s="42">
-        <v>11111111111</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="41" t="s">
-        <v>672</v>
-      </c>
-      <c r="B144" s="43" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>674</v>
-      </c>
-      <c r="B145" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="44" t="s">
-        <v>676</v>
-      </c>
-      <c r="B146" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="44" t="s">
-        <v>677</v>
-      </c>
-      <c r="B147" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="45" t="s">
-        <v>678</v>
-      </c>
-      <c r="B148" s="45">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="45" t="s">
-        <v>679</v>
-      </c>
-      <c r="B149" s="45" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="45" t="s">
-        <v>681</v>
-      </c>
-      <c r="B150" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="45" t="s">
-        <v>682</v>
-      </c>
-      <c r="B151" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="46" t="s">
-        <v>683</v>
-      </c>
-      <c r="B152" s="47" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="48" t="s">
-        <v>640</v>
-      </c>
-      <c r="B153" s="49" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="2" t="s">
-        <v>685</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>686</v>
-      </c>
-      <c r="B155" s="50" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>688</v>
-      </c>
-      <c r="B156" s="39" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>690</v>
-      </c>
-      <c r="B157" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="51" t="s">
-        <v>692</v>
-      </c>
-      <c r="B158" s="52" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="51" t="s">
-        <v>694</v>
-      </c>
-      <c r="B159" s="52" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="2" t="s">
-        <v>696</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>698</v>
-      </c>
-      <c r="B161" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>700</v>
-      </c>
-      <c r="B162" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>701</v>
-      </c>
-      <c r="B163" s="53" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>703</v>
-      </c>
-      <c r="B164" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>705</v>
-      </c>
-      <c r="B165" s="53" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>686</v>
-      </c>
-      <c r="B166" s="50" t="s">
-        <v>687</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C166"/>
-  <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection sqref="A1:C166"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
-        <v>457</v>
-      </c>
-      <c r="B1" s="38" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>459</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>689</v>
-      </c>
-      <c r="C2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>462</v>
-      </c>
-      <c r="B3" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>464</v>
-      </c>
-      <c r="B4" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="B6" s="2">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>707</v>
-      </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>708</v>
-      </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>709</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="B12" s="2">
-        <v>20</v>
-      </c>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>710</v>
-      </c>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>483</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>484</v>
-      </c>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>486</v>
-      </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="B18" s="2">
-        <v>100000</v>
-      </c>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>493</v>
-      </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>495</v>
-      </c>
-      <c r="C21" s="2"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="C23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>500</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>501</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>502</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="B29" s="2">
-        <v>500000</v>
-      </c>
-      <c r="C29" s="2"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>506</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="C31" s="2"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>510</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="C33" s="2"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="C34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C35" s="2"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>516</v>
-      </c>
-      <c r="C36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>517</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="C37" s="2"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="2"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>520</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="C39" s="2"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="B40" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C40" s="2"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="B41" s="2">
-        <v>100</v>
-      </c>
-      <c r="C41" s="2"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="C42" s="2"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="C43" s="2"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>528</v>
-      </c>
-      <c r="C44" s="2"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="C45" s="2"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="C46" s="2"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>536</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="B50" s="2">
-        <v>100</v>
-      </c>
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>543</v>
-      </c>
-      <c r="C54" s="2"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="C55" s="2"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C56" s="2"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="B57" s="2">
-        <v>1234</v>
-      </c>
-      <c r="C57" s="2"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C58" s="2"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="C59" s="2"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="B60" s="2">
-        <v>9999999999</v>
-      </c>
-      <c r="C60" s="2"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="C61" s="2"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="C62" s="2"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>556</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="C63" s="2"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="C64" s="2"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="B65" s="2">
-        <v>4</v>
-      </c>
-      <c r="C65" s="2"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>561</v>
-      </c>
-      <c r="B66" s="2">
-        <v>3</v>
-      </c>
-      <c r="C66" s="2"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C67" s="2"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="C68" s="2"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>566</v>
-      </c>
-      <c r="C69" s="2"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C70" s="2"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="C71" s="2"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="C72" s="2"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="C73" s="2"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="B74" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C74" s="2"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="B75" s="2">
-        <v>1</v>
-      </c>
-      <c r="C75" s="2"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>576</v>
-      </c>
-      <c r="C76" s="2"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="B77" s="2">
-        <v>5</v>
-      </c>
-      <c r="C77" s="2"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="B78" s="2">
-        <v>5</v>
-      </c>
-      <c r="C78" s="2"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="B79" s="2">
-        <v>1</v>
-      </c>
-      <c r="C79" s="2"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="B80" s="2">
-        <v>1</v>
-      </c>
-      <c r="C80" s="2"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="C81" s="2"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="B82" s="2">
-        <v>110</v>
-      </c>
-      <c r="C82" s="2"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="B84" s="2">
-        <v>25</v>
-      </c>
-      <c r="C84" s="2"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="C85" s="2"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C86" s="2"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>589</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C87" s="2"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>590</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="C88" s="2"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>592</v>
-      </c>
-      <c r="C89" s="2"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>593</v>
-      </c>
-      <c r="B90" s="2">
-        <v>201</v>
-      </c>
-      <c r="C90" s="2"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>594</v>
-      </c>
-      <c r="B91" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C91" s="2"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="C92" s="2"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>596</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C93" s="2"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C94" s="2"/>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>598</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>599</v>
-      </c>
-      <c r="C95" s="2"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>601</v>
-      </c>
-      <c r="C96" s="2"/>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="B97" s="2">
-        <v>6</v>
-      </c>
-      <c r="C97" s="2"/>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>603</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="C98" s="2"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="B99" s="2">
-        <v>9999999999</v>
-      </c>
-      <c r="C99" s="2"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="B100" s="2">
-        <v>10</v>
-      </c>
-      <c r="C100" s="2"/>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="C101" s="2"/>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>609</v>
-      </c>
-      <c r="B102" s="2">
-        <v>9</v>
-      </c>
-      <c r="C102" s="2"/>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="B103" s="2">
-        <v>16</v>
-      </c>
-      <c r="C103" s="2"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="C104" s="2"/>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="C105" s="2"/>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="C106" s="2"/>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="C107" s="2"/>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>619</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>620</v>
-      </c>
-      <c r="C108" s="2"/>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="B109" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C109" s="2"/>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="C110" s="2"/>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>624</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>625</v>
-      </c>
-      <c r="C111" s="2"/>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>627</v>
-      </c>
-      <c r="C112" s="2"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="C113" s="2"/>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>629</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>630</v>
-      </c>
-      <c r="C114" s="2"/>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>631</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="C115" s="2"/>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>632</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C116" s="2"/>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>633</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="C117" s="2"/>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>635</v>
-      </c>
-      <c r="B118" s="2">
-        <v>5</v>
-      </c>
-      <c r="C118" s="2"/>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>636</v>
-      </c>
-      <c r="B119" s="2">
-        <v>5</v>
-      </c>
-      <c r="C119" s="2"/>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>637</v>
-      </c>
-      <c r="B120" s="2">
-        <v>5</v>
-      </c>
-      <c r="C120" s="2"/>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
-        <v>638</v>
-      </c>
-      <c r="B121" s="2">
-        <v>411006</v>
-      </c>
-      <c r="C121" s="2"/>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
-        <v>639</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C122" s="2"/>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
-        <v>640</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>641</v>
-      </c>
-      <c r="C123" s="2"/>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>642</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>643</v>
-      </c>
-      <c r="C124" s="2"/>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
-        <v>644</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="B126" s="2">
-        <v>5</v>
-      </c>
-      <c r="C126" s="2"/>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="C127" s="2"/>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="s">
-        <v>648</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>649</v>
-      </c>
-      <c r="C128" s="2" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C129" s="2"/>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>652</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>653</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>656</v>
-      </c>
-      <c r="C131" s="2"/>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>657</v>
-      </c>
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="B133" s="2">
-        <v>12345678</v>
-      </c>
-      <c r="C133" s="2"/>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>660</v>
-      </c>
-      <c r="C134" s="2"/>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
-        <v>661</v>
-      </c>
-      <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="B136" s="2">
-        <v>3</v>
-      </c>
-      <c r="C136" s="2"/>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>663</v>
-      </c>
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>664</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>666</v>
-      </c>
-      <c r="B139" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>668</v>
-      </c>
-      <c r="B140" s="40" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>669</v>
-      </c>
-      <c r="B141">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>670</v>
-      </c>
-      <c r="B142">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" s="41" t="s">
-        <v>671</v>
-      </c>
-      <c r="B143" s="42">
-        <v>11111111111</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" s="41" t="s">
-        <v>672</v>
-      </c>
-      <c r="B144" s="43" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>674</v>
-      </c>
-      <c r="B145" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="44" t="s">
-        <v>676</v>
-      </c>
-      <c r="B146" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="44" t="s">
-        <v>677</v>
-      </c>
-      <c r="B147" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="45" t="s">
-        <v>678</v>
-      </c>
-      <c r="B148" s="45">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="45" t="s">
-        <v>679</v>
-      </c>
-      <c r="B149" s="45" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="45" t="s">
-        <v>681</v>
-      </c>
-      <c r="B150" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="45" t="s">
-        <v>682</v>
-      </c>
-      <c r="B151" s="45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="46" t="s">
-        <v>683</v>
-      </c>
-      <c r="B152" s="47" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="48" t="s">
-        <v>640</v>
-      </c>
-      <c r="B153" s="49" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="2" t="s">
-        <v>685</v>
-      </c>
-      <c r="B154" s="2" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>686</v>
-      </c>
-      <c r="B155" s="50" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>688</v>
-      </c>
-      <c r="B156" s="39" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>690</v>
-      </c>
-      <c r="B157" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="51" t="s">
-        <v>692</v>
-      </c>
-      <c r="B158" s="52" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="51" t="s">
-        <v>694</v>
-      </c>
-      <c r="B159" s="52" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="2" t="s">
-        <v>696</v>
-      </c>
-      <c r="B160" s="2" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>698</v>
-      </c>
-      <c r="B161" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>700</v>
-      </c>
-      <c r="B162" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>701</v>
-      </c>
-      <c r="B163" s="53" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>703</v>
-      </c>
-      <c r="B164" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>705</v>
-      </c>
-      <c r="B165" s="53" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>686</v>
-      </c>
-      <c r="B166" s="50" t="s">
-        <v>687</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -10766,7 +6482,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:R6"/>
   <sheetViews>
@@ -11097,7 +6813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -11174,7 +6890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -11248,7 +6964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -11350,4 +7066,436 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BA2"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="28.5703125" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:53" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:53" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="D2" s="9">
+        <v>8520</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="L2" s="9"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="U2" s="9">
+        <v>16</v>
+      </c>
+      <c r="V2" s="9">
+        <v>16</v>
+      </c>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="32" t="s">
+        <v>379</v>
+      </c>
+      <c r="Z2" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="AA2" s="9">
+        <v>45665456</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD2" s="9">
+        <v>1113332</v>
+      </c>
+      <c r="AE2" s="9">
+        <v>23564589</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG2" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL2" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM2" s="9">
+        <v>411006</v>
+      </c>
+      <c r="AN2" s="9">
+        <v>124421</v>
+      </c>
+      <c r="AO2" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="AP2" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="AQ2" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="AR2" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="AS2" s="9"/>
+      <c r="AT2" s="9"/>
+      <c r="AU2" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="AV2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AW2" s="32" t="s">
+        <v>383</v>
+      </c>
+      <c r="AX2" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="AY2" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="AZ2" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="BA2" s="9" t="s">
+        <v>386</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Y2" r:id="rId1" display="auto@mail.com"/>
+    <hyperlink ref="S2" r:id="rId2" display="auto12@mail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Data changes for institution creation
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12672" windowHeight="6756" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12948" windowHeight="6756" firstSheet="7" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1509" uniqueCount="469">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -933,9 +933,6 @@
     <t>Collect Portal Support</t>
   </si>
   <si>
-    <t>TC1InstituteCreation</t>
-  </si>
-  <si>
     <t>TC264384_Privilege validation for RuPay Settlement Bin Configurations</t>
   </si>
   <si>
@@ -1164,12 +1161,6 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>FEMA</t>
-  </si>
-  <si>
-    <t>1100440052</t>
-  </si>
-  <si>
     <t>English [EN]</t>
   </si>
   <si>
@@ -1179,9 +1170,6 @@
     <t>testuser124421@gmail.com</t>
   </si>
   <si>
-    <t>5431267812</t>
-  </si>
-  <si>
     <t>July/2/2018</t>
   </si>
   <si>
@@ -1191,9 +1179,6 @@
     <t>Record Added Successfully.</t>
   </si>
   <si>
-    <t>999</t>
-  </si>
-  <si>
     <t>Batch [ROLE000052]</t>
   </si>
   <si>
@@ -1432,6 +1417,24 @@
   </si>
   <si>
     <t>Collector [COL]</t>
+  </si>
+  <si>
+    <t>TCInstituteCreationPR</t>
+  </si>
+  <si>
+    <t>ISSUING</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>SDN Verification [SDN001]</t>
+  </si>
+  <si>
+    <t>TCInstituteCreationDC</t>
+  </si>
+  <si>
+    <t>TCInstituteCreationDCPR</t>
   </si>
 </sst>
 </file>
@@ -1575,7 +1578,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1638,7 +1641,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
@@ -2538,212 +2540,212 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:61" s="38" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:61" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>307</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="D1" s="37" t="s">
+        <v>452</v>
+      </c>
+      <c r="E1" s="37" t="s">
         <v>308</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="F1" s="37" t="s">
+        <v>453</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>357</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>454</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>455</v>
+      </c>
+      <c r="L1" s="37" t="s">
+        <v>295</v>
+      </c>
+      <c r="M1" s="37" t="s">
+        <v>296</v>
+      </c>
+      <c r="N1" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="O1" s="37" t="s">
+        <v>456</v>
+      </c>
+      <c r="P1" s="37" t="s">
         <v>457</v>
       </c>
-      <c r="E1" s="38" t="s">
-        <v>309</v>
-      </c>
-      <c r="F1" s="38" t="s">
+      <c r="Q1" s="37" t="s">
         <v>458</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="R1" s="37" t="s">
+        <v>298</v>
+      </c>
+      <c r="S1" s="37" t="s">
         <v>358</v>
       </c>
-      <c r="H1" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="38" t="s">
-        <v>459</v>
-      </c>
-      <c r="J1" s="38" t="s">
-        <v>238</v>
-      </c>
-      <c r="K1" s="38" t="s">
-        <v>460</v>
-      </c>
-      <c r="L1" s="38" t="s">
-        <v>295</v>
-      </c>
-      <c r="M1" s="38" t="s">
-        <v>296</v>
-      </c>
-      <c r="N1" s="38" t="s">
-        <v>297</v>
-      </c>
-      <c r="O1" s="38" t="s">
-        <v>461</v>
-      </c>
-      <c r="P1" s="38" t="s">
-        <v>462</v>
-      </c>
-      <c r="Q1" s="38" t="s">
-        <v>463</v>
-      </c>
-      <c r="R1" s="38" t="s">
-        <v>298</v>
-      </c>
-      <c r="S1" s="38" t="s">
+      <c r="T1" s="37" t="s">
+        <v>299</v>
+      </c>
+      <c r="U1" s="37" t="s">
+        <v>300</v>
+      </c>
+      <c r="V1" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="W1" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="X1" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y1" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="Z1" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="AA1" s="37" t="s">
         <v>359</v>
       </c>
-      <c r="T1" s="38" t="s">
-        <v>299</v>
-      </c>
-      <c r="U1" s="38" t="s">
-        <v>300</v>
-      </c>
-      <c r="V1" s="38" t="s">
-        <v>209</v>
-      </c>
-      <c r="W1" s="38" t="s">
-        <v>210</v>
-      </c>
-      <c r="X1" s="38" t="s">
-        <v>211</v>
-      </c>
-      <c r="Y1" s="38" t="s">
-        <v>212</v>
-      </c>
-      <c r="Z1" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="AA1" s="38" t="s">
+      <c r="AB1" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="AC1" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD1" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="AE1" s="37" t="s">
+        <v>359</v>
+      </c>
+      <c r="AF1" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="AG1" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH1" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="AI1" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="AJ1" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="AK1" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="AL1" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="AM1" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="AN1" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="AO1" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="AP1" s="37" t="s">
+        <v>227</v>
+      </c>
+      <c r="AQ1" s="37" t="s">
         <v>360</v>
       </c>
-      <c r="AB1" s="38" t="s">
-        <v>214</v>
-      </c>
-      <c r="AC1" s="38" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD1" s="38" t="s">
-        <v>216</v>
-      </c>
-      <c r="AE1" s="38" t="s">
-        <v>360</v>
-      </c>
-      <c r="AF1" s="38" t="s">
-        <v>217</v>
-      </c>
-      <c r="AG1" s="38" t="s">
-        <v>218</v>
-      </c>
-      <c r="AH1" s="38" t="s">
-        <v>219</v>
-      </c>
-      <c r="AI1" s="38" t="s">
-        <v>220</v>
-      </c>
-      <c r="AJ1" s="38" t="s">
-        <v>221</v>
-      </c>
-      <c r="AK1" s="38" t="s">
-        <v>222</v>
-      </c>
-      <c r="AL1" s="38" t="s">
-        <v>223</v>
-      </c>
-      <c r="AM1" s="38" t="s">
-        <v>224</v>
-      </c>
-      <c r="AN1" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="AO1" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="AP1" s="38" t="s">
-        <v>227</v>
-      </c>
-      <c r="AQ1" s="38" t="s">
+      <c r="AR1" s="37" t="s">
         <v>361</v>
       </c>
-      <c r="AR1" s="38" t="s">
+      <c r="AS1" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="AT1" s="37" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU1" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="AV1" s="37" t="s">
         <v>362</v>
       </c>
-      <c r="AS1" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="AT1" s="38" t="s">
-        <v>228</v>
-      </c>
-      <c r="AU1" s="38" t="s">
-        <v>229</v>
-      </c>
-      <c r="AV1" s="38" t="s">
+      <c r="AW1" s="37" t="s">
         <v>363</v>
       </c>
-      <c r="AW1" s="38" t="s">
+      <c r="AX1" s="37" t="s">
         <v>364</v>
       </c>
-      <c r="AX1" s="38" t="s">
+      <c r="AY1" s="37" t="s">
         <v>365</v>
       </c>
-      <c r="AY1" s="38" t="s">
+      <c r="AZ1" s="37" t="s">
         <v>366</v>
       </c>
-      <c r="AZ1" s="38" t="s">
+      <c r="BA1" s="37" t="s">
         <v>367</v>
       </c>
-      <c r="BA1" s="38" t="s">
+      <c r="BB1" s="37" t="s">
         <v>368</v>
       </c>
-      <c r="BB1" s="38" t="s">
+      <c r="BC1" s="37" t="s">
         <v>369</v>
       </c>
-      <c r="BC1" s="38" t="s">
+      <c r="BD1" s="37" t="s">
         <v>370</v>
       </c>
-      <c r="BD1" s="38" t="s">
+      <c r="BE1" s="37" t="s">
         <v>371</v>
       </c>
-      <c r="BE1" s="38" t="s">
+      <c r="BF1" s="37" t="s">
         <v>372</v>
       </c>
-      <c r="BF1" s="38" t="s">
+      <c r="BG1" s="37" t="s">
         <v>373</v>
       </c>
-      <c r="BG1" s="38" t="s">
+      <c r="BH1" s="37" t="s">
         <v>374</v>
       </c>
-      <c r="BH1" s="38" t="s">
+      <c r="BI1" s="37" t="s">
         <v>375</v>
-      </c>
-      <c r="BI1" s="38" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:61" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E2" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="F2" s="31" t="s">
         <v>321</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>322</v>
       </c>
       <c r="G2" s="31" t="s">
         <v>187</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="L2" s="31" t="s">
         <v>230</v>
@@ -2842,19 +2844,19 @@
         <v>124421</v>
       </c>
       <c r="AW2" s="31" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="AX2" s="31" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="AY2" s="31" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="AZ2" s="31" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="BC2" s="31" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="BD2" s="31" t="s">
         <v>34</v>
@@ -2863,16 +2865,16 @@
         <v>5431267812</v>
       </c>
       <c r="BF2" s="31" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="BG2" s="31" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="BH2" s="31">
         <v>999</v>
       </c>
       <c r="BI2" s="31" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -2950,7 +2952,7 @@
     </row>
     <row r="2" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>201</v>
@@ -3003,7 +3005,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>201</v>
@@ -3056,7 +3058,7 @@
     </row>
     <row r="4" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>201</v>
@@ -3109,7 +3111,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>201</v>
@@ -3162,7 +3164,7 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>201</v>
@@ -3229,9 +3231,9 @@
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="61.6640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="35" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="34" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="34" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="31" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.44140625" style="31" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="31"/>
@@ -3242,13 +3244,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>308</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>309</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -3259,142 +3261,142 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>357</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>399</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>321</v>
+        <v>356</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>320</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
+        <v>386</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>356</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="B3" s="31" t="s">
-        <v>357</v>
-      </c>
-      <c r="C3" s="34" t="s">
-        <v>399</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>321</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>396</v>
-      </c>
       <c r="F3" s="9" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>357</v>
-      </c>
-      <c r="C4" s="34" t="s">
-        <v>399</v>
-      </c>
-      <c r="D4" s="34" t="s">
-        <v>321</v>
+        <v>356</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>320</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
+        <v>387</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>395</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>392</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>400</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>399</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>321</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>401</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>399</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>321</v>
+        <v>396</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>320</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>397</v>
+      </c>
+      <c r="C7" s="33" t="s">
         <v>394</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>402</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>399</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>321</v>
+      <c r="D7" s="33" t="s">
+        <v>320</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>403</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>399</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>321</v>
+        <v>398</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>320</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -3435,43 +3437,43 @@
         <v>1</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>308</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>309</v>
       </c>
       <c r="E1" s="23" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="23" t="s">
+        <v>309</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>310</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>311</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>312</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>313</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>314</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>315</v>
       </c>
       <c r="L1" s="23" t="s">
         <v>75</v>
       </c>
       <c r="M1" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="N1" s="23" t="s">
         <v>316</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>317</v>
       </c>
       <c r="O1" s="24"/>
       <c r="P1" s="24"/>
@@ -3479,42 +3481,42 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C2" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="25" t="s">
         <v>324</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="J2" s="26" t="s">
         <v>326</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="K2" s="26" t="s">
         <v>327</v>
-      </c>
-      <c r="K2" s="26" t="s">
-        <v>328</v>
       </c>
       <c r="L2" s="25"/>
       <c r="M2" s="25"/>
       <c r="N2" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="O2" s="24"/>
       <c r="P2" s="24"/>
@@ -3570,84 +3572,84 @@
         <v>1</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>307</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>308</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>309</v>
       </c>
       <c r="D1" s="23" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="23" t="s">
+        <v>329</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>330</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" s="23" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>309</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="J1" s="23" t="s">
         <v>331</v>
       </c>
-      <c r="G1" s="23" t="s">
-        <v>312</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>310</v>
-      </c>
-      <c r="I1" s="23" t="s">
-        <v>311</v>
-      </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>332</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="L1" s="23" t="s">
         <v>333</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>334</v>
       </c>
       <c r="M1" s="23" t="s">
         <v>75</v>
       </c>
       <c r="N1" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="O1" s="23" t="s">
         <v>316</v>
-      </c>
-      <c r="O1" s="23" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>321</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>322</v>
       </c>
       <c r="E2" s="25">
         <v>123456</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>134</v>
       </c>
       <c r="I2" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="J2" s="26" t="s">
         <v>337</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="K2" s="26" t="s">
         <v>338</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="L2" s="26" t="s">
         <v>339</v>
-      </c>
-      <c r="L2" s="26" t="s">
-        <v>340</v>
       </c>
       <c r="M2" s="25"/>
       <c r="N2" s="25"/>
@@ -3655,40 +3657,40 @@
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B3" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="D3" s="25" t="s">
         <v>321</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>322</v>
       </c>
       <c r="E3" s="25">
         <v>123456</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H3" s="25" t="s">
         <v>134</v>
       </c>
       <c r="I3" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="J3" s="26" t="s">
         <v>337</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="K3" s="26" t="s">
         <v>338</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="L3" s="26" t="s">
         <v>339</v>
-      </c>
-      <c r="L3" s="26" t="s">
-        <v>340</v>
       </c>
       <c r="M3" s="25"/>
       <c r="N3" s="25"/>
@@ -3725,69 +3727,69 @@
         <v>1</v>
       </c>
       <c r="B1" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>307</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" s="23" t="s">
         <v>308</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>309</v>
       </c>
       <c r="E1" s="23" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="23" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H1" s="23" t="s">
         <v>75</v>
       </c>
       <c r="I1" s="23" t="s">
+        <v>342</v>
+      </c>
+      <c r="J1" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="27" t="s">
         <v>344</v>
-      </c>
-      <c r="K1" s="27" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
+        <v>345</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>318</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>321</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>346</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>319</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>320</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>321</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>322</v>
-      </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="H2" s="25" t="s">
         <v>347</v>
       </c>
-      <c r="G2" s="25" t="s">
-        <v>325</v>
-      </c>
-      <c r="H2" s="25" t="s">
+      <c r="I2" s="25" t="s">
         <v>348</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="J2" s="25" t="s">
         <v>349</v>
       </c>
-      <c r="J2" s="25" t="s">
-        <v>350</v>
-      </c>
       <c r="K2" s="25" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -3831,13 +3833,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>309</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -3876,10 +3878,10 @@
         <v>105</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>351</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>352</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>106</v>
@@ -4068,16 +4070,16 @@
         <v>50</v>
       </c>
       <c r="CC1" s="4" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="CD1" s="4" t="s">
         <v>76</v>
       </c>
       <c r="CE1" s="4" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="CF1" s="4" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="CG1" s="4" t="s">
         <v>94</v>
@@ -4125,58 +4127,58 @@
         <v>60</v>
       </c>
       <c r="CV1" s="4" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="CW1" s="4" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="CX1" s="4" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="CY1" s="4" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="CZ1" s="4" t="s">
         <v>193</v>
       </c>
       <c r="DA1" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="DB1" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="DC1" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="DD1" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="DE1" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="DF1" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="DB1" s="4" t="s">
+      <c r="DG1" s="4" t="s">
         <v>438</v>
       </c>
-      <c r="DC1" s="4" t="s">
+      <c r="DH1" s="4" t="s">
         <v>439</v>
       </c>
-      <c r="DD1" s="4" t="s">
+      <c r="DI1" s="4" t="s">
         <v>440</v>
       </c>
-      <c r="DE1" s="4" t="s">
+      <c r="DJ1" s="4" t="s">
         <v>441</v>
       </c>
-      <c r="DF1" s="4" t="s">
+      <c r="DK1" s="4" t="s">
         <v>442</v>
       </c>
-      <c r="DG1" s="4" t="s">
+      <c r="DL1" s="4" t="s">
         <v>443</v>
       </c>
-      <c r="DH1" s="4" t="s">
+      <c r="DM1" s="4" t="s">
         <v>444</v>
-      </c>
-      <c r="DI1" s="4" t="s">
-        <v>445</v>
-      </c>
-      <c r="DJ1" s="4" t="s">
-        <v>446</v>
-      </c>
-      <c r="DK1" s="4" t="s">
-        <v>447</v>
-      </c>
-      <c r="DL1" s="4" t="s">
-        <v>448</v>
-      </c>
-      <c r="DM1" s="4" t="s">
-        <v>449</v>
       </c>
       <c r="DN1" s="4"/>
     </row>
@@ -4185,19 +4187,19 @@
         <v>132</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="G2" s="28" t="s">
         <v>129</v>
@@ -4220,16 +4222,16 @@
       </c>
       <c r="N2" s="28"/>
       <c r="O2" s="28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P2" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Q2" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="R2" s="28" t="s">
         <v>354</v>
-      </c>
-      <c r="R2" s="28" t="s">
-        <v>355</v>
       </c>
       <c r="S2" s="29" t="s">
         <v>246</v>
@@ -4241,13 +4243,13 @@
         <v>36</v>
       </c>
       <c r="V2" s="28" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="W2" s="28" t="s">
         <v>122</v>
       </c>
       <c r="X2" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="Y2" s="28" t="s">
         <v>139</v>
@@ -4271,7 +4273,7 @@
         <v>36</v>
       </c>
       <c r="AF2" s="28" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="AG2" s="28" t="s">
         <v>9</v>
@@ -4280,7 +4282,7 @@
         <v>10</v>
       </c>
       <c r="AI2" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AJ2" s="28" t="s">
         <v>11</v>
@@ -4292,7 +4294,7 @@
         <v>56</v>
       </c>
       <c r="AM2" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AN2" s="28" t="s">
         <v>16</v>
@@ -4301,13 +4303,13 @@
         <v>129</v>
       </c>
       <c r="AP2" s="28" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="AQ2" s="28" t="s">
         <v>195</v>
       </c>
       <c r="AR2" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AS2" s="28" t="s">
         <v>147</v>
@@ -4335,19 +4337,19 @@
         <v>36</v>
       </c>
       <c r="BB2" s="28" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="BC2" s="28" t="s">
         <v>31</v>
       </c>
       <c r="BD2" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BE2" s="28" t="s">
         <v>34</v>
       </c>
       <c r="BF2" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BG2" s="28" t="s">
         <v>35</v>
@@ -4375,10 +4377,10 @@
         <v>71</v>
       </c>
       <c r="BP2" s="9" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="BQ2" s="28" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="BR2" s="28"/>
       <c r="BS2" s="9"/>
@@ -4394,7 +4396,7 @@
         <v>195</v>
       </c>
       <c r="BY2" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="BZ2" s="9" t="s">
         <v>48</v>
@@ -4406,7 +4408,7 @@
         <v>61</v>
       </c>
       <c r="CC2" s="9" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="CD2" s="9"/>
       <c r="CE2" s="9"/>
@@ -4415,16 +4417,16 @@
         <v>133</v>
       </c>
       <c r="CH2" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CI2" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="CJ2" s="28" t="s">
         <v>415</v>
       </c>
-      <c r="CJ2" s="28" t="s">
-        <v>420</v>
-      </c>
       <c r="CK2" s="28" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="CL2" s="28" t="s">
         <v>91</v>
@@ -4433,16 +4435,16 @@
         <v>138</v>
       </c>
       <c r="CN2" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CO2" s="9" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="CP2" s="9" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="CQ2" s="28" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="CR2" s="28" t="s">
         <v>200</v>
@@ -4450,14 +4452,14 @@
       <c r="CS2" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="CT2" s="36" t="s">
+      <c r="CT2" s="35" t="s">
         <v>53</v>
       </c>
       <c r="CU2" s="9">
         <v>100</v>
       </c>
-      <c r="CV2" s="37" t="s">
-        <v>450</v>
+      <c r="CV2" s="36" t="s">
+        <v>445</v>
       </c>
       <c r="CW2" s="9">
         <v>5</v>
@@ -4469,16 +4471,16 @@
         <v>71</v>
       </c>
       <c r="CZ2" s="9" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="DA2" s="9" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="DB2" s="9">
         <v>6</v>
       </c>
       <c r="DC2" s="9" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="DD2" s="9">
         <v>2</v>
@@ -4490,13 +4492,13 @@
         <v>1</v>
       </c>
       <c r="DG2" s="9" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="DH2" s="9">
         <v>3</v>
       </c>
       <c r="DI2" s="9" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="DJ2" s="9">
         <v>3</v>
@@ -4504,7 +4506,7 @@
       <c r="DK2" s="9"/>
       <c r="DL2" s="9"/>
       <c r="DM2" s="9" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
@@ -4512,19 +4514,19 @@
         <v>140</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="G3" s="28" t="s">
         <v>129</v>
@@ -4547,16 +4549,16 @@
       </c>
       <c r="N3" s="28"/>
       <c r="O3" s="28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P3" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Q3" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="R3" s="28" t="s">
         <v>354</v>
-      </c>
-      <c r="R3" s="28" t="s">
-        <v>355</v>
       </c>
       <c r="S3" s="29" t="s">
         <v>246</v>
@@ -4568,13 +4570,13 @@
         <v>36</v>
       </c>
       <c r="V3" s="28" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="W3" s="28" t="s">
         <v>122</v>
       </c>
       <c r="X3" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="Y3" s="28" t="s">
         <v>139</v>
@@ -4598,7 +4600,7 @@
         <v>36</v>
       </c>
       <c r="AF3" s="28" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="AG3" s="28" t="s">
         <v>9</v>
@@ -4607,7 +4609,7 @@
         <v>10</v>
       </c>
       <c r="AI3" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AJ3" s="28" t="s">
         <v>11</v>
@@ -4619,7 +4621,7 @@
         <v>56</v>
       </c>
       <c r="AM3" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AN3" s="28" t="s">
         <v>16</v>
@@ -4628,13 +4630,13 @@
         <v>129</v>
       </c>
       <c r="AP3" s="28" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="AQ3" s="28" t="s">
         <v>195</v>
       </c>
       <c r="AR3" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AS3" s="28" t="s">
         <v>148</v>
@@ -4662,19 +4664,19 @@
         <v>36</v>
       </c>
       <c r="BB3" s="28" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="BC3" s="28" t="s">
         <v>31</v>
       </c>
       <c r="BD3" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BE3" s="28" t="s">
         <v>34</v>
       </c>
       <c r="BF3" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BG3" s="28" t="s">
         <v>35</v>
@@ -4702,17 +4704,17 @@
         <v>71</v>
       </c>
       <c r="BP3" s="9" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="BQ3" s="28" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="BR3" s="28"/>
       <c r="BS3" s="9" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="BT3" s="9" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="BU3" s="9" t="s">
         <v>40</v>
@@ -4725,7 +4727,7 @@
         <v>195</v>
       </c>
       <c r="BY3" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="BZ3" s="9" t="s">
         <v>48</v>
@@ -4744,16 +4746,16 @@
         <v>133</v>
       </c>
       <c r="CH3" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CI3" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="CJ3" s="28" t="s">
         <v>415</v>
       </c>
-      <c r="CJ3" s="28" t="s">
-        <v>420</v>
-      </c>
       <c r="CK3" s="9" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="CL3" s="28" t="s">
         <v>91</v>
@@ -4762,16 +4764,16 @@
         <v>138</v>
       </c>
       <c r="CN3" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CO3" s="28" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="CP3" s="28" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="CQ3" s="28" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="CR3" s="29" t="s">
         <v>200</v>
@@ -4791,19 +4793,19 @@
         <v>150</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="G4" s="28" t="s">
         <v>129</v>
@@ -4826,16 +4828,16 @@
       </c>
       <c r="N4" s="28"/>
       <c r="O4" s="28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P4" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Q4" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="R4" s="28" t="s">
         <v>354</v>
-      </c>
-      <c r="R4" s="28" t="s">
-        <v>355</v>
       </c>
       <c r="S4" s="29" t="s">
         <v>246</v>
@@ -4847,13 +4849,13 @@
         <v>36</v>
       </c>
       <c r="V4" s="28" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="W4" s="28" t="s">
         <v>122</v>
       </c>
       <c r="X4" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="Y4" s="28" t="s">
         <v>139</v>
@@ -4877,7 +4879,7 @@
         <v>36</v>
       </c>
       <c r="AF4" s="28" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="AG4" s="28" t="s">
         <v>9</v>
@@ -4886,7 +4888,7 @@
         <v>10</v>
       </c>
       <c r="AI4" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AJ4" s="28" t="s">
         <v>11</v>
@@ -4898,7 +4900,7 @@
         <v>56</v>
       </c>
       <c r="AM4" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AN4" s="28" t="s">
         <v>16</v>
@@ -4907,13 +4909,13 @@
         <v>129</v>
       </c>
       <c r="AP4" s="28" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="AQ4" s="28" t="s">
         <v>195</v>
       </c>
       <c r="AR4" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AS4" s="28" t="s">
         <v>152</v>
@@ -4941,19 +4943,19 @@
         <v>36</v>
       </c>
       <c r="BB4" s="28" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="BC4" s="28" t="s">
         <v>31</v>
       </c>
       <c r="BD4" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BE4" s="28" t="s">
         <v>34</v>
       </c>
       <c r="BF4" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BG4" s="28" t="s">
         <v>35</v>
@@ -4981,17 +4983,17 @@
         <v>71</v>
       </c>
       <c r="BP4" s="9" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="BQ4" s="28" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="BR4" s="28"/>
       <c r="BS4" s="9" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="BT4" s="9" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="BU4" s="9" t="s">
         <v>40</v>
@@ -5004,7 +5006,7 @@
         <v>195</v>
       </c>
       <c r="BY4" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="BZ4" s="9" t="s">
         <v>48</v>
@@ -5023,16 +5025,16 @@
         <v>133</v>
       </c>
       <c r="CH4" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CI4" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="CJ4" s="28" t="s">
         <v>415</v>
       </c>
-      <c r="CJ4" s="28" t="s">
-        <v>420</v>
-      </c>
       <c r="CK4" s="9" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="CL4" s="28" t="s">
         <v>91</v>
@@ -5041,16 +5043,16 @@
         <v>138</v>
       </c>
       <c r="CN4" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CO4" s="28" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="CP4" s="28" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="CQ4" s="28" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="CR4" s="29" t="s">
         <v>200</v>
@@ -5070,19 +5072,19 @@
         <v>156</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="G5" s="28" t="s">
         <v>129</v>
@@ -5105,16 +5107,16 @@
       </c>
       <c r="N5" s="28"/>
       <c r="O5" s="28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P5" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Q5" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="R5" s="28" t="s">
         <v>354</v>
-      </c>
-      <c r="R5" s="28" t="s">
-        <v>355</v>
       </c>
       <c r="S5" s="29" t="s">
         <v>246</v>
@@ -5126,13 +5128,13 @@
         <v>36</v>
       </c>
       <c r="V5" s="28" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="W5" s="28" t="s">
         <v>122</v>
       </c>
       <c r="X5" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="Y5" s="28" t="s">
         <v>139</v>
@@ -5156,7 +5158,7 @@
         <v>36</v>
       </c>
       <c r="AF5" s="28" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="AG5" s="28" t="s">
         <v>9</v>
@@ -5165,7 +5167,7 @@
         <v>10</v>
       </c>
       <c r="AI5" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AJ5" s="28" t="s">
         <v>11</v>
@@ -5177,7 +5179,7 @@
         <v>56</v>
       </c>
       <c r="AM5" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AN5" s="28" t="s">
         <v>16</v>
@@ -5186,13 +5188,13 @@
         <v>129</v>
       </c>
       <c r="AP5" s="28" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="AQ5" s="28" t="s">
         <v>195</v>
       </c>
       <c r="AR5" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AS5" s="28" t="s">
         <v>158</v>
@@ -5220,19 +5222,19 @@
         <v>36</v>
       </c>
       <c r="BB5" s="28" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="BC5" s="28" t="s">
         <v>31</v>
       </c>
       <c r="BD5" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BE5" s="28" t="s">
         <v>34</v>
       </c>
       <c r="BF5" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BG5" s="28" t="s">
         <v>35</v>
@@ -5260,17 +5262,17 @@
         <v>71</v>
       </c>
       <c r="BP5" s="9" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="BQ5" s="28" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="BR5" s="28"/>
       <c r="BS5" s="9" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="BT5" s="9" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="BU5" s="9" t="s">
         <v>40</v>
@@ -5283,7 +5285,7 @@
         <v>195</v>
       </c>
       <c r="BY5" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="BZ5" s="9" t="s">
         <v>48</v>
@@ -5302,16 +5304,16 @@
         <v>133</v>
       </c>
       <c r="CH5" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CI5" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="CJ5" s="28" t="s">
         <v>415</v>
       </c>
-      <c r="CJ5" s="28" t="s">
-        <v>420</v>
-      </c>
       <c r="CK5" s="9" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="CL5" s="28" t="s">
         <v>91</v>
@@ -5320,16 +5322,16 @@
         <v>138</v>
       </c>
       <c r="CN5" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CO5" s="28" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="CP5" s="28" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="CQ5" s="28" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="CR5" s="29" t="s">
         <v>200</v>
@@ -5349,19 +5351,19 @@
         <v>163</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="G6" s="28" t="s">
         <v>129</v>
@@ -5384,16 +5386,16 @@
       </c>
       <c r="N6" s="28"/>
       <c r="O6" s="28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P6" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Q6" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="R6" s="28" t="s">
         <v>354</v>
-      </c>
-      <c r="R6" s="28" t="s">
-        <v>355</v>
       </c>
       <c r="S6" s="29" t="s">
         <v>246</v>
@@ -5405,13 +5407,13 @@
         <v>36</v>
       </c>
       <c r="V6" s="28" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="W6" s="28" t="s">
         <v>122</v>
       </c>
       <c r="X6" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="Y6" s="28" t="s">
         <v>139</v>
@@ -5435,7 +5437,7 @@
         <v>36</v>
       </c>
       <c r="AF6" s="28" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="AG6" s="28" t="s">
         <v>9</v>
@@ -5444,7 +5446,7 @@
         <v>10</v>
       </c>
       <c r="AI6" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AJ6" s="28" t="s">
         <v>11</v>
@@ -5456,7 +5458,7 @@
         <v>56</v>
       </c>
       <c r="AM6" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AN6" s="28" t="s">
         <v>16</v>
@@ -5465,13 +5467,13 @@
         <v>129</v>
       </c>
       <c r="AP6" s="28" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="AQ6" s="28" t="s">
         <v>195</v>
       </c>
       <c r="AR6" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AS6" s="28" t="s">
         <v>165</v>
@@ -5499,19 +5501,19 @@
         <v>36</v>
       </c>
       <c r="BB6" s="28" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="BC6" s="28" t="s">
         <v>31</v>
       </c>
       <c r="BD6" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BE6" s="28" t="s">
         <v>34</v>
       </c>
       <c r="BF6" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BG6" s="28" t="s">
         <v>35</v>
@@ -5539,17 +5541,17 @@
         <v>71</v>
       </c>
       <c r="BP6" s="9" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="BQ6" s="28" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="BR6" s="28"/>
       <c r="BS6" s="9" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="BT6" s="9" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="BU6" s="9" t="s">
         <v>40</v>
@@ -5562,7 +5564,7 @@
         <v>195</v>
       </c>
       <c r="BY6" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="BZ6" s="9" t="s">
         <v>48</v>
@@ -5581,16 +5583,16 @@
         <v>133</v>
       </c>
       <c r="CH6" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CI6" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="CJ6" s="28" t="s">
         <v>415</v>
       </c>
-      <c r="CJ6" s="28" t="s">
-        <v>420</v>
-      </c>
       <c r="CK6" s="9" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="CL6" s="28" t="s">
         <v>91</v>
@@ -5599,16 +5601,16 @@
         <v>138</v>
       </c>
       <c r="CN6" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CO6" s="28" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="CP6" s="28" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="CQ6" s="28" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="CR6" s="29" t="s">
         <v>200</v>
@@ -5628,19 +5630,19 @@
         <v>169</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="G7" s="28" t="s">
         <v>129</v>
@@ -5663,16 +5665,16 @@
       </c>
       <c r="N7" s="28"/>
       <c r="O7" s="28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P7" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Q7" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="R7" s="28" t="s">
         <v>354</v>
-      </c>
-      <c r="R7" s="28" t="s">
-        <v>355</v>
       </c>
       <c r="S7" s="29" t="s">
         <v>246</v>
@@ -5684,13 +5686,13 @@
         <v>36</v>
       </c>
       <c r="V7" s="28" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="W7" s="28" t="s">
         <v>122</v>
       </c>
       <c r="X7" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="Y7" s="28" t="s">
         <v>139</v>
@@ -5714,7 +5716,7 @@
         <v>36</v>
       </c>
       <c r="AF7" s="28" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="AG7" s="28" t="s">
         <v>9</v>
@@ -5723,7 +5725,7 @@
         <v>10</v>
       </c>
       <c r="AI7" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AJ7" s="28" t="s">
         <v>11</v>
@@ -5735,7 +5737,7 @@
         <v>56</v>
       </c>
       <c r="AM7" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AN7" s="28" t="s">
         <v>16</v>
@@ -5744,13 +5746,13 @@
         <v>129</v>
       </c>
       <c r="AP7" s="28" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="AQ7" s="28" t="s">
         <v>195</v>
       </c>
       <c r="AR7" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AS7" s="28" t="s">
         <v>171</v>
@@ -5778,19 +5780,19 @@
         <v>36</v>
       </c>
       <c r="BB7" s="28" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="BC7" s="28" t="s">
         <v>31</v>
       </c>
       <c r="BD7" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BE7" s="28" t="s">
         <v>34</v>
       </c>
       <c r="BF7" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BG7" s="28" t="s">
         <v>35</v>
@@ -5818,17 +5820,17 @@
         <v>71</v>
       </c>
       <c r="BP7" s="9" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="BQ7" s="28" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="BR7" s="28"/>
       <c r="BS7" s="9" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="BT7" s="9" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="BU7" s="9" t="s">
         <v>40</v>
@@ -5841,7 +5843,7 @@
         <v>195</v>
       </c>
       <c r="BY7" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="BZ7" s="9" t="s">
         <v>48</v>
@@ -5855,23 +5857,23 @@
       <c r="CC7" s="9"/>
       <c r="CD7" s="9"/>
       <c r="CE7" s="9" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="CF7" s="28"/>
       <c r="CG7" s="9" t="s">
         <v>133</v>
       </c>
       <c r="CH7" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CI7" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="CJ7" s="28" t="s">
         <v>415</v>
       </c>
-      <c r="CJ7" s="28" t="s">
-        <v>420</v>
-      </c>
       <c r="CK7" s="9" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="CL7" s="28" t="s">
         <v>91</v>
@@ -5880,16 +5882,16 @@
         <v>138</v>
       </c>
       <c r="CN7" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CO7" s="28" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="CP7" s="28" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="CQ7" s="28" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="CR7" s="29" t="s">
         <v>200</v>
@@ -5909,19 +5911,19 @@
         <v>175</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="G8" s="28" t="s">
         <v>129</v>
@@ -5944,16 +5946,16 @@
       </c>
       <c r="N8" s="28"/>
       <c r="O8" s="28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="P8" s="28" t="s">
         <v>245</v>
       </c>
       <c r="Q8" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="R8" s="28" t="s">
         <v>354</v>
-      </c>
-      <c r="R8" s="28" t="s">
-        <v>355</v>
       </c>
       <c r="S8" s="29" t="s">
         <v>246</v>
@@ -5965,13 +5967,13 @@
         <v>36</v>
       </c>
       <c r="V8" s="28" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="W8" s="28" t="s">
         <v>122</v>
       </c>
       <c r="X8" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="Y8" s="28" t="s">
         <v>139</v>
@@ -5995,7 +5997,7 @@
         <v>36</v>
       </c>
       <c r="AF8" s="28" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="AG8" s="28" t="s">
         <v>9</v>
@@ -6004,7 +6006,7 @@
         <v>10</v>
       </c>
       <c r="AI8" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AJ8" s="28" t="s">
         <v>11</v>
@@ -6016,7 +6018,7 @@
         <v>56</v>
       </c>
       <c r="AM8" s="28" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="AN8" s="28" t="s">
         <v>16</v>
@@ -6025,13 +6027,13 @@
         <v>129</v>
       </c>
       <c r="AP8" s="28" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="AQ8" s="28" t="s">
         <v>195</v>
       </c>
       <c r="AR8" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AS8" s="28" t="s">
         <v>177</v>
@@ -6059,19 +6061,19 @@
         <v>36</v>
       </c>
       <c r="BB8" s="28" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="BC8" s="28" t="s">
         <v>31</v>
       </c>
       <c r="BD8" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BE8" s="28" t="s">
         <v>34</v>
       </c>
       <c r="BF8" s="28" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="BG8" s="28" t="s">
         <v>35</v>
@@ -6099,17 +6101,17 @@
         <v>71</v>
       </c>
       <c r="BP8" s="9" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="BQ8" s="28" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="BR8" s="28"/>
       <c r="BS8" s="9" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="BT8" s="9" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="BU8" s="9" t="s">
         <v>40</v>
@@ -6122,7 +6124,7 @@
         <v>195</v>
       </c>
       <c r="BY8" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="BZ8" s="9" t="s">
         <v>48</v>
@@ -6136,23 +6138,23 @@
       <c r="CC8" s="9"/>
       <c r="CD8" s="9"/>
       <c r="CE8" s="9" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="CF8" s="28"/>
       <c r="CG8" s="9" t="s">
         <v>133</v>
       </c>
       <c r="CH8" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CI8" s="28" t="s">
+        <v>410</v>
+      </c>
+      <c r="CJ8" s="28" t="s">
         <v>415</v>
       </c>
-      <c r="CJ8" s="28" t="s">
-        <v>420</v>
-      </c>
       <c r="CK8" s="9" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="CL8" s="28" t="s">
         <v>91</v>
@@ -6161,16 +6163,16 @@
         <v>138</v>
       </c>
       <c r="CN8" s="28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="CO8" s="28" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="CP8" s="28" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="CQ8" s="28" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="CR8" s="29" t="s">
         <v>200</v>
@@ -7542,17 +7544,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA2"/>
+  <dimension ref="A1:AT4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AU1" sqref="AU1:BA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
@@ -7576,285 +7578,266 @@
     <col min="30" max="30" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:46" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>307</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>358</v>
+        <v>297</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>298</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>297</v>
+        <v>209</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>298</v>
+        <v>210</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>359</v>
+        <v>211</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>299</v>
+        <v>212</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>300</v>
+        <v>213</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="AC1" s="1" t="s">
-        <v>222</v>
+        <v>361</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>223</v>
+        <v>114</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>226</v>
+        <v>362</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>227</v>
+        <v>363</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>114</v>
+        <v>366</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>228</v>
+        <v>367</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>229</v>
+        <v>368</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="BA1" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="2" spans="1:53" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:46" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>357</v>
+        <v>463</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>464</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>377</v>
-      </c>
-      <c r="D2" s="9">
-        <v>8520</v>
+        <v>230</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>465</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>187</v>
+        <v>230</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>378</v>
+        <v>134</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>230</v>
-      </c>
+      <c r="H2" s="9"/>
       <c r="I2" s="9" t="s">
         <v>230</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>134</v>
+        <v>230</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>134</v>
+        <v>230</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="M2" s="28"/>
+        <v>121</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>231</v>
+      </c>
       <c r="N2" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="O2" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>230</v>
+      <c r="O2" s="9">
+        <v>16</v>
+      </c>
+      <c r="P2" s="9">
+        <v>16</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="U2" s="9">
-        <v>16</v>
-      </c>
-      <c r="V2" s="9">
-        <v>16</v>
-      </c>
-      <c r="W2" s="9"/>
-      <c r="X2" s="9"/>
+        <v>466</v>
+      </c>
+      <c r="R2" s="9">
+        <v>1100440052</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="T2" s="9">
+        <v>45665456</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" s="9">
+        <v>1113332</v>
+      </c>
+      <c r="X2" s="9">
+        <v>23564589</v>
+      </c>
       <c r="Y2" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF2" s="9">
+        <v>411006</v>
+      </c>
+      <c r="AG2" s="9">
+        <v>124421</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="Z2" s="33" t="s">
-        <v>232</v>
-      </c>
-      <c r="AA2" s="9">
-        <v>45665456</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AO2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AD2" s="9">
-        <v>1113332</v>
-      </c>
-      <c r="AE2" s="9">
-        <v>23564589</v>
-      </c>
-      <c r="AF2" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="AG2" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="AH2" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="AI2" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="AJ2" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="AK2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL2" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="AM2" s="9">
-        <v>411006</v>
-      </c>
-      <c r="AN2" s="9">
-        <v>124421</v>
-      </c>
-      <c r="AO2" s="9" t="s">
-        <v>389</v>
-      </c>
-      <c r="AP2" s="9" t="s">
-        <v>388</v>
+      <c r="AP2" s="9">
+        <v>5431267812</v>
       </c>
       <c r="AQ2" s="9" t="s">
         <v>380</v>
@@ -7862,36 +7845,291 @@
       <c r="AR2" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="9"/>
-      <c r="AU2" s="9" t="s">
+      <c r="AS2" s="9">
+        <v>999</v>
+      </c>
+      <c r="AT2" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="AV2" s="9" t="s">
+    </row>
+    <row r="3" spans="1:46" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>464</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="M3" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O3" s="9">
+        <v>16</v>
+      </c>
+      <c r="P3" s="9">
+        <v>16</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="R3" s="9">
+        <v>1100440052</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="T3" s="9">
+        <v>45665456</v>
+      </c>
+      <c r="U3" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="V3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AW2" s="32" t="s">
+      <c r="W3" s="9">
+        <v>1113332</v>
+      </c>
+      <c r="X3" s="9">
+        <v>23564589</v>
+      </c>
+      <c r="Y3" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="Z3" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AA3" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE3" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF3" s="9">
+        <v>411006</v>
+      </c>
+      <c r="AG3" s="9">
+        <v>124421</v>
+      </c>
+      <c r="AH3" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="AI3" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="AX2" s="9" t="s">
+      <c r="AJ3" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="AK3" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="AL3" s="9"/>
+      <c r="AM3" s="9"/>
+      <c r="AN3" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="AO3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP3" s="9">
+        <v>5431267812</v>
+      </c>
+      <c r="AQ3" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="AR3" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="AS3" s="9">
+        <v>999</v>
+      </c>
+      <c r="AT3" s="9" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>464</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="M4" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O4" s="9">
+        <v>16</v>
+      </c>
+      <c r="P4" s="9">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>466</v>
+      </c>
+      <c r="R4" s="9">
+        <v>1100440052</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="T4" s="9">
+        <v>45665456</v>
+      </c>
+      <c r="U4" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W4" s="9">
+        <v>1113332</v>
+      </c>
+      <c r="X4" s="9">
+        <v>23564589</v>
+      </c>
+      <c r="Y4" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="Z4" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AA4" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AB4" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AC4" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE4" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AF4" s="9">
+        <v>411006</v>
+      </c>
+      <c r="AG4" s="9">
+        <v>124421</v>
+      </c>
+      <c r="AH4" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="AY2" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="AZ2" s="9" t="s">
-        <v>387</v>
-      </c>
-      <c r="BA2" s="9" t="s">
-        <v>386</v>
+      <c r="AI4" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="AJ4" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="AK4" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="AL4" s="9"/>
+      <c r="AM4" s="9"/>
+      <c r="AN4" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="AO4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP4" s="9">
+        <v>5431267812</v>
+      </c>
+      <c r="AQ4" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="AR4" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="AS4" s="9">
+        <v>999</v>
+      </c>
+      <c r="AT4" s="9" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Y2" r:id="rId1" display="auto@mail.com"/>
-    <hyperlink ref="S2" r:id="rId2" display="auto12@mail.com"/>
+    <hyperlink ref="S2" r:id="rId1"/>
+    <hyperlink ref="Y2" r:id="rId2"/>
+    <hyperlink ref="S3" r:id="rId3"/>
+    <hyperlink ref="Y3" r:id="rId4"/>
+    <hyperlink ref="S4" r:id="rId5"/>
+    <hyperlink ref="Y4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added script to generate audit report
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12945" windowHeight="6750" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12945" windowHeight="6750" firstSheet="12" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,14 @@
     <sheet name="CurrencyExchangeRateMapping" sheetId="14" r:id="rId14"/>
     <sheet name="LoyaltyPlan" sheetId="17" r:id="rId15"/>
     <sheet name="Prepaid_Application_Upload" sheetId="16" r:id="rId16"/>
+    <sheet name="AuditReport" sheetId="18" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2275" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2299" uniqueCount="586">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1745,6 +1746,48 @@
   </si>
   <si>
     <t>ExistingInstitutionCode</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>MODIFY</t>
+  </si>
+  <si>
+    <t>PROGRAM</t>
+  </si>
+  <si>
+    <t>PDF Format [pdf]</t>
+  </si>
+  <si>
+    <t>Online [O]</t>
+  </si>
+  <si>
+    <t>TC_validate_Audit_Report</t>
+  </si>
+  <si>
+    <t>ReportName</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>ScreenName</t>
+  </si>
+  <si>
+    <t>FileType</t>
+  </si>
+  <si>
+    <t>ReportGenerationMode</t>
+  </si>
+  <si>
+    <t>Audit Report</t>
+  </si>
+  <si>
+    <t>AU01</t>
+  </si>
+  <si>
+    <t>http://ech-10-168-131-92.mastercard.int:25003/integratedIssuing-customerPortal/mpts/app/Login</t>
   </si>
 </sst>
 </file>
@@ -1893,7 +1936,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1980,6 +2023,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3790,7 +3834,7 @@
   <dimension ref="A1:EE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4589,7 +4633,7 @@
   <dimension ref="A1:EE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5383,12 +5427,112 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>585</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>536</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>398</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DN177"/>
   <sheetViews>
-    <sheetView topLeftCell="CI1" workbookViewId="0">
-      <selection activeCell="CU3" sqref="CU3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9124,8 +9268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BH1" sqref="BH1:BL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new Application Prepaid changes
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2226" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="568">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1594,9 +1594,6 @@
     <t>TC_Application_Upload_Prepaid</t>
   </si>
   <si>
-    <t>http://ech-10-168-128-251.mastercard.int:25003/integratedIssuing-customerPortal/mpts/app/Login</t>
-  </si>
-  <si>
     <t>AUTO [121212]</t>
   </si>
   <si>
@@ -1727,6 +1724,15 @@
   </si>
   <si>
     <t>http://ech-10-168-128-92.mastercard.int:25003/integratedIssuing-customerPortal/mpts/app/Login</t>
+  </si>
+  <si>
+    <t>http://ech-10-168-131-92.mastercard.int:25003/integratedIssuing-customerPortal/mtps/app/Login</t>
+  </si>
+  <si>
+    <t>WalletPlanDescription</t>
+  </si>
+  <si>
+    <t>WalletPlancode</t>
   </si>
 </sst>
 </file>
@@ -4186,64 +4192,64 @@
     </row>
     <row r="2" spans="1:135" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="B2" t="s">
         <v>564</v>
       </c>
-      <c r="B2" t="s">
-        <v>565</v>
-      </c>
       <c r="C2" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D2" s="38" t="s">
         <v>522</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="E2" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>525</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>526</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>134</v>
       </c>
       <c r="I2" s="28" t="s">
+        <v>526</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="39" t="s">
         <v>528</v>
       </c>
-      <c r="K2" s="39" t="s">
+      <c r="L2" s="39" t="s">
         <v>529</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="M2" s="39" t="s">
         <v>530</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="N2" s="40" t="s">
         <v>531</v>
       </c>
-      <c r="N2" s="40" t="s">
+      <c r="O2" s="40" t="s">
         <v>532</v>
       </c>
-      <c r="O2" s="40" t="s">
+      <c r="P2" s="40" t="s">
+        <v>532</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="P2" s="40" t="s">
-        <v>533</v>
-      </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="40" t="s">
         <v>534</v>
       </c>
-      <c r="R2" s="40" t="s">
+      <c r="S2" s="40" t="s">
         <v>535</v>
       </c>
-      <c r="S2" s="40" t="s">
+      <c r="T2" s="40" t="s">
         <v>536</v>
-      </c>
-      <c r="T2" s="40" t="s">
-        <v>537</v>
       </c>
       <c r="U2" s="11">
         <v>50</v>
@@ -4271,16 +4277,16 @@
       </c>
       <c r="AE2" s="12"/>
       <c r="AF2" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="AG2" s="12" t="s">
         <v>538</v>
       </c>
-      <c r="AG2" s="12" t="s">
+      <c r="AH2" s="12" t="s">
         <v>539</v>
       </c>
-      <c r="AH2" s="12" t="s">
+      <c r="AI2" s="12" t="s">
         <v>540</v>
-      </c>
-      <c r="AI2" s="12" t="s">
-        <v>541</v>
       </c>
       <c r="AJ2" s="12" t="s">
         <v>36</v>
@@ -4301,7 +4307,7 @@
         <v>121</v>
       </c>
       <c r="AP2" s="12" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AQ2" s="12" t="s">
         <v>120</v>
@@ -4338,7 +4344,7 @@
         <v>1</v>
       </c>
       <c r="BC2" s="12" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="BD2" s="12" t="s">
         <v>16</v>
@@ -4350,7 +4356,7 @@
         <v>12</v>
       </c>
       <c r="BG2" s="12" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="BH2" s="12">
         <v>2</v>
@@ -4368,7 +4374,7 @@
         <v>29</v>
       </c>
       <c r="BM2" s="12" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="BN2" s="12" t="s">
         <v>199</v>
@@ -4398,20 +4404,20 @@
         <v>12345678</v>
       </c>
       <c r="BW2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="BX2" s="43"/>
       <c r="BY2" s="12" t="s">
         <v>143</v>
       </c>
       <c r="BZ2" s="12" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="CA2" s="12" t="s">
         <v>136</v>
       </c>
       <c r="CB2" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="CC2" s="12" t="s">
         <v>67</v>
@@ -4438,13 +4444,13 @@
         <v>40</v>
       </c>
       <c r="CM2" s="43" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="CN2" s="12" t="s">
         <v>145</v>
       </c>
       <c r="CO2" s="11" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="CP2" s="41" t="s">
         <v>355</v>
@@ -4461,7 +4467,7 @@
       <c r="CT2" s="11"/>
       <c r="CU2" s="11"/>
       <c r="CV2" s="41" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="CW2" s="12" t="s">
         <v>133</v>
@@ -4498,40 +4504,40 @@
         <v>53</v>
       </c>
       <c r="DK2" s="11" t="s">
+        <v>548</v>
+      </c>
+      <c r="DL2" s="11" t="s">
         <v>549</v>
       </c>
-      <c r="DL2" s="11" t="s">
+      <c r="DM2" s="12" t="s">
         <v>550</v>
-      </c>
-      <c r="DM2" s="12" t="s">
-        <v>551</v>
       </c>
       <c r="DN2" s="12" t="s">
         <v>197</v>
       </c>
       <c r="DO2" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="DP2" s="44" t="s">
         <v>552</v>
       </c>
-      <c r="DP2" s="44" t="s">
+      <c r="DQ2" s="44" t="s">
         <v>553</v>
       </c>
-      <c r="DQ2" s="44" t="s">
+      <c r="DR2" s="44" t="s">
         <v>554</v>
       </c>
-      <c r="DR2" s="44" t="s">
+      <c r="DS2" s="45" t="s">
         <v>555</v>
-      </c>
-      <c r="DS2" s="45" t="s">
-        <v>556</v>
       </c>
       <c r="DT2" s="45" t="s">
         <v>405</v>
       </c>
       <c r="DU2" s="45" t="s">
+        <v>556</v>
+      </c>
+      <c r="DV2" s="44" t="s">
         <v>557</v>
-      </c>
-      <c r="DV2" s="44" t="s">
-        <v>558</v>
       </c>
       <c r="DW2" s="44" t="s">
         <v>134</v>
@@ -4540,25 +4546,25 @@
         <v>404</v>
       </c>
       <c r="DY2" s="45" t="s">
+        <v>558</v>
+      </c>
+      <c r="DZ2" s="45" t="s">
         <v>559</v>
       </c>
-      <c r="DZ2" s="45" t="s">
+      <c r="EA2" s="45" t="s">
+        <v>530</v>
+      </c>
+      <c r="EB2" s="45" t="s">
+        <v>559</v>
+      </c>
+      <c r="EC2" s="45" t="s">
         <v>560</v>
       </c>
-      <c r="EA2" s="45" t="s">
-        <v>531</v>
-      </c>
-      <c r="EB2" s="45" t="s">
-        <v>560</v>
-      </c>
-      <c r="EC2" s="45" t="s">
+      <c r="ED2" s="45" t="s">
         <v>561</v>
       </c>
-      <c r="ED2" s="45" t="s">
+      <c r="EE2" s="44" t="s">
         <v>562</v>
-      </c>
-      <c r="EE2" s="44" t="s">
-        <v>563</v>
       </c>
     </row>
   </sheetData>
@@ -4568,15 +4574,15 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EE2"/>
+  <dimension ref="A1:EG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="DG1" workbookViewId="0">
+      <selection activeCell="DY12" sqref="DY12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:135" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:137" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4977,72 +4983,78 @@
         <v>517</v>
       </c>
       <c r="ED1" s="37" t="s">
+        <v>566</v>
+      </c>
+      <c r="EE1" s="37" t="s">
+        <v>567</v>
+      </c>
+      <c r="EF1" s="37" t="s">
         <v>518</v>
       </c>
-      <c r="EE1" s="37" t="s">
+      <c r="EG1" s="37" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="2" spans="1:135" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:137" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>520</v>
       </c>
       <c r="B2" t="s">
+        <v>565</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="38" t="s">
         <v>522</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="E2" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>525</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>526</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>134</v>
       </c>
       <c r="I2" s="28" t="s">
+        <v>526</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="39" t="s">
         <v>528</v>
       </c>
-      <c r="K2" s="39" t="s">
+      <c r="L2" s="39" t="s">
         <v>529</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="M2" s="39" t="s">
         <v>530</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="N2" s="40" t="s">
         <v>531</v>
       </c>
-      <c r="N2" s="40" t="s">
+      <c r="O2" s="40" t="s">
         <v>532</v>
       </c>
-      <c r="O2" s="40" t="s">
+      <c r="P2" s="40" t="s">
+        <v>532</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="P2" s="40" t="s">
-        <v>533</v>
-      </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="40" t="s">
         <v>534</v>
       </c>
-      <c r="R2" s="40" t="s">
+      <c r="S2" s="40" t="s">
         <v>535</v>
       </c>
-      <c r="S2" s="40" t="s">
+      <c r="T2" s="40" t="s">
         <v>536</v>
-      </c>
-      <c r="T2" s="40" t="s">
-        <v>537</v>
       </c>
       <c r="U2" s="11">
         <v>50</v>
@@ -5070,16 +5082,16 @@
       </c>
       <c r="AE2" s="12"/>
       <c r="AF2" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="AG2" s="12" t="s">
         <v>538</v>
       </c>
-      <c r="AG2" s="12" t="s">
+      <c r="AH2" s="12" t="s">
         <v>539</v>
       </c>
-      <c r="AH2" s="12" t="s">
+      <c r="AI2" s="12" t="s">
         <v>540</v>
-      </c>
-      <c r="AI2" s="12" t="s">
-        <v>541</v>
       </c>
       <c r="AJ2" s="12" t="s">
         <v>36</v>
@@ -5100,7 +5112,7 @@
         <v>121</v>
       </c>
       <c r="AP2" s="12" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AQ2" s="12" t="s">
         <v>120</v>
@@ -5137,7 +5149,7 @@
         <v>1</v>
       </c>
       <c r="BC2" s="12" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="BD2" s="12" t="s">
         <v>16</v>
@@ -5149,7 +5161,7 @@
         <v>12</v>
       </c>
       <c r="BG2" s="12" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="BH2" s="12">
         <v>2</v>
@@ -5167,7 +5179,7 @@
         <v>29</v>
       </c>
       <c r="BM2" s="12" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="BN2" s="12" t="s">
         <v>199</v>
@@ -5197,20 +5209,20 @@
         <v>12345678</v>
       </c>
       <c r="BW2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="BX2" s="43"/>
       <c r="BY2" s="12" t="s">
         <v>143</v>
       </c>
       <c r="BZ2" s="12" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="CA2" s="12" t="s">
         <v>136</v>
       </c>
       <c r="CB2" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="CC2" s="12" t="s">
         <v>67</v>
@@ -5237,13 +5249,13 @@
         <v>40</v>
       </c>
       <c r="CM2" s="43" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="CN2" s="12" t="s">
         <v>145</v>
       </c>
       <c r="CO2" s="11" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="CP2" s="41" t="s">
         <v>355</v>
@@ -5260,7 +5272,7 @@
       <c r="CT2" s="11"/>
       <c r="CU2" s="11"/>
       <c r="CV2" s="41" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="CW2" s="12" t="s">
         <v>133</v>
@@ -5297,40 +5309,40 @@
         <v>53</v>
       </c>
       <c r="DK2" s="11" t="s">
+        <v>548</v>
+      </c>
+      <c r="DL2" s="11" t="s">
         <v>549</v>
       </c>
-      <c r="DL2" s="11" t="s">
+      <c r="DM2" s="12" t="s">
         <v>550</v>
-      </c>
-      <c r="DM2" s="12" t="s">
-        <v>551</v>
       </c>
       <c r="DN2" s="12" t="s">
         <v>197</v>
       </c>
       <c r="DO2" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="DP2" s="44" t="s">
         <v>552</v>
       </c>
-      <c r="DP2" s="44" t="s">
+      <c r="DQ2" s="44" t="s">
         <v>553</v>
       </c>
-      <c r="DQ2" s="44" t="s">
+      <c r="DR2" s="44" t="s">
         <v>554</v>
       </c>
-      <c r="DR2" s="44" t="s">
+      <c r="DS2" s="45" t="s">
         <v>555</v>
-      </c>
-      <c r="DS2" s="45" t="s">
-        <v>556</v>
       </c>
       <c r="DT2" s="45" t="s">
         <v>405</v>
       </c>
       <c r="DU2" s="45" t="s">
+        <v>556</v>
+      </c>
+      <c r="DV2" s="44" t="s">
         <v>557</v>
-      </c>
-      <c r="DV2" s="44" t="s">
-        <v>558</v>
       </c>
       <c r="DW2" s="44" t="s">
         <v>134</v>
@@ -5339,25 +5351,27 @@
         <v>404</v>
       </c>
       <c r="DY2" s="45" t="s">
+        <v>558</v>
+      </c>
+      <c r="DZ2" s="45" t="s">
         <v>559</v>
       </c>
-      <c r="DZ2" s="45" t="s">
+      <c r="EA2" s="45" t="s">
+        <v>530</v>
+      </c>
+      <c r="EB2" s="45" t="s">
+        <v>559</v>
+      </c>
+      <c r="EC2" s="45" t="s">
         <v>560</v>
       </c>
-      <c r="EA2" s="45" t="s">
-        <v>531</v>
-      </c>
-      <c r="EB2" s="45" t="s">
-        <v>560</v>
-      </c>
-      <c r="EC2" s="45" t="s">
+      <c r="ED2" s="45"/>
+      <c r="EE2" s="45"/>
+      <c r="EF2" s="45" t="s">
         <v>561</v>
       </c>
-      <c r="ED2" s="45" t="s">
+      <c r="EG2" s="44" t="s">
         <v>562</v>
-      </c>
-      <c r="EE2" s="44" t="s">
-        <v>563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code refactoring and credit FileUpload scenarios added
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12945" windowHeight="6750" firstSheet="11" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12945" windowHeight="6750" firstSheet="12" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,14 @@
     <sheet name="CurrencyExchangeRateMapping" sheetId="14" r:id="rId14"/>
     <sheet name="LoyaltyPlan" sheetId="17" r:id="rId15"/>
     <sheet name="Prepaid_Application_Upload" sheetId="16" r:id="rId16"/>
+    <sheet name="AuditReport" sheetId="18" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2424" uniqueCount="600">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1726,13 +1727,109 @@
     <t>http://ech-10-168-128-92.mastercard.int:25003/integratedIssuing-customerPortal/mpts/app/Login</t>
   </si>
   <si>
+    <t>ASC_Vendor</t>
+  </si>
+  <si>
+    <t>MPIN</t>
+  </si>
+  <si>
+    <t>SmsProvider</t>
+  </si>
+  <si>
+    <t>WIBMO [002]</t>
+  </si>
+  <si>
+    <t>TCEditInstitute</t>
+  </si>
+  <si>
+    <t>ExistingInstitutionCode</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>MODIFY</t>
+  </si>
+  <si>
+    <t>PROGRAM</t>
+  </si>
+  <si>
+    <t>PDF Format [pdf]</t>
+  </si>
+  <si>
+    <t>Online [O]</t>
+  </si>
+  <si>
+    <t>TC_validate_Audit_Report</t>
+  </si>
+  <si>
+    <t>ReportName</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>ScreenName</t>
+  </si>
+  <si>
+    <t>FileType</t>
+  </si>
+  <si>
+    <t>ReportGenerationMode</t>
+  </si>
+  <si>
+    <t>Audit Report</t>
+  </si>
+  <si>
+    <t>AU01</t>
+  </si>
+  <si>
+    <t>http://ech-10-168-131-92.mastercard.int:25003/integratedIssuing-customerPortal/mpts/app/Login</t>
+  </si>
+  <si>
+    <t>WalletPlanDescription</t>
+  </si>
+  <si>
+    <t>WalletPlancode</t>
+  </si>
+  <si>
+    <t>creditLimit</t>
+  </si>
+  <si>
+    <t>maxCreditLimit</t>
+  </si>
+  <si>
+    <t>cashLimitType</t>
+  </si>
+  <si>
+    <t>cashLimitAmount</t>
+  </si>
+  <si>
+    <t>cashLimitReset</t>
+  </si>
+  <si>
+    <t>addOnLimitReset</t>
+  </si>
+  <si>
     <t>http://ech-10-168-131-92.mastercard.int:25003/integratedIssuing-customerPortal/mtps/app/Login</t>
   </si>
   <si>
-    <t>WalletPlanDescription</t>
-  </si>
-  <si>
-    <t>WalletPlancode</t>
+    <t>TC_Application_Upload_Credit</t>
+  </si>
+  <si>
+    <t>554466</t>
+  </si>
+  <si>
+    <t>Credit[C}</t>
+  </si>
+  <si>
+    <t>10-2028</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>Payment [1]</t>
   </si>
 </sst>
 </file>
@@ -1881,7 +1978,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1968,6 +2065,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3778,7 +3877,7 @@
   <dimension ref="A1:EE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4574,15 +4673,20 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EG2"/>
+  <dimension ref="A1:EM3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DG1" workbookViewId="0">
-      <selection activeCell="DY12" sqref="DY12"/>
+    <sheetView tabSelected="1" topLeftCell="DD1" workbookViewId="0">
+      <selection activeCell="DV6" sqref="DV6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:137" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:143" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -4983,24 +5087,42 @@
         <v>517</v>
       </c>
       <c r="ED1" s="37" t="s">
-        <v>566</v>
+        <v>585</v>
       </c>
       <c r="EE1" s="37" t="s">
-        <v>567</v>
+        <v>586</v>
       </c>
       <c r="EF1" s="37" t="s">
         <v>518</v>
       </c>
       <c r="EG1" s="37" t="s">
+        <v>587</v>
+      </c>
+      <c r="EH1" s="37" t="s">
+        <v>588</v>
+      </c>
+      <c r="EI1" s="37" t="s">
+        <v>589</v>
+      </c>
+      <c r="EJ1" s="37" t="s">
+        <v>590</v>
+      </c>
+      <c r="EK1" s="37" t="s">
+        <v>591</v>
+      </c>
+      <c r="EL1" s="37" t="s">
+        <v>592</v>
+      </c>
+      <c r="EM1" s="37" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="2" spans="1:137" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:143" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>520</v>
       </c>
       <c r="B2" t="s">
-        <v>565</v>
+        <v>593</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>521</v>
@@ -5370,12 +5492,515 @@
       <c r="EF2" s="45" t="s">
         <v>561</v>
       </c>
-      <c r="EG2" s="44" t="s">
+      <c r="EG2" s="45"/>
+      <c r="EH2" s="45"/>
+      <c r="EI2" s="45"/>
+      <c r="EJ2" s="45"/>
+      <c r="EK2" s="45"/>
+      <c r="EL2" s="45"/>
+      <c r="EM2" s="44" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="3" spans="1:143" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="B3" t="s">
+        <v>593</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>595</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>526</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="K3" s="39" t="s">
+        <v>528</v>
+      </c>
+      <c r="L3" s="39" t="s">
+        <v>529</v>
+      </c>
+      <c r="M3" s="39" t="s">
+        <v>530</v>
+      </c>
+      <c r="N3" s="40" t="s">
+        <v>531</v>
+      </c>
+      <c r="O3" s="40" t="s">
+        <v>532</v>
+      </c>
+      <c r="P3" s="40" t="s">
+        <v>532</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="R3" s="40" t="s">
+        <v>534</v>
+      </c>
+      <c r="S3" s="40" t="s">
+        <v>389</v>
+      </c>
+      <c r="T3" s="40" t="s">
+        <v>536</v>
+      </c>
+      <c r="U3" s="11">
+        <v>50</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>596</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="12"/>
+      <c r="AD3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE3" s="12"/>
+      <c r="AF3" s="11" t="s">
+        <v>537</v>
+      </c>
+      <c r="AG3" s="12" t="s">
+        <v>538</v>
+      </c>
+      <c r="AH3" s="12" t="s">
+        <v>539</v>
+      </c>
+      <c r="AI3" s="12" t="s">
+        <v>540</v>
+      </c>
+      <c r="AJ3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK3" s="12">
+        <v>1989</v>
+      </c>
+      <c r="AL3" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM3" s="14">
+        <v>12345678</v>
+      </c>
+      <c r="AN3" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="AO3" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP3" s="12" t="s">
+        <v>541</v>
+      </c>
+      <c r="AQ3" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="AR3" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="AS3" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="AT3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU3" s="11"/>
+      <c r="AV3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AW3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="AX3" s="11">
+        <v>1</v>
+      </c>
+      <c r="AY3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AZ3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="BA3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="BB3" s="12">
+        <v>1</v>
+      </c>
+      <c r="BC3" s="12" t="s">
+        <v>542</v>
+      </c>
+      <c r="BD3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="BE3" s="12" t="s">
+        <v>596</v>
+      </c>
+      <c r="BF3" s="12">
+        <v>12</v>
+      </c>
+      <c r="BG3" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="BH3" s="12">
+        <v>2</v>
+      </c>
+      <c r="BI3" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="BJ3" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK3" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="BL3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="BM3" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="BN3" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="BO3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="BP3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="BQ3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="BR3" s="42" t="s">
+        <v>406</v>
+      </c>
+      <c r="BS3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="BT3" s="12">
+        <v>12345678</v>
+      </c>
+      <c r="BU3" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="BV3" s="12">
+        <v>12345678</v>
+      </c>
+      <c r="BW3" t="s">
+        <v>545</v>
+      </c>
+      <c r="BX3" s="43"/>
+      <c r="BY3" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="BZ3" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="CA3" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="CB3" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="CC3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="CD3" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="CE3" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="CF3" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="CG3" s="12"/>
+      <c r="CH3" s="43" t="s">
+        <v>405</v>
+      </c>
+      <c r="CI3" s="43" t="s">
+        <v>407</v>
+      </c>
+      <c r="CJ3" s="41"/>
+      <c r="CK3" s="41"/>
+      <c r="CL3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="CM3" s="43" t="s">
+        <v>547</v>
+      </c>
+      <c r="CN3" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="CO3" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="CP3" s="41" t="s">
+        <v>355</v>
+      </c>
+      <c r="CQ3" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="CR3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="CS3" s="47" t="s">
+        <v>597</v>
+      </c>
+      <c r="CT3" s="11"/>
+      <c r="CU3" s="11"/>
+      <c r="CV3" s="41" t="s">
+        <v>532</v>
+      </c>
+      <c r="CW3" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="CX3" s="41" t="s">
+        <v>409</v>
+      </c>
+      <c r="CY3" s="41" t="s">
+        <v>405</v>
+      </c>
+      <c r="CZ3" s="41" t="s">
+        <v>410</v>
+      </c>
+      <c r="DA3" s="41" t="s">
+        <v>411</v>
+      </c>
+      <c r="DB3" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="DC3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="DD3" s="12"/>
+      <c r="DE3" s="12"/>
+      <c r="DF3" s="12"/>
+      <c r="DG3" s="12"/>
+      <c r="DH3" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="DI3" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="DJ3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="DK3" s="11" t="s">
+        <v>548</v>
+      </c>
+      <c r="DL3" s="11" t="s">
+        <v>549</v>
+      </c>
+      <c r="DM3" s="12" t="s">
+        <v>550</v>
+      </c>
+      <c r="DN3" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="DO3" s="11" t="s">
+        <v>551</v>
+      </c>
+      <c r="DP3" s="44" t="s">
+        <v>552</v>
+      </c>
+      <c r="DQ3" s="44" t="s">
+        <v>553</v>
+      </c>
+      <c r="DR3" s="44" t="s">
+        <v>554</v>
+      </c>
+      <c r="DS3" s="45" t="s">
+        <v>555</v>
+      </c>
+      <c r="DT3" s="45" t="s">
+        <v>405</v>
+      </c>
+      <c r="DU3" s="45" t="s">
+        <v>556</v>
+      </c>
+      <c r="DV3" s="44" t="s">
+        <v>557</v>
+      </c>
+      <c r="DW3" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="DX3" s="45" t="s">
+        <v>404</v>
+      </c>
+      <c r="DY3" s="45" t="s">
+        <v>558</v>
+      </c>
+      <c r="DZ3" s="45" t="s">
+        <v>559</v>
+      </c>
+      <c r="EA3" s="45" t="s">
+        <v>530</v>
+      </c>
+      <c r="EB3" s="45" t="s">
+        <v>559</v>
+      </c>
+      <c r="EC3" s="45" t="s">
+        <v>560</v>
+      </c>
+      <c r="ED3" s="45"/>
+      <c r="EE3" s="45"/>
+      <c r="EF3" s="45" t="s">
+        <v>561</v>
+      </c>
+      <c r="EG3" s="45" t="s">
+        <v>410</v>
+      </c>
+      <c r="EH3" s="45" t="s">
+        <v>409</v>
+      </c>
+      <c r="EI3" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="EJ3" s="45" t="s">
+        <v>598</v>
+      </c>
+      <c r="EK3" s="45" t="s">
+        <v>599</v>
+      </c>
+      <c r="EL3" s="45" t="s">
+        <v>599</v>
+      </c>
+      <c r="EM3" s="44" t="s">
         <v>562</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>584</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>398</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5383,8 +6008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DN177"/>
   <sheetViews>
-    <sheetView topLeftCell="CI1" workbookViewId="0">
-      <selection activeCell="CU3" sqref="CU3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9118,10 +9743,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC11"/>
+  <dimension ref="A1:BG12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="BH1" sqref="BH1:BL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9162,9 +9787,12 @@
     <col min="53" max="53" width="21.85546875" customWidth="1"/>
     <col min="54" max="54" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="15.85546875" customWidth="1"/>
+    <col min="56" max="56" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -9330,8 +9958,20 @@
       <c r="BC1" s="1" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="2" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD1" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="BG1" s="1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="2" spans="1:59" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>447</v>
       </c>
@@ -9491,8 +10131,12 @@
         <v>460</v>
       </c>
       <c r="BC2" s="9"/>
-    </row>
-    <row r="3" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD2" s="9"/>
+      <c r="BE2" s="9"/>
+      <c r="BF2" s="9"/>
+      <c r="BG2" s="9"/>
+    </row>
+    <row r="3" spans="1:59" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>449</v>
       </c>
@@ -9650,8 +10294,12 @@
       </c>
       <c r="BB3" s="9"/>
       <c r="BC3" s="9"/>
-    </row>
-    <row r="4" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD3" s="9"/>
+      <c r="BE3" s="9"/>
+      <c r="BF3" s="9"/>
+      <c r="BG3" s="9"/>
+    </row>
+    <row r="4" spans="1:59" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>462</v>
       </c>
@@ -9809,8 +10457,12 @@
       </c>
       <c r="BB4" s="9"/>
       <c r="BC4" s="9"/>
-    </row>
-    <row r="5" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD4" s="9"/>
+      <c r="BE4" s="9"/>
+      <c r="BF4" s="9"/>
+      <c r="BG4" s="9"/>
+    </row>
+    <row r="5" spans="1:59" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>450</v>
       </c>
@@ -9970,8 +10622,12 @@
         <v>482</v>
       </c>
       <c r="BC5" s="9"/>
-    </row>
-    <row r="6" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD5" s="9"/>
+      <c r="BE5" s="9"/>
+      <c r="BF5" s="9"/>
+      <c r="BG5" s="9"/>
+    </row>
+    <row r="6" spans="1:59" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>461</v>
       </c>
@@ -10131,8 +10787,12 @@
         <v>460</v>
       </c>
       <c r="BC6" s="9"/>
-    </row>
-    <row r="7" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD6" s="9"/>
+      <c r="BE6" s="9"/>
+      <c r="BF6" s="9"/>
+      <c r="BG6" s="9"/>
+    </row>
+    <row r="7" spans="1:59" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>463</v>
       </c>
@@ -10292,8 +10952,12 @@
         <v>460</v>
       </c>
       <c r="BC7" s="9"/>
-    </row>
-    <row r="8" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD7" s="9"/>
+      <c r="BE7" s="9"/>
+      <c r="BF7" s="9"/>
+      <c r="BG7" s="9"/>
+    </row>
+    <row r="8" spans="1:59" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>464</v>
       </c>
@@ -10453,8 +11117,12 @@
         <v>460</v>
       </c>
       <c r="BC8" s="9"/>
-    </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BD8" s="9"/>
+      <c r="BE8" s="9"/>
+      <c r="BF8" s="9"/>
+      <c r="BG8" s="9"/>
+    </row>
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>465</v>
       </c>
@@ -10612,8 +11280,12 @@
       </c>
       <c r="BB9" s="9"/>
       <c r="BC9" s="9"/>
-    </row>
-    <row r="10" spans="1:55" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BD9" s="9"/>
+      <c r="BE9" s="9"/>
+      <c r="BF9" s="9"/>
+      <c r="BG9" s="9"/>
+    </row>
+    <row r="10" spans="1:59" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>466</v>
       </c>
@@ -10771,8 +11443,12 @@
       </c>
       <c r="BB10" s="9"/>
       <c r="BC10" s="9"/>
-    </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BD10" s="9"/>
+      <c r="BE10" s="9"/>
+      <c r="BF10" s="9"/>
+      <c r="BG10" s="9"/>
+    </row>
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>471</v>
       </c>
@@ -10932,6 +11608,183 @@
         <v>460</v>
       </c>
       <c r="BC11" s="9"/>
+      <c r="BD11" s="9"/>
+      <c r="BE11" s="9"/>
+      <c r="BF11" s="9"/>
+      <c r="BG11" s="9"/>
+    </row>
+    <row r="12" spans="1:59" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>448</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="P12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>16</v>
+      </c>
+      <c r="R12" s="9">
+        <v>16</v>
+      </c>
+      <c r="S12" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="T12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="U12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="V12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="W12" s="9">
+        <v>1100440052</v>
+      </c>
+      <c r="X12" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y12" s="9">
+        <v>45665456</v>
+      </c>
+      <c r="Z12" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="AA12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB12" s="9">
+        <v>1113332</v>
+      </c>
+      <c r="AC12" s="9">
+        <v>23564589</v>
+      </c>
+      <c r="AD12" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="AE12" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AF12" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AG12" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="AH12" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="AI12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ12" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="AK12" s="9">
+        <v>411006</v>
+      </c>
+      <c r="AL12" s="9">
+        <v>124421</v>
+      </c>
+      <c r="AM12" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="AN12" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="AO12" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="AP12" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="AQ12" s="9"/>
+      <c r="AR12" s="9"/>
+      <c r="AS12" s="9" t="s">
+        <v>375</v>
+      </c>
+      <c r="AT12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AU12" s="9">
+        <v>5431267812</v>
+      </c>
+      <c r="AV12" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="AW12" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="AX12" s="9">
+        <v>999</v>
+      </c>
+      <c r="AY12" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="AZ12" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="BA12" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="BB12" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="BC12" s="9"/>
+      <c r="BD12" s="9" t="s">
+        <v>568</v>
+      </c>
+      <c r="BE12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BF12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="BG12" s="9">
+        <v>121212</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -10955,8 +11808,10 @@
     <hyperlink ref="AD10" r:id="rId18"/>
     <hyperlink ref="X11" r:id="rId19"/>
     <hyperlink ref="AD11" r:id="rId20"/>
+    <hyperlink ref="X12" r:id="rId21"/>
+    <hyperlink ref="AD12" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CHP Wallet to wallet fund transfer story file and test data
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12945" windowHeight="6750" firstSheet="12" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12945" windowHeight="6750" firstSheet="12" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,14 @@
     <sheet name="LoyaltyPlan" sheetId="17" r:id="rId15"/>
     <sheet name="Prepaid_Application_Upload" sheetId="16" r:id="rId16"/>
     <sheet name="AuditReport" sheetId="18" r:id="rId17"/>
+    <sheet name="CardHolder" sheetId="19" r:id="rId18"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2299" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2714" uniqueCount="703">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1788,6 +1789,357 @@
   </si>
   <si>
     <t>http://ech-10-168-131-92.mastercard.int:25003/integratedIssuing-customerPortal/mpts/app/Login</t>
+  </si>
+  <si>
+    <t>TranSactionType</t>
+  </si>
+  <si>
+    <t>TransactionAmount</t>
+  </si>
+  <si>
+    <t>TransactionCurrency</t>
+  </si>
+  <si>
+    <t>ConversionRate</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>TransferAmount</t>
+  </si>
+  <si>
+    <t>CurrencyName</t>
+  </si>
+  <si>
+    <t>ContactNumber</t>
+  </si>
+  <si>
+    <t>TransfererName</t>
+  </si>
+  <si>
+    <t>Memo</t>
+  </si>
+  <si>
+    <t>TransactionPassword</t>
+  </si>
+  <si>
+    <t>TransactionRemarks</t>
+  </si>
+  <si>
+    <t>AmountToTransferWalletToWallet</t>
+  </si>
+  <si>
+    <t>WalletTransferCurrecny</t>
+  </si>
+  <si>
+    <t>WalletNumberFromTransferMoney</t>
+  </si>
+  <si>
+    <t>WalletToAmountTransfer</t>
+  </si>
+  <si>
+    <t>WalletToWalletTransferSucessMsg</t>
+  </si>
+  <si>
+    <t>NoOfTransactionsCount</t>
+  </si>
+  <si>
+    <t>FromDate</t>
+  </si>
+  <si>
+    <t>ToDate</t>
+  </si>
+  <si>
+    <t>ReplacementResone</t>
+  </si>
+  <si>
+    <t>ReplaceConfirmMessage</t>
+  </si>
+  <si>
+    <t>BlockCardRemark</t>
+  </si>
+  <si>
+    <t>BlockConfirmationMsg</t>
+  </si>
+  <si>
+    <t>UnblockCardRemark</t>
+  </si>
+  <si>
+    <t>UnblockConfirmationMsg</t>
+  </si>
+  <si>
+    <t>WalletActivationRemark</t>
+  </si>
+  <si>
+    <t>WalletDeactivateRemark</t>
+  </si>
+  <si>
+    <t>WalletActivateConfirmMsg</t>
+  </si>
+  <si>
+    <t>WalletDeactivateConfirmMsg</t>
+  </si>
+  <si>
+    <t>eComActivationConfirmMsg</t>
+  </si>
+  <si>
+    <t>beneficiaryID</t>
+  </si>
+  <si>
+    <t>beneficiaryFirstName</t>
+  </si>
+  <si>
+    <t>beneficiaryMiddleName</t>
+  </si>
+  <si>
+    <t>beneficiaryLastName</t>
+  </si>
+  <si>
+    <t>beneficiaryAddressLine1</t>
+  </si>
+  <si>
+    <t>beneficiaryAddressLine2</t>
+  </si>
+  <si>
+    <t>beneficiaryAddressLine3</t>
+  </si>
+  <si>
+    <t>beneficiaryCountryName</t>
+  </si>
+  <si>
+    <t>beneficiaryStateName</t>
+  </si>
+  <si>
+    <t>beneficiaryCityName</t>
+  </si>
+  <si>
+    <t>beneficiaryZIPCode</t>
+  </si>
+  <si>
+    <t>beneficiaryEmailAddress</t>
+  </si>
+  <si>
+    <t>beneficiaryMobileNumber</t>
+  </si>
+  <si>
+    <t>beneficiaryRemittanceAamount</t>
+  </si>
+  <si>
+    <t>beneficiaryRemittanceCurrency</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>CardHolderTransPassword</t>
+  </si>
+  <si>
+    <t>FirstSequrityQuestion</t>
+  </si>
+  <si>
+    <t>FirstSequrityAnswer</t>
+  </si>
+  <si>
+    <t>SecondSequrityQuestion</t>
+  </si>
+  <si>
+    <t>SecondSequrityAnswer</t>
+  </si>
+  <si>
+    <t>TC_walletToWalletTransfer</t>
+  </si>
+  <si>
+    <t>http://ech-10-168-129-105.mastercard.int:25003/integratedIssuing-cardholderPortal/WebPages/Login.jsp</t>
+  </si>
+  <si>
+    <t>12121218044000192</t>
+  </si>
+  <si>
+    <t>Fund Transfer</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>0.016000</t>
+  </si>
+  <si>
+    <t>5887659200346112</t>
+  </si>
+  <si>
+    <t>aBcd1234*</t>
+  </si>
+  <si>
+    <t>Wallet to wallet fund transfer</t>
+  </si>
+  <si>
+    <t>1802131212120070068</t>
+  </si>
+  <si>
+    <t>1802131212120070067</t>
+  </si>
+  <si>
+    <t>Your transaction is successful</t>
+  </si>
+  <si>
+    <t>TC_LoginCardholderPortal</t>
+  </si>
+  <si>
+    <t>TC_ViewChargeForFundTransfer</t>
+  </si>
+  <si>
+    <t>12121218036000463</t>
+  </si>
+  <si>
+    <t>TC_masterCardMoneyTransfer</t>
+  </si>
+  <si>
+    <t>10000117311000005</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>CMKO-45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">454564Done </t>
+  </si>
+  <si>
+    <t>TC_checkInterbankTransfer</t>
+  </si>
+  <si>
+    <t>TC_viewTransactionHistoryForWallet</t>
+  </si>
+  <si>
+    <t>05/10/2017</t>
+  </si>
+  <si>
+    <t>31/10/2017</t>
+  </si>
+  <si>
+    <t>TC_deviceReplaceService</t>
+  </si>
+  <si>
+    <t>Emergency Replacement</t>
+  </si>
+  <si>
+    <t>Request is forwarded to institution</t>
+  </si>
+  <si>
+    <t>TC_deviceBlockFromCardHolder</t>
+  </si>
+  <si>
+    <t>Card need to block as it is stolne</t>
+  </si>
+  <si>
+    <t>Device Blocked Call Reference Number</t>
+  </si>
+  <si>
+    <t>Block my card</t>
+  </si>
+  <si>
+    <t>Unblock Device process successful</t>
+  </si>
+  <si>
+    <t>TC_deviceUnblockFromCardholder</t>
+  </si>
+  <si>
+    <t>TC_walletActivateFromCardHolder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activate Wallet </t>
+  </si>
+  <si>
+    <t>Request has been processed successfully with reference number</t>
+  </si>
+  <si>
+    <t>TC_walletDeActivateFromCardHolder</t>
+  </si>
+  <si>
+    <t>Deactivate Wallet</t>
+  </si>
+  <si>
+    <t>TC_activateEcomForLifeLong</t>
+  </si>
+  <si>
+    <t>DEVICE is already activated for life long use</t>
+  </si>
+  <si>
+    <t>TC_activationEcomForDuration</t>
+  </si>
+  <si>
+    <t>TC_activateEcomForNHours</t>
+  </si>
+  <si>
+    <t>TC_cashRemittanceBookting</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t>Mname</t>
+  </si>
+  <si>
+    <t>Lname</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address3</t>
+  </si>
+  <si>
+    <t>INDIA</t>
+  </si>
+  <si>
+    <t>MAHARASTHRA</t>
+  </si>
+  <si>
+    <t>mastercard@mastercard.com</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>TC_signUpCardholderPortal</t>
+  </si>
+  <si>
+    <t>TC_activationForInternationalUse</t>
+  </si>
+  <si>
+    <t>TC_activationNHoursForInternationalUse</t>
+  </si>
+  <si>
+    <t>TC_activationLifeLongForInternationalUse</t>
+  </si>
+  <si>
+    <t>TC_ViewChargeForWalletToWalletDebit</t>
+  </si>
+  <si>
+    <t>TC_ViewChargeForWalletClosure</t>
+  </si>
+  <si>
+    <t>TC_ViewChargeForVisaMoneyTransferDebit</t>
+  </si>
+  <si>
+    <t>TC_ViewChargeForIntraBnkWalletToWalletTransferDebit</t>
+  </si>
+  <si>
+    <t>TC_ViewChargeForMasterCardMoneySend</t>
+  </si>
+  <si>
+    <t>TC_RequestVirtualPrepaidCard</t>
+  </si>
+  <si>
+    <t>TC_createPinSetRquest</t>
+  </si>
+  <si>
+    <t>TC_visaMoneyTransfer</t>
   </si>
 </sst>
 </file>
@@ -1797,7 +2149,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\-yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1821,8 +2173,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1835,8 +2195,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1931,12 +2303,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2024,8 +2406,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -5431,8 +5832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5524,6 +5925,2644 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BD28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.5703125" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="64" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="31" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" style="31" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" style="31" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="17" max="17" width="30.85546875" customWidth="1"/>
+    <col min="18" max="18" width="22.28515625" customWidth="1"/>
+    <col min="19" max="20" width="30.42578125" customWidth="1"/>
+    <col min="21" max="21" width="31.85546875" customWidth="1"/>
+    <col min="22" max="22" width="23.140625" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" style="31" customWidth="1"/>
+    <col min="24" max="24" width="12.42578125" customWidth="1"/>
+    <col min="25" max="25" width="24.28515625" customWidth="1"/>
+    <col min="26" max="26" width="31.5703125" customWidth="1"/>
+    <col min="27" max="27" width="33.5703125" customWidth="1"/>
+    <col min="28" max="28" width="29.7109375" customWidth="1"/>
+    <col min="29" max="29" width="28" customWidth="1"/>
+    <col min="30" max="30" width="30.5703125" customWidth="1"/>
+    <col min="31" max="31" width="24.7109375" customWidth="1"/>
+    <col min="32" max="32" width="22.85546875" customWidth="1"/>
+    <col min="33" max="33" width="45.28515625" customWidth="1"/>
+    <col min="34" max="34" width="56.7109375" customWidth="1"/>
+    <col min="35" max="35" width="41.140625" customWidth="1"/>
+    <col min="36" max="36" width="16.5703125" customWidth="1"/>
+    <col min="37" max="37" width="19.7109375" customWidth="1"/>
+    <col min="38" max="38" width="22.85546875" customWidth="1"/>
+    <col min="39" max="39" width="18.42578125" customWidth="1"/>
+    <col min="40" max="41" width="22.28515625" customWidth="1"/>
+    <col min="42" max="43" width="22.5703125" customWidth="1"/>
+    <col min="44" max="44" width="24.42578125" customWidth="1"/>
+    <col min="45" max="45" width="20.140625" customWidth="1"/>
+    <col min="46" max="46" width="19.140625" customWidth="1"/>
+    <col min="47" max="47" width="23.7109375" customWidth="1"/>
+    <col min="48" max="48" width="23.5703125" customWidth="1"/>
+    <col min="49" max="49" width="29.7109375" customWidth="1"/>
+    <col min="50" max="50" width="28.85546875" customWidth="1"/>
+    <col min="51" max="56" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>306</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>308</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>586</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>587</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>588</v>
+      </c>
+      <c r="H1" s="49" t="s">
+        <v>589</v>
+      </c>
+      <c r="I1" s="49" t="s">
+        <v>590</v>
+      </c>
+      <c r="J1" s="49" t="s">
+        <v>591</v>
+      </c>
+      <c r="K1" s="49" t="s">
+        <v>592</v>
+      </c>
+      <c r="L1" s="49" t="s">
+        <v>593</v>
+      </c>
+      <c r="M1" s="49" t="s">
+        <v>594</v>
+      </c>
+      <c r="N1" s="49" t="s">
+        <v>595</v>
+      </c>
+      <c r="O1" s="49" t="s">
+        <v>596</v>
+      </c>
+      <c r="P1" s="49" t="s">
+        <v>597</v>
+      </c>
+      <c r="Q1" s="49" t="s">
+        <v>598</v>
+      </c>
+      <c r="R1" s="49" t="s">
+        <v>599</v>
+      </c>
+      <c r="S1" s="50" t="s">
+        <v>600</v>
+      </c>
+      <c r="T1" s="50" t="s">
+        <v>601</v>
+      </c>
+      <c r="U1" s="51" t="s">
+        <v>602</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="AA1" s="49" t="s">
+        <v>608</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="AK1" s="52" t="s">
+        <v>618</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="2" spans="1:56" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="53" t="s">
+        <v>638</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>639</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>640</v>
+      </c>
+      <c r="D2" s="55" t="s">
+        <v>640</v>
+      </c>
+      <c r="E2" s="53" t="s">
+        <v>641</v>
+      </c>
+      <c r="F2" s="53">
+        <v>10</v>
+      </c>
+      <c r="G2" s="53" t="s">
+        <v>642</v>
+      </c>
+      <c r="H2" s="56" t="s">
+        <v>643</v>
+      </c>
+      <c r="I2" s="57" t="s">
+        <v>644</v>
+      </c>
+      <c r="J2" s="56" t="s">
+        <v>559</v>
+      </c>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53">
+        <v>9021723007</v>
+      </c>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="58" t="s">
+        <v>645</v>
+      </c>
+      <c r="P2" s="53" t="s">
+        <v>646</v>
+      </c>
+      <c r="Q2" s="59">
+        <v>5</v>
+      </c>
+      <c r="R2" s="59" t="s">
+        <v>642</v>
+      </c>
+      <c r="S2" s="59" t="s">
+        <v>647</v>
+      </c>
+      <c r="T2" s="59" t="s">
+        <v>648</v>
+      </c>
+      <c r="U2" s="53" t="s">
+        <v>649</v>
+      </c>
+      <c r="V2" s="53"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="53"/>
+      <c r="Z2" s="53"/>
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="53"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="53"/>
+      <c r="AF2" s="53"/>
+      <c r="AG2" s="53"/>
+      <c r="AH2" s="53"/>
+      <c r="AI2" s="53"/>
+      <c r="AJ2" s="53"/>
+      <c r="AK2" s="53"/>
+      <c r="AL2" s="53"/>
+      <c r="AM2" s="53"/>
+      <c r="AN2" s="53"/>
+      <c r="AO2" s="53"/>
+      <c r="AP2" s="53"/>
+      <c r="AQ2" s="53"/>
+      <c r="AR2" s="53"/>
+      <c r="AS2" s="53"/>
+      <c r="AT2" s="53"/>
+      <c r="AU2" s="53"/>
+      <c r="AV2" s="53"/>
+      <c r="AW2" s="53"/>
+      <c r="AX2" s="53"/>
+      <c r="AY2" s="53"/>
+      <c r="AZ2" s="53"/>
+      <c r="BA2" s="53"/>
+      <c r="BB2" s="53"/>
+      <c r="BC2" s="53"/>
+      <c r="BD2" s="53"/>
+    </row>
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C3" s="55" t="s">
+        <v>640</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>640</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+      <c r="BD3" s="2"/>
+    </row>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="B4" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C4" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="2"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2"/>
+      <c r="AZ4" s="2"/>
+      <c r="BA4" s="2"/>
+      <c r="BB4" s="2"/>
+      <c r="BC4" s="2"/>
+      <c r="BD4" s="2"/>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="L5" s="2">
+        <v>955689456</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="O5" s="61" t="s">
+        <v>645</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="2"/>
+      <c r="AS5" s="2"/>
+      <c r="AT5" s="2"/>
+      <c r="AU5" s="2"/>
+      <c r="AV5" s="2"/>
+      <c r="AW5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="2"/>
+      <c r="AZ5" s="2"/>
+      <c r="BA5" s="2"/>
+      <c r="BB5" s="2"/>
+      <c r="BC5" s="2"/>
+      <c r="BD5" s="2"/>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="B6" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D6" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2"/>
+      <c r="AV6" s="2"/>
+      <c r="AW6" s="2"/>
+      <c r="AX6" s="2"/>
+      <c r="AY6" s="2"/>
+      <c r="AZ6" s="2"/>
+      <c r="BA6" s="2"/>
+      <c r="BB6" s="2"/>
+      <c r="BC6" s="2"/>
+      <c r="BD6" s="2"/>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2">
+        <v>10</v>
+      </c>
+      <c r="W7" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AS7" s="2"/>
+      <c r="AT7" s="2"/>
+      <c r="AU7" s="2"/>
+      <c r="AV7" s="2"/>
+      <c r="AW7" s="2"/>
+      <c r="AX7" s="2"/>
+      <c r="AY7" s="2"/>
+      <c r="AZ7" s="2"/>
+      <c r="BA7" s="2"/>
+      <c r="BB7" s="2"/>
+      <c r="BC7" s="2"/>
+      <c r="BD7" s="2"/>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="B8" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2">
+        <v>10</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="Z8" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AS8" s="2"/>
+      <c r="AT8" s="2"/>
+      <c r="AU8" s="2"/>
+      <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
+      <c r="AY8" s="2"/>
+      <c r="AZ8" s="2"/>
+      <c r="BA8" s="2"/>
+      <c r="BB8" s="2"/>
+      <c r="BC8" s="2"/>
+      <c r="BD8" s="2"/>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="B9" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D9" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2">
+        <v>10</v>
+      </c>
+      <c r="W9" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="Z9" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="AA9" s="62" t="s">
+        <v>666</v>
+      </c>
+      <c r="AB9" s="62" t="s">
+        <v>667</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="AD9" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="2"/>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="2"/>
+      <c r="AW9" s="2"/>
+      <c r="AX9" s="2"/>
+      <c r="AY9" s="2"/>
+      <c r="AZ9" s="2"/>
+      <c r="BA9" s="2"/>
+      <c r="BB9" s="2"/>
+      <c r="BC9" s="2"/>
+      <c r="BD9" s="2"/>
+    </row>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D10" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2">
+        <v>10</v>
+      </c>
+      <c r="W10" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="Z10" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="AA10" s="62" t="s">
+        <v>666</v>
+      </c>
+      <c r="AB10" s="62" t="s">
+        <v>667</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2"/>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="2"/>
+      <c r="AS10" s="2"/>
+      <c r="AT10" s="2"/>
+      <c r="AU10" s="2"/>
+      <c r="AV10" s="2"/>
+      <c r="AW10" s="2"/>
+      <c r="AX10" s="2"/>
+      <c r="AY10" s="2"/>
+      <c r="AZ10" s="2"/>
+      <c r="BA10" s="2"/>
+      <c r="BB10" s="2"/>
+      <c r="BC10" s="2"/>
+      <c r="BD10" s="2"/>
+    </row>
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C11" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2">
+        <v>10</v>
+      </c>
+      <c r="W11" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="Z11" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="AA11" s="62" t="s">
+        <v>666</v>
+      </c>
+      <c r="AB11" s="62" t="s">
+        <v>667</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="AD11" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AH11" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="2"/>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="2"/>
+      <c r="AS11" s="2"/>
+      <c r="AT11" s="2"/>
+      <c r="AU11" s="2"/>
+      <c r="AV11" s="2"/>
+      <c r="AW11" s="2"/>
+      <c r="AX11" s="2"/>
+      <c r="AY11" s="2"/>
+      <c r="AZ11" s="2"/>
+      <c r="BA11" s="2"/>
+      <c r="BB11" s="2"/>
+      <c r="BC11" s="2"/>
+      <c r="BD11" s="2"/>
+    </row>
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D12" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2">
+        <v>10</v>
+      </c>
+      <c r="W12" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="Z12" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="AA12" s="62" t="s">
+        <v>666</v>
+      </c>
+      <c r="AB12" s="62" t="s">
+        <v>667</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="AD12" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="AG12" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AH12" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="2"/>
+      <c r="AU12" s="2"/>
+      <c r="AV12" s="2"/>
+      <c r="AW12" s="2"/>
+      <c r="AX12" s="2"/>
+      <c r="AY12" s="2"/>
+      <c r="AZ12" s="2"/>
+      <c r="BA12" s="2"/>
+      <c r="BB12" s="2"/>
+      <c r="BC12" s="2"/>
+      <c r="BD12" s="2"/>
+    </row>
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C13" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D13" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2">
+        <v>10</v>
+      </c>
+      <c r="W13" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="Z13" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="AA13" s="62" t="s">
+        <v>666</v>
+      </c>
+      <c r="AB13" s="62" t="s">
+        <v>667</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="AD13" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AH13" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AI13" s="62" t="s">
+        <v>677</v>
+      </c>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="2"/>
+      <c r="AN13" s="2"/>
+      <c r="AO13" s="2"/>
+      <c r="AP13" s="2"/>
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="2"/>
+      <c r="AS13" s="2"/>
+      <c r="AT13" s="2"/>
+      <c r="AU13" s="2"/>
+      <c r="AV13" s="2"/>
+      <c r="AW13" s="2"/>
+      <c r="AX13" s="2"/>
+      <c r="AY13" s="2"/>
+      <c r="AZ13" s="2"/>
+      <c r="BA13" s="2"/>
+      <c r="BB13" s="2"/>
+      <c r="BC13" s="2"/>
+      <c r="BD13" s="2"/>
+    </row>
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2">
+        <v>10</v>
+      </c>
+      <c r="W14" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="Y14" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="Z14" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="AA14" s="62" t="s">
+        <v>666</v>
+      </c>
+      <c r="AB14" s="62" t="s">
+        <v>667</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="AD14" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AH14" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AI14" s="62" t="s">
+        <v>677</v>
+      </c>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2"/>
+      <c r="AT14" s="2"/>
+      <c r="AU14" s="2"/>
+      <c r="AV14" s="2"/>
+      <c r="AW14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="AY14" s="2"/>
+      <c r="AZ14" s="2"/>
+      <c r="BA14" s="2"/>
+      <c r="BB14" s="2"/>
+      <c r="BC14" s="2"/>
+      <c r="BD14" s="2"/>
+    </row>
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="B15" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2">
+        <v>10</v>
+      </c>
+      <c r="W15" s="9" t="s">
+        <v>660</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="Y15" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="Z15" s="62" t="s">
+        <v>664</v>
+      </c>
+      <c r="AA15" s="62" t="s">
+        <v>666</v>
+      </c>
+      <c r="AB15" s="62" t="s">
+        <v>667</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="AD15" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AH15" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AI15" s="62" t="s">
+        <v>677</v>
+      </c>
+      <c r="AJ15" s="2"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
+      <c r="AN15" s="2"/>
+      <c r="AO15" s="2"/>
+      <c r="AP15" s="2"/>
+      <c r="AQ15" s="2"/>
+      <c r="AR15" s="2"/>
+      <c r="AS15" s="2"/>
+      <c r="AT15" s="2"/>
+      <c r="AU15" s="2"/>
+      <c r="AV15" s="2"/>
+      <c r="AW15" s="2"/>
+      <c r="AX15" s="2"/>
+      <c r="AY15" s="2"/>
+      <c r="AZ15" s="2"/>
+      <c r="BA15" s="2"/>
+      <c r="BB15" s="2"/>
+      <c r="BC15" s="2"/>
+      <c r="BD15" s="2"/>
+    </row>
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D16" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="AK16" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="AL16" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="AM16" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="AN16" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="AO16" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="AP16" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="AQ16" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="AR16" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="AS16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT16" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AU16" s="46" t="s">
+        <v>689</v>
+      </c>
+      <c r="AV16" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AW16" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AX16" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="AY16" s="2"/>
+      <c r="AZ16" s="2"/>
+      <c r="BA16" s="2"/>
+      <c r="BB16" s="2"/>
+      <c r="BC16" s="2"/>
+      <c r="BD16" s="2"/>
+    </row>
+    <row r="17" spans="1:56" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="53" t="s">
+        <v>691</v>
+      </c>
+      <c r="B17" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C17" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D17" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E17" s="53" t="s">
+        <v>641</v>
+      </c>
+      <c r="F17" s="53">
+        <v>5</v>
+      </c>
+      <c r="G17" s="53" t="s">
+        <v>642</v>
+      </c>
+      <c r="H17" s="56" t="s">
+        <v>643</v>
+      </c>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="53"/>
+      <c r="S17" s="53"/>
+      <c r="T17" s="53"/>
+      <c r="U17" s="53"/>
+      <c r="V17" s="53"/>
+      <c r="W17" s="56"/>
+      <c r="X17" s="53"/>
+      <c r="Y17" s="53"/>
+      <c r="Z17" s="53"/>
+      <c r="AA17" s="53"/>
+      <c r="AB17" s="53"/>
+      <c r="AC17" s="53"/>
+      <c r="AD17" s="53"/>
+      <c r="AE17" s="53"/>
+      <c r="AF17" s="53"/>
+      <c r="AG17" s="53"/>
+      <c r="AH17" s="53"/>
+      <c r="AI17" s="53"/>
+      <c r="AJ17" s="53" t="s">
+        <v>681</v>
+      </c>
+      <c r="AK17" s="53" t="s">
+        <v>682</v>
+      </c>
+      <c r="AL17" s="53" t="s">
+        <v>683</v>
+      </c>
+      <c r="AM17" s="53" t="s">
+        <v>684</v>
+      </c>
+      <c r="AN17" s="53" t="s">
+        <v>685</v>
+      </c>
+      <c r="AO17" s="53" t="s">
+        <v>685</v>
+      </c>
+      <c r="AP17" s="53" t="s">
+        <v>686</v>
+      </c>
+      <c r="AQ17" s="53" t="s">
+        <v>687</v>
+      </c>
+      <c r="AR17" s="53" t="s">
+        <v>688</v>
+      </c>
+      <c r="AS17" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT17" s="53">
+        <v>411033</v>
+      </c>
+      <c r="AU17" s="63" t="s">
+        <v>689</v>
+      </c>
+      <c r="AV17" s="53">
+        <v>7896543215</v>
+      </c>
+      <c r="AW17" s="53">
+        <v>5000</v>
+      </c>
+      <c r="AX17" s="53" t="s">
+        <v>690</v>
+      </c>
+      <c r="AY17" s="53" t="s">
+        <v>645</v>
+      </c>
+      <c r="AZ17" s="53" t="s">
+        <v>645</v>
+      </c>
+      <c r="BA17" s="53"/>
+      <c r="BB17" s="53"/>
+      <c r="BC17" s="53"/>
+      <c r="BD17" s="53"/>
+    </row>
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="B18" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D18" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F18" s="2">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="AK18" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="AL18" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="AM18" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="AN18" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="AO18" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="AP18" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="AQ18" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="AR18" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="AS18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT18" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AU18" s="46" t="s">
+        <v>689</v>
+      </c>
+      <c r="AV18" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AW18" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AX18" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="AY18" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="AZ18" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="BA18" s="2"/>
+      <c r="BB18" s="2"/>
+      <c r="BC18" s="2"/>
+      <c r="BD18" s="2"/>
+    </row>
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="B19" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C19" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D19" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2"/>
+      <c r="AJ19" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="AK19" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="AL19" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="AM19" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="AN19" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="AO19" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="AP19" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="AQ19" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="AR19" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="AS19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT19" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AU19" s="46" t="s">
+        <v>689</v>
+      </c>
+      <c r="AV19" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AW19" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AX19" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="AY19" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="AZ19" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="BA19" s="2"/>
+      <c r="BB19" s="2"/>
+      <c r="BC19" s="2"/>
+      <c r="BD19" s="2"/>
+    </row>
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="B20" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C20" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D20" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2"/>
+      <c r="AJ20" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="AK20" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="AL20" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="AM20" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="AN20" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="AO20" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="AP20" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="AQ20" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="AR20" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="AS20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT20" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AU20" s="46" t="s">
+        <v>689</v>
+      </c>
+      <c r="AV20" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AW20" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AX20" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="AY20" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="AZ20" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="BA20" s="2"/>
+      <c r="BB20" s="2"/>
+      <c r="BC20" s="2"/>
+      <c r="BD20" s="2"/>
+    </row>
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="B21" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2"/>
+      <c r="AH21" s="2"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="2"/>
+      <c r="AK21" s="2"/>
+      <c r="AL21" s="2"/>
+      <c r="AM21" s="2"/>
+      <c r="AN21" s="2"/>
+      <c r="AO21" s="2"/>
+      <c r="AP21" s="2"/>
+      <c r="AQ21" s="2"/>
+      <c r="AR21" s="2"/>
+      <c r="AS21" s="2"/>
+      <c r="AT21" s="2"/>
+      <c r="AU21" s="2"/>
+      <c r="AV21" s="2"/>
+      <c r="AW21" s="2"/>
+      <c r="AX21" s="2"/>
+      <c r="AY21" s="2"/>
+      <c r="AZ21" s="2"/>
+      <c r="BA21" s="2"/>
+      <c r="BB21" s="2"/>
+      <c r="BC21" s="2"/>
+      <c r="BD21" s="2"/>
+    </row>
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>696</v>
+      </c>
+      <c r="B22" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C22" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D22" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="2"/>
+      <c r="AK22" s="2"/>
+      <c r="AL22" s="2"/>
+      <c r="AM22" s="2"/>
+      <c r="AN22" s="2"/>
+      <c r="AO22" s="2"/>
+      <c r="AP22" s="2"/>
+      <c r="AQ22" s="2"/>
+      <c r="AR22" s="2"/>
+      <c r="AS22" s="2"/>
+      <c r="AT22" s="2"/>
+      <c r="AU22" s="2"/>
+      <c r="AV22" s="2"/>
+      <c r="AW22" s="2"/>
+      <c r="AX22" s="2"/>
+      <c r="AY22" s="2"/>
+      <c r="AZ22" s="2"/>
+      <c r="BA22" s="2"/>
+      <c r="BB22" s="2"/>
+      <c r="BC22" s="2"/>
+      <c r="BD22" s="2"/>
+    </row>
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="B23" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C23" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D23" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F23" s="2">
+        <v>5</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="2"/>
+      <c r="AK23" s="2"/>
+      <c r="AL23" s="2"/>
+      <c r="AM23" s="2"/>
+      <c r="AN23" s="2"/>
+      <c r="AO23" s="2"/>
+      <c r="AP23" s="2"/>
+      <c r="AQ23" s="2"/>
+      <c r="AR23" s="2"/>
+      <c r="AS23" s="2"/>
+      <c r="AT23" s="2"/>
+      <c r="AU23" s="2"/>
+      <c r="AV23" s="2"/>
+      <c r="AW23" s="2"/>
+      <c r="AX23" s="2"/>
+      <c r="AY23" s="2"/>
+      <c r="AZ23" s="2"/>
+      <c r="BA23" s="2"/>
+      <c r="BB23" s="2"/>
+      <c r="BC23" s="2"/>
+      <c r="BD23" s="2"/>
+    </row>
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="B24" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C24" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D24" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F24" s="2">
+        <v>5</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="2"/>
+      <c r="AI24" s="2"/>
+      <c r="AJ24" s="2"/>
+      <c r="AK24" s="2"/>
+      <c r="AL24" s="2"/>
+      <c r="AM24" s="2"/>
+      <c r="AN24" s="2"/>
+      <c r="AO24" s="2"/>
+      <c r="AP24" s="2"/>
+      <c r="AQ24" s="2"/>
+      <c r="AR24" s="2"/>
+      <c r="AS24" s="2"/>
+      <c r="AT24" s="2"/>
+      <c r="AU24" s="2"/>
+      <c r="AV24" s="2"/>
+      <c r="AW24" s="2"/>
+      <c r="AX24" s="2"/>
+      <c r="AY24" s="2"/>
+      <c r="AZ24" s="2"/>
+      <c r="BA24" s="2"/>
+      <c r="BB24" s="2"/>
+      <c r="BC24" s="2"/>
+      <c r="BD24" s="2"/>
+    </row>
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="B25" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C25" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D25" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F25" s="2">
+        <v>5</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="2"/>
+      <c r="AI25" s="2"/>
+      <c r="AJ25" s="2"/>
+      <c r="AK25" s="2"/>
+      <c r="AL25" s="2"/>
+      <c r="AM25" s="2"/>
+      <c r="AN25" s="2"/>
+      <c r="AO25" s="2"/>
+      <c r="AP25" s="2"/>
+      <c r="AQ25" s="2"/>
+      <c r="AR25" s="2"/>
+      <c r="AS25" s="2"/>
+      <c r="AT25" s="2"/>
+      <c r="AU25" s="2"/>
+      <c r="AV25" s="2"/>
+      <c r="AW25" s="2"/>
+      <c r="AX25" s="2"/>
+      <c r="AY25" s="2"/>
+      <c r="AZ25" s="2"/>
+      <c r="BA25" s="2"/>
+      <c r="BB25" s="2"/>
+      <c r="BC25" s="2"/>
+      <c r="BD25" s="2"/>
+    </row>
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="B26" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C26" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D26" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F26" s="2">
+        <v>5</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="2"/>
+      <c r="Y26" s="2"/>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="2"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="2"/>
+      <c r="AE26" s="2"/>
+      <c r="AF26" s="2"/>
+      <c r="AG26" s="2"/>
+      <c r="AH26" s="2"/>
+      <c r="AI26" s="2"/>
+      <c r="AJ26" s="2"/>
+      <c r="AK26" s="2"/>
+      <c r="AL26" s="2"/>
+      <c r="AM26" s="2"/>
+      <c r="AN26" s="2"/>
+      <c r="AO26" s="2"/>
+      <c r="AP26" s="2"/>
+      <c r="AQ26" s="2"/>
+      <c r="AR26" s="2"/>
+      <c r="AS26" s="2"/>
+      <c r="AT26" s="2"/>
+      <c r="AU26" s="2"/>
+      <c r="AV26" s="2"/>
+      <c r="AW26" s="2"/>
+      <c r="AX26" s="2"/>
+      <c r="AY26" s="2"/>
+      <c r="AZ26" s="2"/>
+      <c r="BA26" s="2"/>
+      <c r="BB26" s="2"/>
+      <c r="BC26" s="2"/>
+      <c r="BD26" s="2"/>
+    </row>
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="B27" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C27" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D27" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F27" s="2">
+        <v>5</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+      <c r="AF27" s="2"/>
+      <c r="AG27" s="2"/>
+      <c r="AH27" s="2"/>
+      <c r="AI27" s="2"/>
+      <c r="AJ27" s="2"/>
+      <c r="AK27" s="2"/>
+      <c r="AL27" s="2"/>
+      <c r="AM27" s="2"/>
+      <c r="AN27" s="2"/>
+      <c r="AO27" s="2"/>
+      <c r="AP27" s="2"/>
+      <c r="AQ27" s="2"/>
+      <c r="AR27" s="2"/>
+      <c r="AS27" s="2"/>
+      <c r="AT27" s="2"/>
+      <c r="AU27" s="2"/>
+      <c r="AV27" s="2"/>
+      <c r="AW27" s="2"/>
+      <c r="AX27" s="2"/>
+      <c r="AY27" s="2"/>
+      <c r="AZ27" s="2"/>
+      <c r="BA27" s="2"/>
+      <c r="BB27" s="2"/>
+      <c r="BC27" s="2"/>
+      <c r="BD27" s="2"/>
+    </row>
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>702</v>
+      </c>
+      <c r="B28" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="C28" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="D28" s="55" t="s">
+        <v>652</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F28" s="2">
+        <v>5</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="H28" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="L28" s="2">
+        <v>955689456</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="O28" s="61" t="s">
+        <v>645</v>
+      </c>
+      <c r="P28" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="2"/>
+      <c r="Y28" s="2"/>
+      <c r="Z28" s="2"/>
+      <c r="AA28" s="2"/>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="2"/>
+      <c r="AE28" s="2"/>
+      <c r="AF28" s="2"/>
+      <c r="AG28" s="2"/>
+      <c r="AH28" s="2"/>
+      <c r="AI28" s="2"/>
+      <c r="AJ28" s="2"/>
+      <c r="AK28" s="2"/>
+      <c r="AL28" s="2"/>
+      <c r="AM28" s="2"/>
+      <c r="AN28" s="2"/>
+      <c r="AO28" s="2"/>
+      <c r="AP28" s="2"/>
+      <c r="AQ28" s="2"/>
+      <c r="AR28" s="2"/>
+      <c r="AS28" s="2"/>
+      <c r="AT28" s="2"/>
+      <c r="AU28" s="2"/>
+      <c r="AV28" s="2"/>
+      <c r="AW28" s="2"/>
+      <c r="AX28" s="2"/>
+      <c r="AY28" s="2"/>
+      <c r="AZ28" s="2"/>
+      <c r="BA28" s="2"/>
+      <c r="BB28" s="2"/>
+      <c r="BC28" s="2"/>
+      <c r="BD28" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AU16" r:id="rId1"/>
+    <hyperlink ref="AU17" r:id="rId2"/>
+    <hyperlink ref="AU18" r:id="rId3"/>
+    <hyperlink ref="AU19" r:id="rId4"/>
+    <hyperlink ref="AU20" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="B3:B28" r:id="rId7" display="http://ech-10-168-129-105.mastercard.int:25003/integratedIssuing-cardholderPortal/WebPages/Login.jsp"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
wibmo report changes added
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -8981,8 +8981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DN177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3:AF11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
test data changed for debit bin
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3036" uniqueCount="754">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3167" uniqueCount="755">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -2293,6 +2293,9 @@
   </si>
   <si>
     <t>TC264318_Embossing File Generation_VISA</t>
+  </si>
+  <si>
+    <t>adaptiveAuth_debit</t>
   </si>
 </sst>
 </file>
@@ -9157,10 +9160,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EP177"/>
+  <dimension ref="A1:EP178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:CW8"/>
+    <sheetView tabSelected="1" topLeftCell="BN7" workbookViewId="0">
+      <selection activeCell="CH9" sqref="CH9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11999,25 +12002,25 @@
     </row>
     <row r="9" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>737</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>704</v>
+        <v>754</v>
+      </c>
+      <c r="B9" s="66" t="s">
+        <v>746</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>703</v>
+        <v>489</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>367</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>702</v>
+        <v>475</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>368</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>266</v>
+        <v>129</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>128</v>
@@ -12088,10 +12091,10 @@
         <v>36</v>
       </c>
       <c r="AF9" s="28" t="s">
-        <v>371</v>
+        <v>738</v>
       </c>
       <c r="AG9" s="28" t="s">
-        <v>9</v>
+        <v>739</v>
       </c>
       <c r="AH9" s="28" t="s">
         <v>10</v>
@@ -12127,13 +12130,13 @@
         <v>325</v>
       </c>
       <c r="AS9" s="28" t="s">
-        <v>146</v>
+        <v>740</v>
       </c>
       <c r="AT9" s="28" t="s">
-        <v>79</v>
+        <v>741</v>
       </c>
       <c r="AU9" s="28" t="s">
-        <v>147</v>
+        <v>742</v>
       </c>
       <c r="AV9" s="28" t="s">
         <v>29</v>
@@ -12143,7 +12146,7 @@
         <v>175</v>
       </c>
       <c r="AY9" s="28" t="s">
-        <v>736</v>
+        <v>30</v>
       </c>
       <c r="AZ9" s="28" t="s">
         <v>30</v>
@@ -12192,88 +12195,90 @@
         <v>71</v>
       </c>
       <c r="BP9" s="9" t="s">
+        <v>747</v>
+      </c>
+      <c r="BQ9" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="BQ9" s="28" t="s">
-        <v>375</v>
-      </c>
-      <c r="BR9" s="28"/>
-      <c r="BS9" s="9"/>
-      <c r="BT9" s="9"/>
-      <c r="BU9" s="9" t="s">
+      <c r="BR9" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="BS9" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="BT9" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="BU9" s="9"/>
+      <c r="BV9" s="9"/>
+      <c r="BW9" s="9"/>
+      <c r="BX9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BV9" s="9"/>
-      <c r="BW9" s="9" t="s">
+      <c r="BY9" s="9"/>
+      <c r="BZ9" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="BX9" s="9" t="s">
+      <c r="CA9" s="28" t="s">
         <v>171</v>
       </c>
-      <c r="BY9" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="BZ9" s="9" t="s">
+      <c r="CB9" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="CC9" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="CA9" s="28" t="s">
+      <c r="CD9" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="CB9" s="9" t="s">
+      <c r="CE9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="CC9" s="9" t="s">
+      <c r="CF9" s="28" t="s">
         <v>376</v>
       </c>
-      <c r="CD9" s="9"/>
-      <c r="CE9" s="9"/>
-      <c r="CF9" s="28"/>
-      <c r="CG9" s="9" t="s">
+      <c r="CG9" s="9"/>
+      <c r="CH9" s="28">
+        <v>587765</v>
+      </c>
+      <c r="CI9" s="28"/>
+      <c r="CJ9" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="CH9" s="28" t="s">
+      <c r="CK9" s="28" t="s">
         <v>377</v>
       </c>
-      <c r="CI9" s="28" t="s">
+      <c r="CL9" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="CJ9" s="28" t="s">
+      <c r="CM9" s="28" t="s">
         <v>378</v>
       </c>
-      <c r="CK9" s="28" t="s">
+      <c r="CN9" s="28" t="s">
         <v>379</v>
       </c>
-      <c r="CL9" s="28" t="s">
+      <c r="CO9" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="CM9" s="28"/>
-      <c r="CN9" s="28"/>
-      <c r="CO9" s="9" t="s">
+      <c r="CP9" s="28"/>
+      <c r="CQ9" s="9"/>
+      <c r="CR9" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="CP9" s="28" t="s">
+      <c r="CS9" s="28" t="s">
         <v>377</v>
       </c>
-      <c r="CQ9" s="9" t="s">
+      <c r="CT9" s="28" t="s">
         <v>380</v>
       </c>
-      <c r="CR9" s="9" t="s">
+      <c r="CU9" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="CS9" s="28" t="s">
+      <c r="CV9" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="CT9" s="28" t="s">
+      <c r="CW9" s="9" t="s">
         <v>176</v>
-      </c>
-      <c r="CU9" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="CV9" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="CW9" s="9">
-        <v>100</v>
       </c>
       <c r="CX9" s="9" t="s">
         <v>395</v>
@@ -12411,13 +12416,418 @@
         <v>671</v>
       </c>
     </row>
-    <row r="10" spans="1:146" x14ac:dyDescent="0.3">
-      <c r="CU10"/>
-      <c r="CV10" t="s">
+    <row r="10" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>737</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>704</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>703</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>702</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="L10" s="9"/>
+      <c r="M10" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28" t="s">
+        <v>322</v>
+      </c>
+      <c r="P10" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q10" s="28" t="s">
+        <v>323</v>
+      </c>
+      <c r="R10" s="28" t="s">
+        <v>324</v>
+      </c>
+      <c r="S10" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="T10" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="U10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="V10" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="W10" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="X10" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="Y10" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z10" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB10" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC10" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD10" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF10" s="28" t="s">
+        <v>371</v>
+      </c>
+      <c r="AG10" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="AH10" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI10" s="28" t="s">
+        <v>372</v>
+      </c>
+      <c r="AJ10" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK10" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL10" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="AM10" s="28" t="s">
+        <v>372</v>
+      </c>
+      <c r="AN10" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="AO10" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="AP10" s="28" t="s">
+        <v>373</v>
+      </c>
+      <c r="AQ10" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="AR10" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="AS10" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="AT10" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU10" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV10" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="AW10" s="29"/>
+      <c r="AX10" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="AY10" s="28" t="s">
+        <v>736</v>
+      </c>
+      <c r="AZ10" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="BA10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB10" s="28" t="s">
+        <v>374</v>
+      </c>
+      <c r="BC10" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="BD10" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="BE10" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="BF10" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="BG10" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="BH10" s="28"/>
+      <c r="BI10" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="BJ10" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="BK10" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="BL10" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="BM10" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="BN10" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="BO10" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="BP10" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="BQ10" s="28" t="s">
+        <v>375</v>
+      </c>
+      <c r="BR10" s="28"/>
+      <c r="BS10" s="9"/>
+      <c r="BT10" s="9"/>
+      <c r="BU10" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BV10" s="9"/>
+      <c r="BW10" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="BX10" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="BY10" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="BZ10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="CA10" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="CB10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="CC10" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="CD10" s="9"/>
+      <c r="CE10" s="9"/>
+      <c r="CF10" s="28"/>
+      <c r="CG10" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="CH10" s="28" t="s">
+        <v>377</v>
+      </c>
+      <c r="CI10" s="28" t="s">
+        <v>373</v>
+      </c>
+      <c r="CJ10" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="CK10" s="28" t="s">
+        <v>379</v>
+      </c>
+      <c r="CL10" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="CM10" s="28"/>
+      <c r="CN10" s="28"/>
+      <c r="CO10" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="CP10" s="28" t="s">
+        <v>377</v>
+      </c>
+      <c r="CQ10" s="9" t="s">
+        <v>380</v>
+      </c>
+      <c r="CR10" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="CS10" s="28" t="s">
+        <v>381</v>
+      </c>
+      <c r="CT10" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="CU10" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="CW10">
+      <c r="CV10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="CW10" s="9">
         <v>100</v>
+      </c>
+      <c r="CX10" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="CY10" s="9">
+        <v>5</v>
+      </c>
+      <c r="CZ10" s="9">
+        <v>12</v>
+      </c>
+      <c r="DA10" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="DB10" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="DC10" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="DD10" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="DE10" s="9" t="s">
+        <v>701</v>
+      </c>
+      <c r="DF10" s="9" t="s">
+        <v>700</v>
+      </c>
+      <c r="DG10" s="9" t="s">
+        <v>699</v>
+      </c>
+      <c r="DH10" s="35" t="s">
+        <v>698</v>
+      </c>
+      <c r="DI10" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="DJ10" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="DK10" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="DL10" s="9" t="s">
+        <v>696</v>
+      </c>
+      <c r="DM10" s="66" t="s">
+        <v>695</v>
+      </c>
+      <c r="DN10" s="66" t="s">
+        <v>488</v>
+      </c>
+      <c r="DO10" s="66" t="s">
+        <v>694</v>
+      </c>
+      <c r="DP10" s="65" t="s">
+        <v>693</v>
+      </c>
+      <c r="DQ10" s="65" t="s">
+        <v>692</v>
+      </c>
+      <c r="DR10" s="65" t="s">
+        <v>691</v>
+      </c>
+      <c r="DS10" s="65" t="s">
+        <v>690</v>
+      </c>
+      <c r="DT10" s="65" t="s">
+        <v>689</v>
+      </c>
+      <c r="DU10" s="65" t="s">
+        <v>688</v>
+      </c>
+      <c r="DV10" s="65" t="s">
+        <v>687</v>
+      </c>
+      <c r="DW10" s="65" t="s">
+        <v>686</v>
+      </c>
+      <c r="DX10" s="65" t="s">
+        <v>685</v>
+      </c>
+      <c r="DY10" s="65" t="s">
+        <v>684</v>
+      </c>
+      <c r="DZ10" s="65" t="s">
+        <v>683</v>
+      </c>
+      <c r="EA10" s="65" t="s">
+        <v>372</v>
+      </c>
+      <c r="EB10" s="65" t="s">
+        <v>372</v>
+      </c>
+      <c r="EC10" s="65" t="s">
+        <v>372</v>
+      </c>
+      <c r="ED10" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="EE10" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="EF10" s="37" t="s">
+        <v>680</v>
+      </c>
+      <c r="EG10" s="37" t="s">
+        <v>679</v>
+      </c>
+      <c r="EH10" s="37" t="s">
+        <v>678</v>
+      </c>
+      <c r="EI10" s="37" t="s">
+        <v>677</v>
+      </c>
+      <c r="EJ10" s="37" t="s">
+        <v>676</v>
+      </c>
+      <c r="EK10" s="37" t="s">
+        <v>675</v>
+      </c>
+      <c r="EL10" s="37" t="s">
+        <v>674</v>
+      </c>
+      <c r="EM10" s="37" t="s">
+        <v>673</v>
+      </c>
+      <c r="EN10" s="61" t="s">
+        <v>672</v>
+      </c>
+      <c r="EO10" s="61" t="s">
+        <v>500</v>
+      </c>
+      <c r="EP10" s="61" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="11" spans="1:146" x14ac:dyDescent="0.3">
@@ -12431,6 +12841,12 @@
     </row>
     <row r="12" spans="1:146" x14ac:dyDescent="0.3">
       <c r="CU12"/>
+      <c r="CV12" t="s">
+        <v>156</v>
+      </c>
+      <c r="CW12">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" spans="1:146" x14ac:dyDescent="0.3">
       <c r="CU13"/>
@@ -12926,6 +13342,9 @@
     </row>
     <row r="177" spans="99:99" x14ac:dyDescent="0.3">
       <c r="CU177"/>
+    </row>
+    <row r="178" spans="99:99" x14ac:dyDescent="0.3">
+      <c r="CU178"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Instituiion setup for debit
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12945" windowHeight="6750" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12945" windowHeight="6750" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3033" uniqueCount="779">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3035" uniqueCount="786">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1449,12 +1449,6 @@
     <t>PRECRE</t>
   </si>
   <si>
-    <t>DEBCRE</t>
-  </si>
-  <si>
-    <t>ALLISS</t>
-  </si>
-  <si>
     <t>PREWOAGNT</t>
   </si>
   <si>
@@ -2262,9 +2256,6 @@
     <t>Sequence number</t>
   </si>
   <si>
-    <t>BlackEyeCreDE [034062]</t>
-  </si>
-  <si>
     <t>Swap</t>
   </si>
   <si>
@@ -2368,6 +2359,36 @@
   </si>
   <si>
     <t>AmexInstituionSetup</t>
+  </si>
+  <si>
+    <t>OMR [512]</t>
+  </si>
+  <si>
+    <t>91111111111</t>
+  </si>
+  <si>
+    <t>5431267812</t>
+  </si>
+  <si>
+    <t>July/2/2020</t>
+  </si>
+  <si>
+    <t>BLACKEYE</t>
+  </si>
+  <si>
+    <t>AMEXCREDIT</t>
+  </si>
+  <si>
+    <t>BLACKEYEFD [576771]</t>
+  </si>
+  <si>
+    <t>Amex Credit</t>
+  </si>
+  <si>
+    <t>AMEXBLACKE</t>
+  </si>
+  <si>
+    <t>http://ech-10-168-131-18.mastercard.int:25003/integratedIssuing-customerPortal/mtps/app/Login?0</t>
   </si>
 </sst>
 </file>
@@ -4481,49 +4502,49 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>206</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>489</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>491</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>307</v>
@@ -4634,7 +4655,7 @@
         <v>12</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="BD1" s="1" t="s">
         <v>13</v>
@@ -4673,7 +4694,7 @@
         <v>22</v>
       </c>
       <c r="BP1" s="4" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="BQ1" s="4" t="s">
         <v>24</v>
@@ -4709,7 +4730,7 @@
         <v>135</v>
       </c>
       <c r="CB1" s="4" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="CC1" s="4" t="s">
         <v>66</v>
@@ -4814,129 +4835,129 @@
         <v>52</v>
       </c>
       <c r="DK1" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="DM1" s="4" t="s">
         <v>495</v>
-      </c>
-      <c r="DL1" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="DM1" s="4" t="s">
-        <v>497</v>
       </c>
       <c r="DN1" s="1" t="s">
         <v>196</v>
       </c>
       <c r="DO1" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="DP1" s="36" t="s">
+        <v>497</v>
+      </c>
+      <c r="DQ1" s="36" t="s">
         <v>498</v>
       </c>
-      <c r="DP1" s="36" t="s">
+      <c r="DR1" s="36" t="s">
         <v>499</v>
       </c>
-      <c r="DQ1" s="36" t="s">
+      <c r="DS1" s="36" t="s">
         <v>500</v>
       </c>
-      <c r="DR1" s="36" t="s">
+      <c r="DT1" s="36" t="s">
         <v>501</v>
       </c>
-      <c r="DS1" s="36" t="s">
+      <c r="DU1" s="36" t="s">
         <v>502</v>
       </c>
-      <c r="DT1" s="36" t="s">
+      <c r="DV1" s="36" t="s">
         <v>503</v>
       </c>
-      <c r="DU1" s="36" t="s">
+      <c r="DW1" s="36" t="s">
         <v>504</v>
       </c>
-      <c r="DV1" s="36" t="s">
+      <c r="DX1" s="36" t="s">
         <v>505</v>
       </c>
-      <c r="DW1" s="36" t="s">
+      <c r="DY1" s="36" t="s">
         <v>506</v>
       </c>
-      <c r="DX1" s="36" t="s">
+      <c r="DZ1" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="DY1" s="36" t="s">
+      <c r="EA1" s="36" t="s">
         <v>508</v>
       </c>
-      <c r="DZ1" s="36" t="s">
+      <c r="EB1" s="36" t="s">
         <v>509</v>
       </c>
-      <c r="EA1" s="36" t="s">
+      <c r="EC1" s="36" t="s">
         <v>510</v>
       </c>
-      <c r="EB1" s="36" t="s">
+      <c r="ED1" s="36" t="s">
         <v>511</v>
       </c>
-      <c r="EC1" s="36" t="s">
+      <c r="EE1" s="36" t="s">
         <v>512</v>
-      </c>
-      <c r="ED1" s="36" t="s">
-        <v>513</v>
-      </c>
-      <c r="EE1" s="36" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="2" spans="1:135" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>515</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="F2" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>518</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>520</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>134</v>
       </c>
       <c r="I2" s="28" t="s">
+        <v>519</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="K2" s="38" t="s">
         <v>521</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="38" t="s">
         <v>522</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="M2" s="38" t="s">
         <v>523</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="N2" s="39" t="s">
         <v>524</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="O2" s="39" t="s">
         <v>525</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="P2" s="39" t="s">
+        <v>525</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="O2" s="39" t="s">
+      <c r="R2" s="39" t="s">
         <v>527</v>
       </c>
-      <c r="P2" s="39" t="s">
-        <v>527</v>
-      </c>
-      <c r="Q2" s="3" t="s">
+      <c r="S2" s="39" t="s">
         <v>528</v>
       </c>
-      <c r="R2" s="39" t="s">
+      <c r="T2" s="39" t="s">
         <v>529</v>
-      </c>
-      <c r="S2" s="39" t="s">
-        <v>530</v>
-      </c>
-      <c r="T2" s="39" t="s">
-        <v>531</v>
       </c>
       <c r="U2" s="11">
         <v>50</v>
@@ -4964,16 +4985,16 @@
       </c>
       <c r="AE2" s="12"/>
       <c r="AF2" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="AG2" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="AH2" s="12" t="s">
         <v>532</v>
       </c>
-      <c r="AG2" s="12" t="s">
+      <c r="AI2" s="12" t="s">
         <v>533</v>
-      </c>
-      <c r="AH2" s="12" t="s">
-        <v>534</v>
-      </c>
-      <c r="AI2" s="12" t="s">
-        <v>535</v>
       </c>
       <c r="AJ2" s="12" t="s">
         <v>36</v>
@@ -4994,7 +5015,7 @@
         <v>121</v>
       </c>
       <c r="AP2" s="12" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="AQ2" s="12" t="s">
         <v>120</v>
@@ -5031,7 +5052,7 @@
         <v>1</v>
       </c>
       <c r="BC2" s="12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="BD2" s="12" t="s">
         <v>16</v>
@@ -5043,7 +5064,7 @@
         <v>12</v>
       </c>
       <c r="BG2" s="12" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="BH2" s="12">
         <v>2</v>
@@ -5061,7 +5082,7 @@
         <v>29</v>
       </c>
       <c r="BM2" s="12" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="BN2" s="12" t="s">
         <v>199</v>
@@ -5091,20 +5112,20 @@
         <v>12345678</v>
       </c>
       <c r="BW2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="BX2" s="42"/>
       <c r="BY2" s="12" t="s">
         <v>143</v>
       </c>
       <c r="BZ2" s="12" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="CA2" s="12" t="s">
         <v>136</v>
       </c>
       <c r="CB2" s="12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="CC2" s="12" t="s">
         <v>67</v>
@@ -5131,13 +5152,13 @@
         <v>40</v>
       </c>
       <c r="CM2" s="42" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="CN2" s="12" t="s">
         <v>145</v>
       </c>
       <c r="CO2" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="CP2" s="40" t="s">
         <v>355</v>
@@ -5154,7 +5175,7 @@
       <c r="CT2" s="11"/>
       <c r="CU2" s="11"/>
       <c r="CV2" s="40" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="CW2" s="12" t="s">
         <v>133</v>
@@ -5191,40 +5212,40 @@
         <v>53</v>
       </c>
       <c r="DK2" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="DL2" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="DM2" s="12" t="s">
         <v>543</v>
-      </c>
-      <c r="DL2" s="11" t="s">
-        <v>544</v>
-      </c>
-      <c r="DM2" s="12" t="s">
-        <v>545</v>
       </c>
       <c r="DN2" s="12" t="s">
         <v>197</v>
       </c>
       <c r="DO2" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="DP2" s="43" t="s">
+        <v>545</v>
+      </c>
+      <c r="DQ2" s="43" t="s">
         <v>546</v>
       </c>
-      <c r="DP2" s="43" t="s">
+      <c r="DR2" s="43" t="s">
         <v>547</v>
       </c>
-      <c r="DQ2" s="43" t="s">
+      <c r="DS2" s="44" t="s">
         <v>548</v>
-      </c>
-      <c r="DR2" s="43" t="s">
-        <v>549</v>
-      </c>
-      <c r="DS2" s="44" t="s">
-        <v>550</v>
       </c>
       <c r="DT2" s="44" t="s">
         <v>405</v>
       </c>
       <c r="DU2" s="44" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="DV2" s="43" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="DW2" s="43" t="s">
         <v>134</v>
@@ -5233,25 +5254,25 @@
         <v>404</v>
       </c>
       <c r="DY2" s="44" t="s">
+        <v>551</v>
+      </c>
+      <c r="DZ2" s="44" t="s">
+        <v>552</v>
+      </c>
+      <c r="EA2" s="44" t="s">
+        <v>523</v>
+      </c>
+      <c r="EB2" s="44" t="s">
+        <v>552</v>
+      </c>
+      <c r="EC2" s="44" t="s">
         <v>553</v>
       </c>
-      <c r="DZ2" s="44" t="s">
+      <c r="ED2" s="44" t="s">
         <v>554</v>
       </c>
-      <c r="EA2" s="44" t="s">
-        <v>525</v>
-      </c>
-      <c r="EB2" s="44" t="s">
-        <v>554</v>
-      </c>
-      <c r="EC2" s="44" t="s">
+      <c r="EE2" s="43" t="s">
         <v>555</v>
-      </c>
-      <c r="ED2" s="44" t="s">
-        <v>556</v>
-      </c>
-      <c r="EE2" s="43" t="s">
-        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -5285,49 +5306,49 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>206</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>488</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>489</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>491</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>307</v>
@@ -5438,7 +5459,7 @@
         <v>12</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="BD1" s="1" t="s">
         <v>13</v>
@@ -5477,7 +5498,7 @@
         <v>22</v>
       </c>
       <c r="BP1" s="4" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="BQ1" s="4" t="s">
         <v>24</v>
@@ -5513,7 +5534,7 @@
         <v>135</v>
       </c>
       <c r="CB1" s="4" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="CC1" s="4" t="s">
         <v>66</v>
@@ -5618,153 +5639,153 @@
         <v>52</v>
       </c>
       <c r="DK1" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="DL1" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="DM1" s="4" t="s">
         <v>495</v>
-      </c>
-      <c r="DL1" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="DM1" s="4" t="s">
-        <v>497</v>
       </c>
       <c r="DN1" s="1" t="s">
         <v>196</v>
       </c>
       <c r="DO1" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="DP1" s="36" t="s">
+        <v>497</v>
+      </c>
+      <c r="DQ1" s="36" t="s">
         <v>498</v>
       </c>
-      <c r="DP1" s="36" t="s">
+      <c r="DR1" s="36" t="s">
         <v>499</v>
       </c>
-      <c r="DQ1" s="36" t="s">
+      <c r="DS1" s="36" t="s">
         <v>500</v>
       </c>
-      <c r="DR1" s="36" t="s">
+      <c r="DT1" s="36" t="s">
         <v>501</v>
       </c>
-      <c r="DS1" s="36" t="s">
+      <c r="DU1" s="36" t="s">
         <v>502</v>
       </c>
-      <c r="DT1" s="36" t="s">
+      <c r="DV1" s="36" t="s">
         <v>503</v>
       </c>
-      <c r="DU1" s="36" t="s">
+      <c r="DW1" s="36" t="s">
         <v>504</v>
       </c>
-      <c r="DV1" s="36" t="s">
+      <c r="DX1" s="36" t="s">
         <v>505</v>
       </c>
-      <c r="DW1" s="36" t="s">
+      <c r="DY1" s="36" t="s">
         <v>506</v>
       </c>
-      <c r="DX1" s="36" t="s">
+      <c r="DZ1" s="36" t="s">
         <v>507</v>
       </c>
-      <c r="DY1" s="36" t="s">
+      <c r="EA1" s="36" t="s">
         <v>508</v>
       </c>
-      <c r="DZ1" s="36" t="s">
+      <c r="EB1" s="36" t="s">
         <v>509</v>
       </c>
-      <c r="EA1" s="36" t="s">
+      <c r="EC1" s="36" t="s">
         <v>510</v>
       </c>
-      <c r="EB1" s="36" t="s">
+      <c r="ED1" s="36" t="s">
+        <v>695</v>
+      </c>
+      <c r="EE1" s="36" t="s">
+        <v>696</v>
+      </c>
+      <c r="EF1" s="36" t="s">
         <v>511</v>
       </c>
-      <c r="EC1" s="36" t="s">
+      <c r="EG1" s="36" t="s">
+        <v>697</v>
+      </c>
+      <c r="EH1" s="36" t="s">
+        <v>698</v>
+      </c>
+      <c r="EI1" s="36" t="s">
+        <v>699</v>
+      </c>
+      <c r="EJ1" s="36" t="s">
+        <v>700</v>
+      </c>
+      <c r="EK1" s="36" t="s">
+        <v>701</v>
+      </c>
+      <c r="EL1" s="36" t="s">
+        <v>702</v>
+      </c>
+      <c r="EM1" s="36" t="s">
         <v>512</v>
-      </c>
-      <c r="ED1" s="36" t="s">
-        <v>697</v>
-      </c>
-      <c r="EE1" s="36" t="s">
-        <v>698</v>
-      </c>
-      <c r="EF1" s="36" t="s">
-        <v>513</v>
-      </c>
-      <c r="EG1" s="36" t="s">
-        <v>699</v>
-      </c>
-      <c r="EH1" s="36" t="s">
-        <v>700</v>
-      </c>
-      <c r="EI1" s="36" t="s">
-        <v>701</v>
-      </c>
-      <c r="EJ1" s="36" t="s">
-        <v>702</v>
-      </c>
-      <c r="EK1" s="36" t="s">
-        <v>703</v>
-      </c>
-      <c r="EL1" s="36" t="s">
-        <v>704</v>
-      </c>
-      <c r="EM1" s="36" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="2" spans="1:143" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="B2" t="s">
+        <v>703</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>515</v>
       </c>
-      <c r="B2" t="s">
-        <v>705</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>516</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="F2" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>518</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>520</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>134</v>
       </c>
       <c r="I2" s="28" t="s">
+        <v>519</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="K2" s="38" t="s">
         <v>521</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="38" t="s">
         <v>522</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="M2" s="38" t="s">
         <v>523</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="N2" s="39" t="s">
         <v>524</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="O2" s="39" t="s">
         <v>525</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="P2" s="39" t="s">
+        <v>525</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="O2" s="39" t="s">
+      <c r="R2" s="39" t="s">
         <v>527</v>
       </c>
-      <c r="P2" s="39" t="s">
-        <v>527</v>
-      </c>
-      <c r="Q2" s="3" t="s">
+      <c r="S2" s="39" t="s">
         <v>528</v>
       </c>
-      <c r="R2" s="39" t="s">
+      <c r="T2" s="39" t="s">
         <v>529</v>
-      </c>
-      <c r="S2" s="39" t="s">
-        <v>530</v>
-      </c>
-      <c r="T2" s="39" t="s">
-        <v>531</v>
       </c>
       <c r="U2" s="11">
         <v>50</v>
@@ -5792,16 +5813,16 @@
       </c>
       <c r="AE2" s="12"/>
       <c r="AF2" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="AG2" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="AH2" s="12" t="s">
         <v>532</v>
       </c>
-      <c r="AG2" s="12" t="s">
+      <c r="AI2" s="12" t="s">
         <v>533</v>
-      </c>
-      <c r="AH2" s="12" t="s">
-        <v>534</v>
-      </c>
-      <c r="AI2" s="12" t="s">
-        <v>535</v>
       </c>
       <c r="AJ2" s="12" t="s">
         <v>36</v>
@@ -5822,7 +5843,7 @@
         <v>121</v>
       </c>
       <c r="AP2" s="12" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="AQ2" s="12" t="s">
         <v>120</v>
@@ -5859,7 +5880,7 @@
         <v>1</v>
       </c>
       <c r="BC2" s="12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="BD2" s="12" t="s">
         <v>16</v>
@@ -5871,7 +5892,7 @@
         <v>12</v>
       </c>
       <c r="BG2" s="12" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="BH2" s="12">
         <v>2</v>
@@ -5889,7 +5910,7 @@
         <v>29</v>
       </c>
       <c r="BM2" s="12" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="BN2" s="12" t="s">
         <v>199</v>
@@ -5919,20 +5940,20 @@
         <v>12345678</v>
       </c>
       <c r="BW2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="BX2" s="42"/>
       <c r="BY2" s="12" t="s">
         <v>143</v>
       </c>
       <c r="BZ2" s="12" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="CA2" s="12" t="s">
         <v>136</v>
       </c>
       <c r="CB2" s="12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="CC2" s="12" t="s">
         <v>67</v>
@@ -5959,13 +5980,13 @@
         <v>40</v>
       </c>
       <c r="CM2" s="42" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="CN2" s="12" t="s">
         <v>145</v>
       </c>
       <c r="CO2" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="CP2" s="40" t="s">
         <v>355</v>
@@ -5982,7 +6003,7 @@
       <c r="CT2" s="11"/>
       <c r="CU2" s="11"/>
       <c r="CV2" s="40" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="CW2" s="12" t="s">
         <v>133</v>
@@ -6019,40 +6040,40 @@
         <v>53</v>
       </c>
       <c r="DK2" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="DL2" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="DM2" s="12" t="s">
         <v>543</v>
-      </c>
-      <c r="DL2" s="11" t="s">
-        <v>544</v>
-      </c>
-      <c r="DM2" s="12" t="s">
-        <v>545</v>
       </c>
       <c r="DN2" s="12" t="s">
         <v>197</v>
       </c>
       <c r="DO2" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="DP2" s="43" t="s">
+        <v>545</v>
+      </c>
+      <c r="DQ2" s="43" t="s">
         <v>546</v>
       </c>
-      <c r="DP2" s="43" t="s">
+      <c r="DR2" s="43" t="s">
         <v>547</v>
       </c>
-      <c r="DQ2" s="43" t="s">
+      <c r="DS2" s="44" t="s">
         <v>548</v>
-      </c>
-      <c r="DR2" s="43" t="s">
-        <v>549</v>
-      </c>
-      <c r="DS2" s="44" t="s">
-        <v>550</v>
       </c>
       <c r="DT2" s="44" t="s">
         <v>405</v>
       </c>
       <c r="DU2" s="44" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="DV2" s="43" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="DW2" s="43" t="s">
         <v>134</v>
@@ -6061,24 +6082,24 @@
         <v>404</v>
       </c>
       <c r="DY2" s="44" t="s">
+        <v>551</v>
+      </c>
+      <c r="DZ2" s="44" t="s">
+        <v>552</v>
+      </c>
+      <c r="EA2" s="44" t="s">
+        <v>523</v>
+      </c>
+      <c r="EB2" s="44" t="s">
+        <v>552</v>
+      </c>
+      <c r="EC2" s="44" t="s">
         <v>553</v>
-      </c>
-      <c r="DZ2" s="44" t="s">
-        <v>554</v>
-      </c>
-      <c r="EA2" s="44" t="s">
-        <v>525</v>
-      </c>
-      <c r="EB2" s="44" t="s">
-        <v>554</v>
-      </c>
-      <c r="EC2" s="44" t="s">
-        <v>555</v>
       </c>
       <c r="ED2" s="44"/>
       <c r="EE2" s="44"/>
       <c r="EF2" s="44" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="EG2" s="44"/>
       <c r="EH2" s="44"/>
@@ -6087,75 +6108,75 @@
       <c r="EK2" s="44"/>
       <c r="EL2" s="44"/>
       <c r="EM2" s="43" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="3" spans="1:143" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B3" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>386</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>518</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>519</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>520</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>134</v>
       </c>
       <c r="I3" s="28" t="s">
+        <v>519</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="K3" s="38" t="s">
         <v>521</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="38" t="s">
         <v>522</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="M3" s="38" t="s">
         <v>523</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="N3" s="39" t="s">
         <v>524</v>
       </c>
-      <c r="M3" s="38" t="s">
+      <c r="O3" s="39" t="s">
         <v>525</v>
       </c>
-      <c r="N3" s="39" t="s">
+      <c r="P3" s="39" t="s">
+        <v>525</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>526</v>
       </c>
-      <c r="O3" s="39" t="s">
+      <c r="R3" s="39" t="s">
         <v>527</v>
-      </c>
-      <c r="P3" s="39" t="s">
-        <v>527</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="R3" s="39" t="s">
-        <v>529</v>
       </c>
       <c r="S3" s="39" t="s">
         <v>389</v>
       </c>
       <c r="T3" s="39" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="U3" s="11">
         <v>50</v>
       </c>
       <c r="V3" s="11" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="W3" s="11" t="s">
         <v>128</v>
@@ -6177,16 +6198,16 @@
       </c>
       <c r="AE3" s="12"/>
       <c r="AF3" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="AG3" s="12" t="s">
+        <v>531</v>
+      </c>
+      <c r="AH3" s="12" t="s">
         <v>532</v>
       </c>
-      <c r="AG3" s="12" t="s">
+      <c r="AI3" s="12" t="s">
         <v>533</v>
-      </c>
-      <c r="AH3" s="12" t="s">
-        <v>534</v>
-      </c>
-      <c r="AI3" s="12" t="s">
-        <v>535</v>
       </c>
       <c r="AJ3" s="12" t="s">
         <v>36</v>
@@ -6207,7 +6228,7 @@
         <v>121</v>
       </c>
       <c r="AP3" s="12" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="AQ3" s="12" t="s">
         <v>120</v>
@@ -6244,19 +6265,19 @@
         <v>1</v>
       </c>
       <c r="BC3" s="12" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="BD3" s="12" t="s">
         <v>16</v>
       </c>
       <c r="BE3" s="12" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="BF3" s="12">
         <v>12</v>
       </c>
       <c r="BG3" s="12" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="BH3" s="12">
         <v>2</v>
@@ -6274,7 +6295,7 @@
         <v>29</v>
       </c>
       <c r="BM3" s="12" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="BN3" s="12" t="s">
         <v>199</v>
@@ -6304,20 +6325,20 @@
         <v>12345678</v>
       </c>
       <c r="BW3" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="BX3" s="42"/>
       <c r="BY3" s="12" t="s">
         <v>143</v>
       </c>
       <c r="BZ3" s="12" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="CA3" s="12" t="s">
         <v>136</v>
       </c>
       <c r="CB3" s="12" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="CC3" s="12" t="s">
         <v>67</v>
@@ -6344,13 +6365,13 @@
         <v>40</v>
       </c>
       <c r="CM3" s="42" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="CN3" s="12" t="s">
         <v>145</v>
       </c>
       <c r="CO3" s="11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="CP3" s="40" t="s">
         <v>355</v>
@@ -6362,12 +6383,12 @@
         <v>51</v>
       </c>
       <c r="CS3" s="64" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="CT3" s="11"/>
       <c r="CU3" s="11"/>
       <c r="CV3" s="40" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="CW3" s="12" t="s">
         <v>133</v>
@@ -6404,40 +6425,40 @@
         <v>53</v>
       </c>
       <c r="DK3" s="11" t="s">
+        <v>541</v>
+      </c>
+      <c r="DL3" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="DM3" s="12" t="s">
         <v>543</v>
-      </c>
-      <c r="DL3" s="11" t="s">
-        <v>544</v>
-      </c>
-      <c r="DM3" s="12" t="s">
-        <v>545</v>
       </c>
       <c r="DN3" s="12" t="s">
         <v>197</v>
       </c>
       <c r="DO3" s="11" t="s">
+        <v>544</v>
+      </c>
+      <c r="DP3" s="43" t="s">
+        <v>545</v>
+      </c>
+      <c r="DQ3" s="43" t="s">
         <v>546</v>
       </c>
-      <c r="DP3" s="43" t="s">
+      <c r="DR3" s="43" t="s">
         <v>547</v>
       </c>
-      <c r="DQ3" s="43" t="s">
+      <c r="DS3" s="44" t="s">
         <v>548</v>
-      </c>
-      <c r="DR3" s="43" t="s">
-        <v>549</v>
-      </c>
-      <c r="DS3" s="44" t="s">
-        <v>550</v>
       </c>
       <c r="DT3" s="44" t="s">
         <v>405</v>
       </c>
       <c r="DU3" s="44" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="DV3" s="43" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="DW3" s="43" t="s">
         <v>134</v>
@@ -6446,24 +6467,24 @@
         <v>404</v>
       </c>
       <c r="DY3" s="44" t="s">
+        <v>551</v>
+      </c>
+      <c r="DZ3" s="44" t="s">
+        <v>552</v>
+      </c>
+      <c r="EA3" s="44" t="s">
+        <v>523</v>
+      </c>
+      <c r="EB3" s="44" t="s">
+        <v>552</v>
+      </c>
+      <c r="EC3" s="44" t="s">
         <v>553</v>
-      </c>
-      <c r="DZ3" s="44" t="s">
-        <v>554</v>
-      </c>
-      <c r="EA3" s="44" t="s">
-        <v>525</v>
-      </c>
-      <c r="EB3" s="44" t="s">
-        <v>554</v>
-      </c>
-      <c r="EC3" s="44" t="s">
-        <v>555</v>
       </c>
       <c r="ED3" s="44"/>
       <c r="EE3" s="44"/>
       <c r="EF3" s="44" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="EG3" s="44" t="s">
         <v>410</v>
@@ -6475,16 +6496,16 @@
         <v>51</v>
       </c>
       <c r="EJ3" s="44" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="EK3" s="44" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="EL3" s="44" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="EM3" s="43" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -6518,25 +6539,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>566</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>574</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>576</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>307</v>
@@ -6547,37 +6568,37 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>570</v>
-      </c>
       <c r="K2" s="9" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>398</v>
@@ -6665,192 +6686,192 @@
         <v>308</v>
       </c>
       <c r="E1" s="46" t="s">
+        <v>578</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>579</v>
+      </c>
+      <c r="G1" s="46" t="s">
         <v>580</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="H1" s="48" t="s">
         <v>581</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="I1" s="48" t="s">
         <v>582</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="J1" s="48" t="s">
         <v>583</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="K1" s="48" t="s">
         <v>584</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="L1" s="48" t="s">
         <v>585</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="M1" s="48" t="s">
         <v>586</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="N1" s="48" t="s">
         <v>587</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="O1" s="48" t="s">
         <v>588</v>
       </c>
-      <c r="N1" s="48" t="s">
+      <c r="P1" s="48" t="s">
         <v>589</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="Q1" s="48" t="s">
         <v>590</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="R1" s="48" t="s">
         <v>591</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="S1" s="49" t="s">
         <v>592</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="T1" s="49" t="s">
         <v>593</v>
       </c>
-      <c r="S1" s="49" t="s">
+      <c r="U1" s="50" t="s">
         <v>594</v>
       </c>
-      <c r="T1" s="49" t="s">
+      <c r="V1" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="U1" s="50" t="s">
+      <c r="W1" s="1" t="s">
         <v>596</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>598</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="48" t="s">
         <v>600</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="AA1" s="48" t="s">
+      <c r="AC1" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="51" t="s">
         <v>610</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="AK1" s="51" t="s">
+      <c r="AM1" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>620</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>625</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>627</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>629</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="2" spans="1:56" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
+        <v>630</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>631</v>
+      </c>
+      <c r="C2" s="54" t="s">
         <v>632</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="D2" s="54" t="s">
+        <v>632</v>
+      </c>
+      <c r="E2" s="52" t="s">
         <v>633</v>
-      </c>
-      <c r="C2" s="54" t="s">
-        <v>634</v>
-      </c>
-      <c r="D2" s="54" t="s">
-        <v>634</v>
-      </c>
-      <c r="E2" s="52" t="s">
-        <v>635</v>
       </c>
       <c r="F2" s="52">
         <v>10</v>
       </c>
       <c r="G2" s="52" t="s">
+        <v>634</v>
+      </c>
+      <c r="H2" s="55" t="s">
+        <v>635</v>
+      </c>
+      <c r="I2" s="56" t="s">
         <v>636</v>
       </c>
-      <c r="H2" s="55" t="s">
-        <v>637</v>
-      </c>
-      <c r="I2" s="56" t="s">
-        <v>638</v>
-      </c>
       <c r="J2" s="55" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="K2" s="52"/>
       <c r="L2" s="52">
@@ -6859,25 +6880,25 @@
       <c r="M2" s="52"/>
       <c r="N2" s="52"/>
       <c r="O2" s="57" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="P2" s="52" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="Q2" s="58">
         <v>5</v>
       </c>
       <c r="R2" s="58" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="S2" s="58" t="s">
+        <v>639</v>
+      </c>
+      <c r="T2" s="58" t="s">
+        <v>640</v>
+      </c>
+      <c r="U2" s="52" t="s">
         <v>641</v>
-      </c>
-      <c r="T2" s="58" t="s">
-        <v>642</v>
-      </c>
-      <c r="U2" s="52" t="s">
-        <v>643</v>
       </c>
       <c r="V2" s="52"/>
       <c r="W2" s="55"/>
@@ -6917,28 +6938,28 @@
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="B3" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>632</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>632</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>634</v>
-      </c>
-      <c r="D3" s="54" t="s">
-        <v>634</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F3" s="2">
         <v>5</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -6991,28 +7012,28 @@
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B4" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C4" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D4" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F4" s="2">
         <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
@@ -7065,52 +7086,52 @@
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="B5" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C5" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D5" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F5" s="2">
         <v>5</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>410</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="L5" s="2">
         <v>955689456</v>
       </c>
       <c r="M5" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="O5" s="60" t="s">
+        <v>637</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>649</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>650</v>
-      </c>
-      <c r="O5" s="60" t="s">
-        <v>639</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>651</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -7155,28 +7176,28 @@
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B6" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C6" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D6" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F6" s="2">
         <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
@@ -7229,28 +7250,28 @@
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="B7" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D7" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F7" s="2">
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -7269,10 +7290,10 @@
         <v>10</v>
       </c>
       <c r="W7" s="9" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
@@ -7309,28 +7330,28 @@
     </row>
     <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="B8" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D8" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C8" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D8" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F8" s="2">
         <v>5</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
@@ -7349,16 +7370,16 @@
         <v>10</v>
       </c>
       <c r="W8" s="9" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="X8" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="Y8" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="Y8" s="2" t="s">
-        <v>657</v>
-      </c>
       <c r="Z8" s="61" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
@@ -7393,28 +7414,28 @@
     </row>
     <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B9" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C9" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D9" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F9" s="2">
         <v>5</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
@@ -7433,28 +7454,28 @@
         <v>10</v>
       </c>
       <c r="W9" s="9" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="X9" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="Y9" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="Y9" s="2" t="s">
-        <v>657</v>
-      </c>
       <c r="Z9" s="61" t="s">
+        <v>656</v>
+      </c>
+      <c r="AA9" s="61" t="s">
         <v>658</v>
       </c>
-      <c r="AA9" s="61" t="s">
+      <c r="AB9" s="61" t="s">
+        <v>659</v>
+      </c>
+      <c r="AC9" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="AB9" s="61" t="s">
+      <c r="AD9" s="2" t="s">
         <v>661</v>
-      </c>
-      <c r="AC9" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="AD9" s="2" t="s">
-        <v>663</v>
       </c>
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
@@ -7485,28 +7506,28 @@
     </row>
     <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B10" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C10" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D10" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F10" s="2">
         <v>5</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
@@ -7525,28 +7546,28 @@
         <v>10</v>
       </c>
       <c r="W10" s="9" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="X10" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="Y10" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="Y10" s="2" t="s">
-        <v>657</v>
-      </c>
       <c r="Z10" s="61" t="s">
+        <v>656</v>
+      </c>
+      <c r="AA10" s="61" t="s">
         <v>658</v>
       </c>
-      <c r="AA10" s="61" t="s">
+      <c r="AB10" s="61" t="s">
+        <v>659</v>
+      </c>
+      <c r="AC10" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="AB10" s="61" t="s">
+      <c r="AD10" s="2" t="s">
         <v>661</v>
-      </c>
-      <c r="AC10" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="AD10" s="2" t="s">
-        <v>663</v>
       </c>
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
@@ -7577,28 +7598,28 @@
     </row>
     <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B11" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C11" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D11" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F11" s="2">
         <v>5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
@@ -7617,38 +7638,38 @@
         <v>10</v>
       </c>
       <c r="W11" s="9" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="X11" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="Y11" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="Y11" s="2" t="s">
-        <v>657</v>
-      </c>
       <c r="Z11" s="61" t="s">
+        <v>656</v>
+      </c>
+      <c r="AA11" s="61" t="s">
         <v>658</v>
       </c>
-      <c r="AA11" s="61" t="s">
+      <c r="AB11" s="61" t="s">
+        <v>659</v>
+      </c>
+      <c r="AC11" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="AB11" s="61" t="s">
+      <c r="AD11" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="AC11" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="AD11" s="2" t="s">
-        <v>663</v>
-      </c>
       <c r="AE11" s="2" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="AF11" s="2"/>
       <c r="AG11" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="AH11" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="AI11" s="2"/>
       <c r="AJ11" s="2"/>
@@ -7675,28 +7696,28 @@
     </row>
     <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B12" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D12" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C12" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D12" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F12" s="2">
         <v>5</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -7715,38 +7736,38 @@
         <v>10</v>
       </c>
       <c r="W12" s="9" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="X12" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="Y12" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="Y12" s="2" t="s">
-        <v>657</v>
-      </c>
       <c r="Z12" s="61" t="s">
+        <v>656</v>
+      </c>
+      <c r="AA12" s="61" t="s">
         <v>658</v>
       </c>
-      <c r="AA12" s="61" t="s">
+      <c r="AB12" s="61" t="s">
+        <v>659</v>
+      </c>
+      <c r="AC12" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="AB12" s="61" t="s">
+      <c r="AD12" s="2" t="s">
         <v>661</v>
-      </c>
-      <c r="AC12" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="AD12" s="2" t="s">
-        <v>663</v>
       </c>
       <c r="AE12" s="2"/>
       <c r="AF12" s="2" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="AG12" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="AH12" s="2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="AI12" s="2"/>
       <c r="AJ12" s="2"/>
@@ -7773,28 +7794,28 @@
     </row>
     <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B13" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C13" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D13" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F13" s="2">
         <v>5</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -7813,41 +7834,41 @@
         <v>10</v>
       </c>
       <c r="W13" s="9" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="X13" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="Y13" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="Y13" s="2" t="s">
-        <v>657</v>
-      </c>
       <c r="Z13" s="61" t="s">
+        <v>656</v>
+      </c>
+      <c r="AA13" s="61" t="s">
         <v>658</v>
       </c>
-      <c r="AA13" s="61" t="s">
+      <c r="AB13" s="61" t="s">
+        <v>659</v>
+      </c>
+      <c r="AC13" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="AB13" s="61" t="s">
+      <c r="AD13" s="2" t="s">
         <v>661</v>
-      </c>
-      <c r="AC13" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="AD13" s="2" t="s">
-        <v>663</v>
       </c>
       <c r="AE13" s="2"/>
       <c r="AF13" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="AH13" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="AI13" s="61" t="s">
         <v>669</v>
-      </c>
-      <c r="AG13" s="2" t="s">
-        <v>667</v>
-      </c>
-      <c r="AH13" s="2" t="s">
-        <v>667</v>
-      </c>
-      <c r="AI13" s="61" t="s">
-        <v>671</v>
       </c>
       <c r="AJ13" s="2"/>
       <c r="AK13" s="2"/>
@@ -7873,28 +7894,28 @@
     </row>
     <row r="14" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="B14" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C14" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D14" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F14" s="2">
         <v>5</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -7913,41 +7934,41 @@
         <v>10</v>
       </c>
       <c r="W14" s="9" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="X14" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="Y14" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="Y14" s="2" t="s">
-        <v>657</v>
-      </c>
       <c r="Z14" s="61" t="s">
+        <v>656</v>
+      </c>
+      <c r="AA14" s="61" t="s">
         <v>658</v>
       </c>
-      <c r="AA14" s="61" t="s">
+      <c r="AB14" s="61" t="s">
+        <v>659</v>
+      </c>
+      <c r="AC14" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="AB14" s="61" t="s">
+      <c r="AD14" s="2" t="s">
         <v>661</v>
-      </c>
-      <c r="AC14" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="AD14" s="2" t="s">
-        <v>663</v>
       </c>
       <c r="AE14" s="2"/>
       <c r="AF14" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="AH14" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="AI14" s="61" t="s">
         <v>669</v>
-      </c>
-      <c r="AG14" s="2" t="s">
-        <v>667</v>
-      </c>
-      <c r="AH14" s="2" t="s">
-        <v>667</v>
-      </c>
-      <c r="AI14" s="61" t="s">
-        <v>671</v>
       </c>
       <c r="AJ14" s="2"/>
       <c r="AK14" s="2"/>
@@ -7973,28 +7994,28 @@
     </row>
     <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="B15" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D15" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C15" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D15" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F15" s="2">
         <v>5</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
@@ -8013,41 +8034,41 @@
         <v>10</v>
       </c>
       <c r="W15" s="9" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="X15" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="Y15" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="Y15" s="2" t="s">
-        <v>657</v>
-      </c>
       <c r="Z15" s="61" t="s">
+        <v>656</v>
+      </c>
+      <c r="AA15" s="61" t="s">
         <v>658</v>
       </c>
-      <c r="AA15" s="61" t="s">
+      <c r="AB15" s="61" t="s">
+        <v>659</v>
+      </c>
+      <c r="AC15" s="2" t="s">
         <v>660</v>
       </c>
-      <c r="AB15" s="61" t="s">
+      <c r="AD15" s="2" t="s">
         <v>661</v>
-      </c>
-      <c r="AC15" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="AD15" s="2" t="s">
-        <v>663</v>
       </c>
       <c r="AE15" s="2"/>
       <c r="AF15" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="AH15" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="AI15" s="61" t="s">
         <v>669</v>
-      </c>
-      <c r="AG15" s="2" t="s">
-        <v>667</v>
-      </c>
-      <c r="AH15" s="2" t="s">
-        <v>667</v>
-      </c>
-      <c r="AI15" s="61" t="s">
-        <v>671</v>
       </c>
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
@@ -8073,28 +8094,28 @@
     </row>
     <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B16" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C16" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D16" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F16" s="2">
         <v>5</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
@@ -8124,31 +8145,31 @@
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
       <c r="AJ16" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AK16" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="AL16" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="AK16" s="2" t="s">
+      <c r="AM16" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="AL16" s="2" t="s">
+      <c r="AN16" s="2" t="s">
         <v>677</v>
       </c>
-      <c r="AM16" s="2" t="s">
+      <c r="AO16" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="AP16" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="AN16" s="2" t="s">
+      <c r="AQ16" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="AO16" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="AP16" s="2" t="s">
+      <c r="AR16" s="2" t="s">
         <v>680</v>
-      </c>
-      <c r="AQ16" s="2" t="s">
-        <v>681</v>
-      </c>
-      <c r="AR16" s="2" t="s">
-        <v>682</v>
       </c>
       <c r="AS16" s="2" t="s">
         <v>30</v>
@@ -8157,7 +8178,7 @@
         <v>411033</v>
       </c>
       <c r="AU16" s="45" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="AV16" s="2">
         <v>7896543215</v>
@@ -8166,7 +8187,7 @@
         <v>5000</v>
       </c>
       <c r="AX16" s="2" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="AY16" s="2"/>
       <c r="AZ16" s="2"/>
@@ -8177,28 +8198,28 @@
     </row>
     <row r="17" spans="1:56" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="52" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B17" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D17" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E17" s="52" t="s">
         <v>633</v>
-      </c>
-      <c r="C17" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D17" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E17" s="52" t="s">
-        <v>635</v>
       </c>
       <c r="F17" s="52">
         <v>5</v>
       </c>
       <c r="G17" s="52" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H17" s="55" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I17" s="55"/>
       <c r="J17" s="55"/>
@@ -8228,31 +8249,31 @@
       <c r="AH17" s="52"/>
       <c r="AI17" s="52"/>
       <c r="AJ17" s="52" t="s">
+        <v>673</v>
+      </c>
+      <c r="AK17" s="52" t="s">
+        <v>674</v>
+      </c>
+      <c r="AL17" s="52" t="s">
         <v>675</v>
       </c>
-      <c r="AK17" s="52" t="s">
+      <c r="AM17" s="52" t="s">
         <v>676</v>
       </c>
-      <c r="AL17" s="52" t="s">
+      <c r="AN17" s="52" t="s">
         <v>677</v>
       </c>
-      <c r="AM17" s="52" t="s">
+      <c r="AO17" s="52" t="s">
+        <v>677</v>
+      </c>
+      <c r="AP17" s="52" t="s">
         <v>678</v>
       </c>
-      <c r="AN17" s="52" t="s">
+      <c r="AQ17" s="52" t="s">
         <v>679</v>
       </c>
-      <c r="AO17" s="52" t="s">
-        <v>679</v>
-      </c>
-      <c r="AP17" s="52" t="s">
+      <c r="AR17" s="52" t="s">
         <v>680</v>
-      </c>
-      <c r="AQ17" s="52" t="s">
-        <v>681</v>
-      </c>
-      <c r="AR17" s="52" t="s">
-        <v>682</v>
       </c>
       <c r="AS17" s="52" t="s">
         <v>30</v>
@@ -8261,7 +8282,7 @@
         <v>411033</v>
       </c>
       <c r="AU17" s="62" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="AV17" s="52">
         <v>7896543215</v>
@@ -8270,13 +8291,13 @@
         <v>5000</v>
       </c>
       <c r="AX17" s="52" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="AY17" s="52" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="AZ17" s="52" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="BA17" s="52"/>
       <c r="BB17" s="52"/>
@@ -8285,28 +8306,28 @@
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B18" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C18" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D18" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F18" s="2">
         <v>5</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
@@ -8336,31 +8357,31 @@
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
       <c r="AJ18" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AK18" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="AL18" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="AK18" s="2" t="s">
+      <c r="AM18" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="AL18" s="2" t="s">
+      <c r="AN18" s="2" t="s">
         <v>677</v>
       </c>
-      <c r="AM18" s="2" t="s">
+      <c r="AO18" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="AP18" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="AN18" s="2" t="s">
+      <c r="AQ18" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="AO18" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="AP18" s="2" t="s">
+      <c r="AR18" s="2" t="s">
         <v>680</v>
-      </c>
-      <c r="AQ18" s="2" t="s">
-        <v>681</v>
-      </c>
-      <c r="AR18" s="2" t="s">
-        <v>682</v>
       </c>
       <c r="AS18" s="2" t="s">
         <v>30</v>
@@ -8369,7 +8390,7 @@
         <v>411033</v>
       </c>
       <c r="AU18" s="45" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="AV18" s="2">
         <v>7896543215</v>
@@ -8378,13 +8399,13 @@
         <v>5000</v>
       </c>
       <c r="AX18" s="2" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="AY18" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="AZ18" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="BA18" s="2"/>
       <c r="BB18" s="2"/>
@@ -8393,28 +8414,28 @@
     </row>
     <row r="19" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B19" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C19" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C19" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D19" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F19" s="2">
         <v>5</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
@@ -8444,31 +8465,31 @@
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
       <c r="AJ19" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AK19" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="AL19" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="AK19" s="2" t="s">
+      <c r="AM19" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="AL19" s="2" t="s">
+      <c r="AN19" s="2" t="s">
         <v>677</v>
       </c>
-      <c r="AM19" s="2" t="s">
+      <c r="AO19" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="AP19" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="AN19" s="2" t="s">
+      <c r="AQ19" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="AO19" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="AP19" s="2" t="s">
+      <c r="AR19" s="2" t="s">
         <v>680</v>
-      </c>
-      <c r="AQ19" s="2" t="s">
-        <v>681</v>
-      </c>
-      <c r="AR19" s="2" t="s">
-        <v>682</v>
       </c>
       <c r="AS19" s="2" t="s">
         <v>30</v>
@@ -8477,7 +8498,7 @@
         <v>411033</v>
       </c>
       <c r="AU19" s="45" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="AV19" s="2">
         <v>7896543215</v>
@@ -8486,13 +8507,13 @@
         <v>5000</v>
       </c>
       <c r="AX19" s="2" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="AY19" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="AZ19" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="BA19" s="2"/>
       <c r="BB19" s="2"/>
@@ -8501,28 +8522,28 @@
     </row>
     <row r="20" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B20" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C20" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D20" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F20" s="2">
         <v>5</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
@@ -8552,31 +8573,31 @@
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
       <c r="AJ20" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="AK20" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="AL20" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="AK20" s="2" t="s">
+      <c r="AM20" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="AL20" s="2" t="s">
+      <c r="AN20" s="2" t="s">
         <v>677</v>
       </c>
-      <c r="AM20" s="2" t="s">
+      <c r="AO20" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="AP20" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="AN20" s="2" t="s">
+      <c r="AQ20" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="AO20" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="AP20" s="2" t="s">
+      <c r="AR20" s="2" t="s">
         <v>680</v>
-      </c>
-      <c r="AQ20" s="2" t="s">
-        <v>681</v>
-      </c>
-      <c r="AR20" s="2" t="s">
-        <v>682</v>
       </c>
       <c r="AS20" s="2" t="s">
         <v>30</v>
@@ -8585,7 +8606,7 @@
         <v>411033</v>
       </c>
       <c r="AU20" s="45" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="AV20" s="2">
         <v>7896543215</v>
@@ -8594,13 +8615,13 @@
         <v>5000</v>
       </c>
       <c r="AX20" s="2" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="AY20" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="AZ20" s="2" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="BA20" s="2"/>
       <c r="BB20" s="2"/>
@@ -8609,28 +8630,28 @@
     </row>
     <row r="21" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B21" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D21" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C21" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D21" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F21" s="2">
         <v>5</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
@@ -8683,28 +8704,28 @@
     </row>
     <row r="22" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B22" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D22" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C22" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D22" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F22" s="2">
         <v>5</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -8757,28 +8778,28 @@
     </row>
     <row r="23" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B23" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C23" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D23" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C23" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D23" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F23" s="2">
         <v>5</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
@@ -8831,28 +8852,28 @@
     </row>
     <row r="24" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B24" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D24" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C24" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D24" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F24" s="2">
         <v>5</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -8905,28 +8926,28 @@
     </row>
     <row r="25" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B25" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D25" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C25" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D25" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F25" s="2">
         <v>5</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
@@ -8979,28 +9000,28 @@
     </row>
     <row r="26" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B26" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C26" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D26" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C26" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D26" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F26" s="2">
         <v>5</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
@@ -9053,28 +9074,28 @@
     </row>
     <row r="27" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B27" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C27" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D27" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C27" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D27" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F27" s="2">
         <v>5</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
@@ -9127,52 +9148,52 @@
     </row>
     <row r="28" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B28" s="59" t="s">
+        <v>631</v>
+      </c>
+      <c r="C28" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="D28" s="54" t="s">
+        <v>644</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="C28" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="D28" s="54" t="s">
-        <v>646</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>635</v>
       </c>
       <c r="F28" s="2">
         <v>5</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="I28" s="9" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>410</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="L28" s="2">
         <v>955689456</v>
       </c>
       <c r="M28" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="O28" s="60" t="s">
+        <v>637</v>
+      </c>
+      <c r="P28" s="2" t="s">
         <v>649</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>650</v>
-      </c>
-      <c r="O28" s="60" t="s">
-        <v>639</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>651</v>
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
@@ -9234,8 +9255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EN177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9595,97 +9616,97 @@
         <v>435</v>
       </c>
       <c r="DJ1" s="4" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="DK1" s="4" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="DL1" s="4" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="DM1" s="4" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="DN1" s="4" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="DO1" s="4" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="DP1" s="4" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="DQ1" s="4" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="DR1" s="4" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="DS1" s="4" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="DT1" s="4" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="DU1" s="4" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="DV1" s="4" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="DW1" s="4" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="DX1" s="4" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="DY1" s="4" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="DZ1" s="4" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="EA1" s="4" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="EB1" s="4" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="EC1" s="4" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="ED1" s="4" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="EE1" s="4" t="s">
-        <v>755</v>
+        <v>752</v>
       </c>
       <c r="EF1" s="4" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="EG1" s="4" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="EH1" s="4" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="EI1" s="4" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="EJ1" s="4" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="EK1" s="4" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="EL1" s="4" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="EM1" s="4" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="EN1" s="4" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="2" spans="1:144" ht="90" x14ac:dyDescent="0.25">
@@ -9693,16 +9714,16 @@
         <v>132</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>745</v>
+        <v>785</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>398</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>743</v>
+        <v>514</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>400</v>
@@ -9983,73 +10004,73 @@
         <v>438</v>
       </c>
       <c r="DB2" s="9" t="s">
+        <v>737</v>
+      </c>
+      <c r="DC2" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="DD2" s="9" t="s">
         <v>739</v>
       </c>
-      <c r="DC2" s="9" t="s">
-        <v>742</v>
-      </c>
-      <c r="DD2" s="9" t="s">
-        <v>741</v>
-      </c>
       <c r="DE2" s="9" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="DF2" s="35" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="DG2" s="9" t="s">
         <v>440</v>
       </c>
       <c r="DH2" s="9" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="DI2" s="9" t="s">
         <v>441</v>
       </c>
       <c r="DJ2" s="9" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="DK2" s="66" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="DL2" s="66" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="DM2" s="66" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="DN2" s="65" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="DO2" s="65" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="DP2" s="65" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="DQ2" s="65" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="DR2" s="65" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="DS2" s="65" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="DT2" s="65" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="DU2" s="65" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="DV2" s="65" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="DW2" s="65" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="DX2" s="65" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="DY2" s="65" t="s">
         <v>404</v>
@@ -10061,43 +10082,43 @@
         <v>404</v>
       </c>
       <c r="EB2" s="2" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="EC2" s="2" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="ED2" s="37" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="EE2" s="37" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="EF2" s="37" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="EG2" s="37" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="EH2" s="37" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="EI2" s="37" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="EJ2" s="37" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="EK2" s="37" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="EL2" s="61" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="EM2" s="61" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="EN2" s="61" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="3" spans="1:144" ht="90" x14ac:dyDescent="0.25">
@@ -12066,19 +12087,19 @@
     </row>
     <row r="9" spans="1:144" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>398</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>743</v>
+        <v>782</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>400</v>
@@ -12210,7 +12231,7 @@
         <v>199</v>
       </c>
       <c r="AY9" s="28" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
       <c r="AZ9" s="28" t="s">
         <v>30</v>
@@ -12332,7 +12353,7 @@
         <v>200</v>
       </c>
       <c r="CS9" s="9" t="s">
-        <v>162</v>
+        <v>783</v>
       </c>
       <c r="CT9" s="9" t="s">
         <v>53</v>
@@ -12359,73 +12380,73 @@
         <v>438</v>
       </c>
       <c r="DB9" s="9" t="s">
+        <v>737</v>
+      </c>
+      <c r="DC9" s="9" t="s">
+        <v>740</v>
+      </c>
+      <c r="DD9" s="9" t="s">
         <v>739</v>
       </c>
-      <c r="DC9" s="9" t="s">
-        <v>742</v>
-      </c>
-      <c r="DD9" s="9" t="s">
-        <v>741</v>
-      </c>
       <c r="DE9" s="9" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="DF9" s="35" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="DG9" s="9" t="s">
         <v>440</v>
       </c>
       <c r="DH9" s="9" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="DI9" s="9" t="s">
         <v>441</v>
       </c>
       <c r="DJ9" s="9" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="DK9" s="66" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="DL9" s="66" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="DM9" s="66" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="DN9" s="65" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="DO9" s="65" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="DP9" s="65" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="DQ9" s="65" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="DR9" s="65" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="DS9" s="65" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="DT9" s="65" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="DU9" s="65" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="DV9" s="65" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="DW9" s="65" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="DX9" s="65" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="DY9" s="65" t="s">
         <v>404</v>
@@ -12437,43 +12458,43 @@
         <v>404</v>
       </c>
       <c r="EB9" s="2" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="EC9" s="2" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="ED9" s="37" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="EE9" s="37" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="EF9" s="37" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="EG9" s="37" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="EH9" s="37" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="EI9" s="37" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="EJ9" s="37" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="EK9" s="37" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="EL9" s="61" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="EM9" s="61" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="EN9" s="61" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
     </row>
     <row r="10" spans="1:144" x14ac:dyDescent="0.25">
@@ -13827,7 +13848,7 @@
   <dimension ref="A1:BG12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="BH1" sqref="BH1:BL2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14040,16 +14061,16 @@
         <v>453</v>
       </c>
       <c r="BD1" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="BF1" s="1" t="s">
         <v>560</v>
       </c>
-      <c r="BE1" s="1" t="s">
-        <v>561</v>
-      </c>
-      <c r="BF1" s="1" t="s">
-        <v>562</v>
-      </c>
       <c r="BG1" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="2" spans="1:59" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -14700,7 +14721,7 @@
         <v>465</v>
       </c>
       <c r="BB5" s="9" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="BC5" s="9"/>
       <c r="BD5" s="9"/>
@@ -14878,7 +14899,7 @@
         <v>458</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>472</v>
+        <v>781</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>230</v>
@@ -15043,7 +15064,7 @@
         <v>459</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>473</v>
+        <v>784</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>230</v>
@@ -15055,7 +15076,7 @@
         <v>230</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>134</v>
+        <v>776</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>230</v>
@@ -15066,8 +15087,8 @@
       <c r="I8" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="J8" s="9" t="s">
-        <v>134</v>
+      <c r="J8" s="28" t="s">
+        <v>776</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>230</v>
@@ -15120,8 +15141,8 @@
       <c r="AA8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AB8" s="9">
-        <v>1113332</v>
+      <c r="AB8" s="66" t="s">
+        <v>777</v>
       </c>
       <c r="AC8" s="9">
         <v>23564589</v>
@@ -15173,11 +15194,11 @@
       <c r="AT8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AU8" s="9">
-        <v>5431267812</v>
+      <c r="AU8" s="9" t="s">
+        <v>778</v>
       </c>
       <c r="AV8" s="9" t="s">
-        <v>376</v>
+        <v>779</v>
       </c>
       <c r="AW8" s="9" t="s">
         <v>377</v>
@@ -15195,7 +15216,7 @@
         <v>465</v>
       </c>
       <c r="BB8" s="9" t="s">
-        <v>455</v>
+        <v>780</v>
       </c>
       <c r="BC8" s="9"/>
       <c r="BD8" s="9"/>
@@ -15208,7 +15229,7 @@
         <v>460</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>230</v>
@@ -15371,7 +15392,7 @@
         <v>461</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>443</v>
@@ -15534,7 +15555,7 @@
         <v>466</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>230</v>
@@ -15696,10 +15717,10 @@
     </row>
     <row r="12" spans="1:59" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>230</v>
@@ -15855,7 +15876,7 @@
       </c>
       <c r="BC12" s="9"/>
       <c r="BD12" s="9" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="BE12" s="9" t="s">
         <v>230</v>

</xml_diff>

<commit_message>
test data url changed
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3167" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3167" uniqueCount="754">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -2145,9 +2145,6 @@
     <t>Swap</t>
   </si>
   <si>
-    <t>http://ech-10-168-131-92.mastercard.int:25003/integratedIssuing-customerPortal/mtps/app/Login?0</t>
-  </si>
-  <si>
     <t>MDKStatus</t>
   </si>
   <si>
@@ -2271,9 +2268,6 @@
     <t>LoadsAfterKYC</t>
   </si>
   <si>
-    <t>http://ech-10-168-131-92.mastercard.int:25003/integratedIssuing-customerPortal/mpts/app/Login?0</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
@@ -2296,6 +2290,9 @@
   </si>
   <si>
     <t>adaptiveAuth_debit</t>
+  </si>
+  <si>
+    <t>http://ech-10-168-131-18.mastercard.int:25003/integratedIssuing-customerPortal/mpts/app/Login?0</t>
   </si>
 </sst>
 </file>
@@ -9162,8 +9159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EP178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BN7" workbookViewId="0">
-      <selection activeCell="CH9" sqref="CH9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9385,7 +9382,7 @@
         <v>70</v>
       </c>
       <c r="BP1" s="4" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="BQ1" s="4" t="s">
         <v>73</v>
@@ -9394,10 +9391,10 @@
         <v>74</v>
       </c>
       <c r="BS1" s="4" t="s">
+        <v>743</v>
+      </c>
+      <c r="BT1" s="4" t="s">
         <v>744</v>
-      </c>
-      <c r="BT1" s="4" t="s">
-        <v>745</v>
       </c>
       <c r="BU1" s="4" t="s">
         <v>83</v>
@@ -9529,97 +9526,97 @@
         <v>394</v>
       </c>
       <c r="DL1" s="4" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="DM1" s="4" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="DN1" s="4" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="DO1" s="4" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="DP1" s="4" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="DQ1" s="4" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="DR1" s="4" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="DS1" s="4" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="DT1" s="4" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="DU1" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="DV1" s="4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="DW1" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="DX1" s="4" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="DY1" s="4" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="DZ1" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="EA1" s="4" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="EB1" s="4" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="EC1" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="ED1" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="EE1" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="EF1" s="4" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="EG1" s="4" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="EH1" s="4" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="EI1" s="4" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="EJ1" s="4" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="EK1" s="4" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="EL1" s="4" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="EM1" s="4" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="EN1" s="4" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="EO1" s="4" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="EP1" s="4" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="2" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
@@ -9627,7 +9624,7 @@
         <v>132</v>
       </c>
       <c r="B2" s="66" t="s">
-        <v>746</v>
+        <v>753</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>489</v>
@@ -9713,10 +9710,10 @@
         <v>36</v>
       </c>
       <c r="AF2" s="28" t="s">
+        <v>737</v>
+      </c>
+      <c r="AG2" s="28" t="s">
         <v>738</v>
-      </c>
-      <c r="AG2" s="28" t="s">
-        <v>739</v>
       </c>
       <c r="AH2" s="28" t="s">
         <v>10</v>
@@ -9752,13 +9749,13 @@
         <v>325</v>
       </c>
       <c r="AS2" s="28" t="s">
+        <v>739</v>
+      </c>
+      <c r="AT2" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="AT2" s="28" t="s">
+      <c r="AU2" s="28" t="s">
         <v>741</v>
-      </c>
-      <c r="AU2" s="28" t="s">
-        <v>742</v>
       </c>
       <c r="AV2" s="28" t="s">
         <v>29</v>
@@ -9817,7 +9814,7 @@
         <v>71</v>
       </c>
       <c r="BP2" s="9" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="BQ2" s="28" t="s">
         <v>373</v>
@@ -9861,7 +9858,7 @@
       </c>
       <c r="CG2" s="9"/>
       <c r="CH2" s="28" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="CI2" s="28"/>
       <c r="CJ2" s="28" t="s">
@@ -10040,10 +10037,10 @@
     </row>
     <row r="3" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B3" s="66" t="s">
-        <v>746</v>
+        <v>753</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>489</v>
@@ -10129,10 +10126,10 @@
         <v>36</v>
       </c>
       <c r="AF3" s="28" t="s">
+        <v>737</v>
+      </c>
+      <c r="AG3" s="28" t="s">
         <v>738</v>
-      </c>
-      <c r="AG3" s="28" t="s">
-        <v>739</v>
       </c>
       <c r="AH3" s="28" t="s">
         <v>10</v>
@@ -10168,13 +10165,13 @@
         <v>325</v>
       </c>
       <c r="AS3" s="28" t="s">
+        <v>739</v>
+      </c>
+      <c r="AT3" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="AT3" s="28" t="s">
+      <c r="AU3" s="28" t="s">
         <v>741</v>
-      </c>
-      <c r="AU3" s="28" t="s">
-        <v>742</v>
       </c>
       <c r="AV3" s="28" t="s">
         <v>29</v>
@@ -10233,7 +10230,7 @@
         <v>71</v>
       </c>
       <c r="BP3" s="9" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="BQ3" s="28" t="s">
         <v>373</v>
@@ -10277,7 +10274,7 @@
       </c>
       <c r="CG3" s="9"/>
       <c r="CH3" s="28" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="CI3" s="28"/>
       <c r="CJ3" s="28" t="s">
@@ -10385,7 +10382,7 @@
         <v>140</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>746</v>
+        <v>753</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>489</v>
@@ -10471,10 +10468,10 @@
         <v>36</v>
       </c>
       <c r="AF4" s="28" t="s">
+        <v>737</v>
+      </c>
+      <c r="AG4" s="28" t="s">
         <v>738</v>
-      </c>
-      <c r="AG4" s="28" t="s">
-        <v>739</v>
       </c>
       <c r="AH4" s="28" t="s">
         <v>10</v>
@@ -10510,13 +10507,13 @@
         <v>325</v>
       </c>
       <c r="AS4" s="28" t="s">
+        <v>739</v>
+      </c>
+      <c r="AT4" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="AT4" s="28" t="s">
+      <c r="AU4" s="28" t="s">
         <v>741</v>
-      </c>
-      <c r="AU4" s="28" t="s">
-        <v>742</v>
       </c>
       <c r="AV4" s="28" t="s">
         <v>29</v>
@@ -10575,7 +10572,7 @@
         <v>71</v>
       </c>
       <c r="BP4" s="9" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="BQ4" s="28" t="s">
         <v>373</v>
@@ -10603,7 +10600,7 @@
         <v>171</v>
       </c>
       <c r="CB4" s="9" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="CC4" s="9" t="s">
         <v>48</v>
@@ -10617,7 +10614,7 @@
       <c r="CF4" s="28"/>
       <c r="CG4" s="9"/>
       <c r="CH4" s="28" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="CI4" s="28"/>
       <c r="CJ4" s="28" t="s">
@@ -10706,10 +10703,10 @@
     </row>
     <row r="5" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B5" s="66" t="s">
-        <v>746</v>
+        <v>753</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>489</v>
@@ -10795,10 +10792,10 @@
         <v>36</v>
       </c>
       <c r="AF5" s="28" t="s">
+        <v>737</v>
+      </c>
+      <c r="AG5" s="28" t="s">
         <v>738</v>
-      </c>
-      <c r="AG5" s="28" t="s">
-        <v>739</v>
       </c>
       <c r="AH5" s="28" t="s">
         <v>10</v>
@@ -10834,13 +10831,13 @@
         <v>325</v>
       </c>
       <c r="AS5" s="28" t="s">
+        <v>739</v>
+      </c>
+      <c r="AT5" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="AT5" s="28" t="s">
+      <c r="AU5" s="28" t="s">
         <v>741</v>
-      </c>
-      <c r="AU5" s="28" t="s">
-        <v>742</v>
       </c>
       <c r="AV5" s="28" t="s">
         <v>29</v>
@@ -10899,7 +10896,7 @@
         <v>71</v>
       </c>
       <c r="BP5" s="9" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="BQ5" s="28" t="s">
         <v>373</v>
@@ -10927,7 +10924,7 @@
         <v>171</v>
       </c>
       <c r="CB5" s="9" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="CC5" s="9" t="s">
         <v>48</v>
@@ -10941,7 +10938,7 @@
       <c r="CF5" s="28"/>
       <c r="CG5" s="9"/>
       <c r="CH5" s="28" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="CI5" s="28"/>
       <c r="CJ5" s="28" t="s">
@@ -11033,7 +11030,7 @@
         <v>148</v>
       </c>
       <c r="B6" s="66" t="s">
-        <v>746</v>
+        <v>753</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>489</v>
@@ -11119,10 +11116,10 @@
         <v>36</v>
       </c>
       <c r="AF6" s="28" t="s">
+        <v>737</v>
+      </c>
+      <c r="AG6" s="28" t="s">
         <v>738</v>
-      </c>
-      <c r="AG6" s="28" t="s">
-        <v>739</v>
       </c>
       <c r="AH6" s="28" t="s">
         <v>10</v>
@@ -11158,13 +11155,13 @@
         <v>325</v>
       </c>
       <c r="AS6" s="28" t="s">
+        <v>739</v>
+      </c>
+      <c r="AT6" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="AT6" s="28" t="s">
+      <c r="AU6" s="28" t="s">
         <v>741</v>
-      </c>
-      <c r="AU6" s="28" t="s">
-        <v>742</v>
       </c>
       <c r="AV6" s="28" t="s">
         <v>29</v>
@@ -11223,7 +11220,7 @@
         <v>71</v>
       </c>
       <c r="BP6" s="9" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="BQ6" s="28" t="s">
         <v>373</v>
@@ -11265,7 +11262,7 @@
       <c r="CF6" s="28"/>
       <c r="CG6" s="9"/>
       <c r="CH6" s="28" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="CI6" s="28"/>
       <c r="CJ6" s="28" t="s">
@@ -11354,10 +11351,10 @@
     </row>
     <row r="7" spans="1:146" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
+        <v>751</v>
+      </c>
+      <c r="B7" s="66" t="s">
         <v>753</v>
-      </c>
-      <c r="B7" s="66" t="s">
-        <v>746</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>489</v>
@@ -11443,10 +11440,10 @@
         <v>36</v>
       </c>
       <c r="AF7" s="28" t="s">
+        <v>737</v>
+      </c>
+      <c r="AG7" s="28" t="s">
         <v>738</v>
-      </c>
-      <c r="AG7" s="28" t="s">
-        <v>739</v>
       </c>
       <c r="AH7" s="28" t="s">
         <v>10</v>
@@ -11482,13 +11479,13 @@
         <v>325</v>
       </c>
       <c r="AS7" s="28" t="s">
+        <v>739</v>
+      </c>
+      <c r="AT7" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="AT7" s="28" t="s">
+      <c r="AU7" s="28" t="s">
         <v>741</v>
-      </c>
-      <c r="AU7" s="28" t="s">
-        <v>742</v>
       </c>
       <c r="AV7" s="28" t="s">
         <v>29</v>
@@ -11547,7 +11544,7 @@
         <v>71</v>
       </c>
       <c r="BP7" s="9" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="BQ7" s="28" t="s">
         <v>373</v>
@@ -11589,7 +11586,7 @@
       <c r="CF7" s="28"/>
       <c r="CG7" s="9"/>
       <c r="CH7" s="28" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="CI7" s="28"/>
       <c r="CJ7" s="28" t="s">
@@ -11681,7 +11678,7 @@
         <v>152</v>
       </c>
       <c r="B8" s="66" t="s">
-        <v>746</v>
+        <v>753</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>489</v>
@@ -11767,10 +11764,10 @@
         <v>36</v>
       </c>
       <c r="AF8" s="28" t="s">
+        <v>737</v>
+      </c>
+      <c r="AG8" s="28" t="s">
         <v>738</v>
-      </c>
-      <c r="AG8" s="28" t="s">
-        <v>739</v>
       </c>
       <c r="AH8" s="28" t="s">
         <v>10</v>
@@ -11806,13 +11803,13 @@
         <v>325</v>
       </c>
       <c r="AS8" s="28" t="s">
+        <v>739</v>
+      </c>
+      <c r="AT8" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="AT8" s="28" t="s">
+      <c r="AU8" s="28" t="s">
         <v>741</v>
-      </c>
-      <c r="AU8" s="28" t="s">
-        <v>742</v>
       </c>
       <c r="AV8" s="28" t="s">
         <v>29</v>
@@ -11871,7 +11868,7 @@
         <v>71</v>
       </c>
       <c r="BP8" s="9" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="BQ8" s="28" t="s">
         <v>373</v>
@@ -11899,7 +11896,7 @@
         <v>171</v>
       </c>
       <c r="CB8" s="9" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="CC8" s="9" t="s">
         <v>48</v>
@@ -11913,7 +11910,7 @@
       <c r="CF8" s="28"/>
       <c r="CG8" s="9"/>
       <c r="CH8" s="28" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="CI8" s="28"/>
       <c r="CJ8" s="28" t="s">
@@ -12002,10 +11999,10 @@
     </row>
     <row r="9" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B9" s="66" t="s">
-        <v>746</v>
+        <v>753</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>489</v>
@@ -12091,10 +12088,10 @@
         <v>36</v>
       </c>
       <c r="AF9" s="28" t="s">
+        <v>737</v>
+      </c>
+      <c r="AG9" s="28" t="s">
         <v>738</v>
-      </c>
-      <c r="AG9" s="28" t="s">
-        <v>739</v>
       </c>
       <c r="AH9" s="28" t="s">
         <v>10</v>
@@ -12130,13 +12127,13 @@
         <v>325</v>
       </c>
       <c r="AS9" s="28" t="s">
+        <v>739</v>
+      </c>
+      <c r="AT9" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="AT9" s="28" t="s">
+      <c r="AU9" s="28" t="s">
         <v>741</v>
-      </c>
-      <c r="AU9" s="28" t="s">
-        <v>742</v>
       </c>
       <c r="AV9" s="28" t="s">
         <v>29</v>
@@ -12195,7 +12192,7 @@
         <v>71</v>
       </c>
       <c r="BP9" s="9" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="BQ9" s="28" t="s">
         <v>373</v>
@@ -12418,10 +12415,10 @@
     </row>
     <row r="10" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>737</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>704</v>
+        <v>736</v>
+      </c>
+      <c r="B10" s="66" t="s">
+        <v>753</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>703</v>
@@ -12562,7 +12559,7 @@
         <v>175</v>
       </c>
       <c r="AY10" s="28" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="AZ10" s="28" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
issuer bin changed for debit
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3865" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3819" uniqueCount="796">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -2286,9 +2286,6 @@
     <t>HDFCVendor01 [VEN5211]</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>588765</t>
   </si>
   <si>
@@ -2328,9 +2325,6 @@
     <t>NFCEmvProgram</t>
   </si>
   <si>
-    <t>1E+12</t>
-  </si>
-  <si>
     <t>NFC Emv Device plan</t>
   </si>
   <si>
@@ -2419,6 +2413,12 @@
   </si>
   <si>
     <t>adaptiveAuth_debit</t>
+  </si>
+  <si>
+    <t>543210</t>
+  </si>
+  <si>
+    <t>235689</t>
   </si>
 </sst>
 </file>
@@ -2487,7 +2487,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -2549,19 +2549,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -2663,8 +2650,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -2681,14 +2667,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
@@ -2706,6 +2692,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -4880,52 +4869,52 @@
       <c r="DO1" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="DP1" s="36" t="s">
+      <c r="DP1" s="35" t="s">
         <v>452</v>
       </c>
-      <c r="DQ1" s="36" t="s">
+      <c r="DQ1" s="35" t="s">
         <v>453</v>
       </c>
-      <c r="DR1" s="36" t="s">
+      <c r="DR1" s="35" t="s">
         <v>454</v>
       </c>
-      <c r="DS1" s="36" t="s">
+      <c r="DS1" s="35" t="s">
         <v>455</v>
       </c>
-      <c r="DT1" s="36" t="s">
+      <c r="DT1" s="35" t="s">
         <v>456</v>
       </c>
-      <c r="DU1" s="36" t="s">
+      <c r="DU1" s="35" t="s">
         <v>457</v>
       </c>
-      <c r="DV1" s="36" t="s">
+      <c r="DV1" s="35" t="s">
         <v>458</v>
       </c>
-      <c r="DW1" s="36" t="s">
+      <c r="DW1" s="35" t="s">
         <v>459</v>
       </c>
-      <c r="DX1" s="36" t="s">
+      <c r="DX1" s="35" t="s">
         <v>460</v>
       </c>
-      <c r="DY1" s="36" t="s">
+      <c r="DY1" s="35" t="s">
         <v>461</v>
       </c>
-      <c r="DZ1" s="36" t="s">
+      <c r="DZ1" s="35" t="s">
         <v>462</v>
       </c>
-      <c r="EA1" s="36" t="s">
+      <c r="EA1" s="35" t="s">
         <v>463</v>
       </c>
-      <c r="EB1" s="36" t="s">
+      <c r="EB1" s="35" t="s">
         <v>464</v>
       </c>
-      <c r="EC1" s="36" t="s">
+      <c r="EC1" s="35" t="s">
         <v>465</v>
       </c>
-      <c r="ED1" s="36" t="s">
+      <c r="ED1" s="35" t="s">
         <v>466</v>
       </c>
-      <c r="EE1" s="36" t="s">
+      <c r="EE1" s="35" t="s">
         <v>467</v>
       </c>
     </row>
@@ -4939,7 +4928,7 @@
       <c r="C2" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>470</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -4960,34 +4949,34 @@
       <c r="J2" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="37" t="s">
         <v>476</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="L2" s="37" t="s">
         <v>477</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="M2" s="37" t="s">
         <v>478</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="N2" s="38" t="s">
         <v>479</v>
       </c>
-      <c r="O2" s="39" t="s">
+      <c r="O2" s="38" t="s">
         <v>480</v>
       </c>
-      <c r="P2" s="39" t="s">
+      <c r="P2" s="38" t="s">
         <v>480</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="R2" s="39" t="s">
+      <c r="R2" s="38" t="s">
         <v>482</v>
       </c>
-      <c r="S2" s="39" t="s">
+      <c r="S2" s="38" t="s">
         <v>483</v>
       </c>
-      <c r="T2" s="39" t="s">
+      <c r="T2" s="38" t="s">
         <v>484</v>
       </c>
       <c r="U2" s="11">
@@ -5008,8 +4997,8 @@
       <c r="Z2" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
       <c r="AC2" s="12"/>
       <c r="AD2" s="12" t="s">
         <v>45</v>
@@ -5127,7 +5116,7 @@
       <c r="BQ2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="BR2" s="41" t="s">
+      <c r="BR2" s="40" t="s">
         <v>370</v>
       </c>
       <c r="BS2" s="12" t="s">
@@ -5145,7 +5134,7 @@
       <c r="BW2" t="s">
         <v>493</v>
       </c>
-      <c r="BX2" s="42"/>
+      <c r="BX2" s="41"/>
       <c r="BY2" s="12" t="s">
         <v>142</v>
       </c>
@@ -5171,18 +5160,18 @@
         <v>71</v>
       </c>
       <c r="CG2" s="12"/>
-      <c r="CH2" s="42" t="s">
+      <c r="CH2" s="41" t="s">
         <v>369</v>
       </c>
-      <c r="CI2" s="42" t="s">
+      <c r="CI2" s="41" t="s">
         <v>371</v>
       </c>
-      <c r="CJ2" s="40"/>
-      <c r="CK2" s="40"/>
+      <c r="CJ2" s="39"/>
+      <c r="CK2" s="39"/>
       <c r="CL2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="CM2" s="42" t="s">
+      <c r="CM2" s="41" t="s">
         <v>495</v>
       </c>
       <c r="CN2" s="12" t="s">
@@ -5191,7 +5180,7 @@
       <c r="CO2" s="11" t="s">
         <v>491</v>
       </c>
-      <c r="CP2" s="40" t="s">
+      <c r="CP2" s="39" t="s">
         <v>321</v>
       </c>
       <c r="CQ2" s="11" t="s">
@@ -5205,22 +5194,22 @@
       </c>
       <c r="CT2" s="11"/>
       <c r="CU2" s="11"/>
-      <c r="CV2" s="40" t="s">
+      <c r="CV2" s="39" t="s">
         <v>480</v>
       </c>
       <c r="CW2" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="CX2" s="40" t="s">
+      <c r="CX2" s="39" t="s">
         <v>373</v>
       </c>
-      <c r="CY2" s="40" t="s">
+      <c r="CY2" s="39" t="s">
         <v>369</v>
       </c>
-      <c r="CZ2" s="40" t="s">
+      <c r="CZ2" s="39" t="s">
         <v>374</v>
       </c>
-      <c r="DA2" s="40" t="s">
+      <c r="DA2" s="39" t="s">
         <v>375</v>
       </c>
       <c r="DB2" s="12" t="s">
@@ -5257,52 +5246,52 @@
       <c r="DO2" s="11" t="s">
         <v>499</v>
       </c>
-      <c r="DP2" s="43" t="s">
+      <c r="DP2" s="42" t="s">
         <v>500</v>
       </c>
-      <c r="DQ2" s="43" t="s">
+      <c r="DQ2" s="42" t="s">
         <v>501</v>
       </c>
-      <c r="DR2" s="43" t="s">
+      <c r="DR2" s="42" t="s">
         <v>502</v>
       </c>
-      <c r="DS2" s="44" t="s">
+      <c r="DS2" s="43" t="s">
         <v>503</v>
       </c>
-      <c r="DT2" s="44" t="s">
+      <c r="DT2" s="43" t="s">
         <v>369</v>
       </c>
-      <c r="DU2" s="44" t="s">
+      <c r="DU2" s="43" t="s">
         <v>504</v>
       </c>
-      <c r="DV2" s="43" t="s">
+      <c r="DV2" s="42" t="s">
         <v>505</v>
       </c>
-      <c r="DW2" s="43" t="s">
+      <c r="DW2" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="DX2" s="44" t="s">
+      <c r="DX2" s="43" t="s">
         <v>368</v>
       </c>
-      <c r="DY2" s="44" t="s">
+      <c r="DY2" s="43" t="s">
         <v>506</v>
       </c>
-      <c r="DZ2" s="44" t="s">
+      <c r="DZ2" s="43" t="s">
         <v>507</v>
       </c>
-      <c r="EA2" s="44" t="s">
+      <c r="EA2" s="43" t="s">
         <v>478</v>
       </c>
-      <c r="EB2" s="44" t="s">
+      <c r="EB2" s="43" t="s">
         <v>507</v>
       </c>
-      <c r="EC2" s="44" t="s">
+      <c r="EC2" s="43" t="s">
         <v>508</v>
       </c>
-      <c r="ED2" s="44" t="s">
+      <c r="ED2" s="43" t="s">
         <v>509</v>
       </c>
-      <c r="EE2" s="43" t="s">
+      <c r="EE2" s="42" t="s">
         <v>510</v>
       </c>
     </row>
@@ -5684,76 +5673,76 @@
       <c r="DO1" s="4" t="s">
         <v>451</v>
       </c>
-      <c r="DP1" s="36" t="s">
+      <c r="DP1" s="35" t="s">
         <v>452</v>
       </c>
-      <c r="DQ1" s="36" t="s">
+      <c r="DQ1" s="35" t="s">
         <v>453</v>
       </c>
-      <c r="DR1" s="36" t="s">
+      <c r="DR1" s="35" t="s">
         <v>454</v>
       </c>
-      <c r="DS1" s="36" t="s">
+      <c r="DS1" s="35" t="s">
         <v>455</v>
       </c>
-      <c r="DT1" s="36" t="s">
+      <c r="DT1" s="35" t="s">
         <v>456</v>
       </c>
-      <c r="DU1" s="36" t="s">
+      <c r="DU1" s="35" t="s">
         <v>457</v>
       </c>
-      <c r="DV1" s="36" t="s">
+      <c r="DV1" s="35" t="s">
         <v>458</v>
       </c>
-      <c r="DW1" s="36" t="s">
+      <c r="DW1" s="35" t="s">
         <v>459</v>
       </c>
-      <c r="DX1" s="36" t="s">
+      <c r="DX1" s="35" t="s">
         <v>460</v>
       </c>
-      <c r="DY1" s="36" t="s">
+      <c r="DY1" s="35" t="s">
         <v>461</v>
       </c>
-      <c r="DZ1" s="36" t="s">
+      <c r="DZ1" s="35" t="s">
         <v>462</v>
       </c>
-      <c r="EA1" s="36" t="s">
+      <c r="EA1" s="35" t="s">
         <v>463</v>
       </c>
-      <c r="EB1" s="36" t="s">
+      <c r="EB1" s="35" t="s">
         <v>464</v>
       </c>
-      <c r="EC1" s="36" t="s">
+      <c r="EC1" s="35" t="s">
         <v>465</v>
       </c>
-      <c r="ED1" s="36" t="s">
+      <c r="ED1" s="35" t="s">
         <v>650</v>
       </c>
-      <c r="EE1" s="36" t="s">
+      <c r="EE1" s="35" t="s">
         <v>651</v>
       </c>
-      <c r="EF1" s="36" t="s">
+      <c r="EF1" s="35" t="s">
         <v>466</v>
       </c>
-      <c r="EG1" s="36" t="s">
+      <c r="EG1" s="35" t="s">
         <v>652</v>
       </c>
-      <c r="EH1" s="36" t="s">
+      <c r="EH1" s="35" t="s">
         <v>653</v>
       </c>
-      <c r="EI1" s="36" t="s">
+      <c r="EI1" s="35" t="s">
         <v>654</v>
       </c>
-      <c r="EJ1" s="36" t="s">
+      <c r="EJ1" s="35" t="s">
         <v>655</v>
       </c>
-      <c r="EK1" s="36" t="s">
+      <c r="EK1" s="35" t="s">
         <v>656</v>
       </c>
-      <c r="EL1" s="36" t="s">
+      <c r="EL1" s="35" t="s">
         <v>657</v>
       </c>
-      <c r="EM1" s="36" t="s">
+      <c r="EM1" s="35" t="s">
         <v>467</v>
       </c>
     </row>
@@ -5767,7 +5756,7 @@
       <c r="C2" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>470</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -5788,34 +5777,34 @@
       <c r="J2" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="37" t="s">
         <v>476</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="L2" s="37" t="s">
         <v>477</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="M2" s="37" t="s">
         <v>478</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="N2" s="38" t="s">
         <v>479</v>
       </c>
-      <c r="O2" s="39" t="s">
+      <c r="O2" s="38" t="s">
         <v>480</v>
       </c>
-      <c r="P2" s="39" t="s">
+      <c r="P2" s="38" t="s">
         <v>480</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="R2" s="39" t="s">
+      <c r="R2" s="38" t="s">
         <v>482</v>
       </c>
-      <c r="S2" s="39" t="s">
+      <c r="S2" s="38" t="s">
         <v>483</v>
       </c>
-      <c r="T2" s="39" t="s">
+      <c r="T2" s="38" t="s">
         <v>484</v>
       </c>
       <c r="U2" s="11">
@@ -5836,8 +5825,8 @@
       <c r="Z2" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="AA2" s="40"/>
-      <c r="AB2" s="40"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
       <c r="AC2" s="12"/>
       <c r="AD2" s="12" t="s">
         <v>45</v>
@@ -5955,7 +5944,7 @@
       <c r="BQ2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="BR2" s="41" t="s">
+      <c r="BR2" s="40" t="s">
         <v>370</v>
       </c>
       <c r="BS2" s="12" t="s">
@@ -5973,7 +5962,7 @@
       <c r="BW2" t="s">
         <v>493</v>
       </c>
-      <c r="BX2" s="42"/>
+      <c r="BX2" s="41"/>
       <c r="BY2" s="12" t="s">
         <v>142</v>
       </c>
@@ -5999,18 +5988,18 @@
         <v>71</v>
       </c>
       <c r="CG2" s="12"/>
-      <c r="CH2" s="42" t="s">
+      <c r="CH2" s="41" t="s">
         <v>369</v>
       </c>
-      <c r="CI2" s="42" t="s">
+      <c r="CI2" s="41" t="s">
         <v>371</v>
       </c>
-      <c r="CJ2" s="40"/>
-      <c r="CK2" s="40"/>
+      <c r="CJ2" s="39"/>
+      <c r="CK2" s="39"/>
       <c r="CL2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="CM2" s="42" t="s">
+      <c r="CM2" s="41" t="s">
         <v>495</v>
       </c>
       <c r="CN2" s="12" t="s">
@@ -6019,7 +6008,7 @@
       <c r="CO2" s="11" t="s">
         <v>491</v>
       </c>
-      <c r="CP2" s="40" t="s">
+      <c r="CP2" s="39" t="s">
         <v>321</v>
       </c>
       <c r="CQ2" s="11" t="s">
@@ -6033,22 +6022,22 @@
       </c>
       <c r="CT2" s="11"/>
       <c r="CU2" s="11"/>
-      <c r="CV2" s="40" t="s">
+      <c r="CV2" s="39" t="s">
         <v>480</v>
       </c>
       <c r="CW2" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="CX2" s="40" t="s">
+      <c r="CX2" s="39" t="s">
         <v>373</v>
       </c>
-      <c r="CY2" s="40" t="s">
+      <c r="CY2" s="39" t="s">
         <v>369</v>
       </c>
-      <c r="CZ2" s="40" t="s">
+      <c r="CZ2" s="39" t="s">
         <v>374</v>
       </c>
-      <c r="DA2" s="40" t="s">
+      <c r="DA2" s="39" t="s">
         <v>375</v>
       </c>
       <c r="DB2" s="12" t="s">
@@ -6085,60 +6074,60 @@
       <c r="DO2" s="11" t="s">
         <v>499</v>
       </c>
-      <c r="DP2" s="43" t="s">
+      <c r="DP2" s="42" t="s">
         <v>500</v>
       </c>
-      <c r="DQ2" s="43" t="s">
+      <c r="DQ2" s="42" t="s">
         <v>501</v>
       </c>
-      <c r="DR2" s="43" t="s">
+      <c r="DR2" s="42" t="s">
         <v>502</v>
       </c>
-      <c r="DS2" s="44" t="s">
+      <c r="DS2" s="43" t="s">
         <v>503</v>
       </c>
-      <c r="DT2" s="44" t="s">
+      <c r="DT2" s="43" t="s">
         <v>369</v>
       </c>
-      <c r="DU2" s="44" t="s">
+      <c r="DU2" s="43" t="s">
         <v>504</v>
       </c>
-      <c r="DV2" s="43" t="s">
+      <c r="DV2" s="42" t="s">
         <v>505</v>
       </c>
-      <c r="DW2" s="43" t="s">
+      <c r="DW2" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="DX2" s="44" t="s">
+      <c r="DX2" s="43" t="s">
         <v>368</v>
       </c>
-      <c r="DY2" s="44" t="s">
+      <c r="DY2" s="43" t="s">
         <v>506</v>
       </c>
-      <c r="DZ2" s="44" t="s">
+      <c r="DZ2" s="43" t="s">
         <v>507</v>
       </c>
-      <c r="EA2" s="44" t="s">
+      <c r="EA2" s="43" t="s">
         <v>478</v>
       </c>
-      <c r="EB2" s="44" t="s">
+      <c r="EB2" s="43" t="s">
         <v>507</v>
       </c>
-      <c r="EC2" s="44" t="s">
+      <c r="EC2" s="43" t="s">
         <v>508</v>
       </c>
-      <c r="ED2" s="44"/>
-      <c r="EE2" s="44"/>
-      <c r="EF2" s="44" t="s">
+      <c r="ED2" s="43"/>
+      <c r="EE2" s="43"/>
+      <c r="EF2" s="43" t="s">
         <v>509</v>
       </c>
-      <c r="EG2" s="44"/>
-      <c r="EH2" s="44"/>
-      <c r="EI2" s="44"/>
-      <c r="EJ2" s="44"/>
-      <c r="EK2" s="44"/>
-      <c r="EL2" s="44"/>
-      <c r="EM2" s="43" t="s">
+      <c r="EG2" s="43"/>
+      <c r="EH2" s="43"/>
+      <c r="EI2" s="43"/>
+      <c r="EJ2" s="43"/>
+      <c r="EK2" s="43"/>
+      <c r="EL2" s="43"/>
+      <c r="EM2" s="42" t="s">
         <v>510</v>
       </c>
     </row>
@@ -6152,7 +6141,7 @@
       <c r="C3" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="36" t="s">
         <v>660</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -6173,34 +6162,34 @@
       <c r="J3" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="37" t="s">
         <v>476</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="37" t="s">
         <v>477</v>
       </c>
-      <c r="M3" s="38" t="s">
+      <c r="M3" s="37" t="s">
         <v>478</v>
       </c>
-      <c r="N3" s="39" t="s">
+      <c r="N3" s="38" t="s">
         <v>479</v>
       </c>
-      <c r="O3" s="39" t="s">
+      <c r="O3" s="38" t="s">
         <v>480</v>
       </c>
-      <c r="P3" s="39" t="s">
+      <c r="P3" s="38" t="s">
         <v>480</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="R3" s="39" t="s">
+      <c r="R3" s="38" t="s">
         <v>482</v>
       </c>
-      <c r="S3" s="39" t="s">
+      <c r="S3" s="38" t="s">
         <v>355</v>
       </c>
-      <c r="T3" s="39" t="s">
+      <c r="T3" s="38" t="s">
         <v>484</v>
       </c>
       <c r="U3" s="11">
@@ -6221,8 +6210,8 @@
       <c r="Z3" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="AA3" s="40"/>
-      <c r="AB3" s="40"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
       <c r="AC3" s="12"/>
       <c r="AD3" s="12" t="s">
         <v>45</v>
@@ -6340,7 +6329,7 @@
       <c r="BQ3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="BR3" s="41" t="s">
+      <c r="BR3" s="40" t="s">
         <v>370</v>
       </c>
       <c r="BS3" s="12" t="s">
@@ -6358,7 +6347,7 @@
       <c r="BW3" t="s">
         <v>493</v>
       </c>
-      <c r="BX3" s="42"/>
+      <c r="BX3" s="41"/>
       <c r="BY3" s="12" t="s">
         <v>142</v>
       </c>
@@ -6384,18 +6373,18 @@
         <v>71</v>
       </c>
       <c r="CG3" s="12"/>
-      <c r="CH3" s="42" t="s">
+      <c r="CH3" s="41" t="s">
         <v>369</v>
       </c>
-      <c r="CI3" s="42" t="s">
+      <c r="CI3" s="41" t="s">
         <v>371</v>
       </c>
-      <c r="CJ3" s="40"/>
-      <c r="CK3" s="40"/>
+      <c r="CJ3" s="39"/>
+      <c r="CK3" s="39"/>
       <c r="CL3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="CM3" s="42" t="s">
+      <c r="CM3" s="41" t="s">
         <v>495</v>
       </c>
       <c r="CN3" s="12" t="s">
@@ -6404,7 +6393,7 @@
       <c r="CO3" s="11" t="s">
         <v>491</v>
       </c>
-      <c r="CP3" s="40" t="s">
+      <c r="CP3" s="39" t="s">
         <v>321</v>
       </c>
       <c r="CQ3" s="11" t="s">
@@ -6413,27 +6402,27 @@
       <c r="CR3" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="CS3" s="64" t="s">
+      <c r="CS3" s="63" t="s">
         <v>662</v>
       </c>
       <c r="CT3" s="11"/>
       <c r="CU3" s="11"/>
-      <c r="CV3" s="40" t="s">
+      <c r="CV3" s="39" t="s">
         <v>480</v>
       </c>
       <c r="CW3" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="CX3" s="40" t="s">
+      <c r="CX3" s="39" t="s">
         <v>373</v>
       </c>
-      <c r="CY3" s="40" t="s">
+      <c r="CY3" s="39" t="s">
         <v>369</v>
       </c>
-      <c r="CZ3" s="40" t="s">
+      <c r="CZ3" s="39" t="s">
         <v>374</v>
       </c>
-      <c r="DA3" s="40" t="s">
+      <c r="DA3" s="39" t="s">
         <v>375</v>
       </c>
       <c r="DB3" s="12" t="s">
@@ -6470,72 +6459,72 @@
       <c r="DO3" s="11" t="s">
         <v>499</v>
       </c>
-      <c r="DP3" s="43" t="s">
+      <c r="DP3" s="42" t="s">
         <v>500</v>
       </c>
-      <c r="DQ3" s="43" t="s">
+      <c r="DQ3" s="42" t="s">
         <v>501</v>
       </c>
-      <c r="DR3" s="43" t="s">
+      <c r="DR3" s="42" t="s">
         <v>502</v>
       </c>
-      <c r="DS3" s="44" t="s">
+      <c r="DS3" s="43" t="s">
         <v>503</v>
       </c>
-      <c r="DT3" s="44" t="s">
+      <c r="DT3" s="43" t="s">
         <v>369</v>
       </c>
-      <c r="DU3" s="44" t="s">
+      <c r="DU3" s="43" t="s">
         <v>504</v>
       </c>
-      <c r="DV3" s="43" t="s">
+      <c r="DV3" s="42" t="s">
         <v>505</v>
       </c>
-      <c r="DW3" s="43" t="s">
+      <c r="DW3" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="DX3" s="44" t="s">
+      <c r="DX3" s="43" t="s">
         <v>368</v>
       </c>
-      <c r="DY3" s="44" t="s">
+      <c r="DY3" s="43" t="s">
         <v>506</v>
       </c>
-      <c r="DZ3" s="44" t="s">
+      <c r="DZ3" s="43" t="s">
         <v>507</v>
       </c>
-      <c r="EA3" s="44" t="s">
+      <c r="EA3" s="43" t="s">
         <v>478</v>
       </c>
-      <c r="EB3" s="44" t="s">
+      <c r="EB3" s="43" t="s">
         <v>507</v>
       </c>
-      <c r="EC3" s="44" t="s">
+      <c r="EC3" s="43" t="s">
         <v>508</v>
       </c>
-      <c r="ED3" s="44"/>
-      <c r="EE3" s="44"/>
-      <c r="EF3" s="44" t="s">
+      <c r="ED3" s="43"/>
+      <c r="EE3" s="43"/>
+      <c r="EF3" s="43" t="s">
         <v>509</v>
       </c>
-      <c r="EG3" s="44" t="s">
+      <c r="EG3" s="43" t="s">
         <v>374</v>
       </c>
-      <c r="EH3" s="44" t="s">
+      <c r="EH3" s="43" t="s">
         <v>373</v>
       </c>
-      <c r="EI3" s="44" t="s">
+      <c r="EI3" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="EJ3" s="44" t="s">
+      <c r="EJ3" s="43" t="s">
         <v>663</v>
       </c>
-      <c r="EK3" s="44" t="s">
+      <c r="EK3" s="43" t="s">
         <v>664</v>
       </c>
-      <c r="EL3" s="44" t="s">
+      <c r="EL3" s="43" t="s">
         <v>664</v>
       </c>
-      <c r="EM3" s="43" t="s">
+      <c r="EM3" s="42" t="s">
         <v>510</v>
       </c>
     </row>
@@ -6601,7 +6590,7 @@
       <c r="A2" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="44" t="s">
         <v>532</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -6656,7 +6645,7 @@
   <cols>
     <col min="1" max="1" width="40.5546875" customWidth="1"/>
     <col min="2" max="2" width="51.33203125" style="31" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" style="63" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="62" customWidth="1"/>
     <col min="4" max="4" width="19.109375" style="31" customWidth="1"/>
     <col min="5" max="5" width="18.5546875" customWidth="1"/>
     <col min="6" max="6" width="25.6640625" customWidth="1"/>
@@ -6704,67 +6693,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>272</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>273</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="45" t="s">
         <v>274</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="45" t="s">
         <v>533</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="45" t="s">
         <v>534</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="45" t="s">
         <v>535</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="47" t="s">
         <v>536</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="47" t="s">
         <v>537</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="47" t="s">
         <v>538</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="K1" s="47" t="s">
         <v>539</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="47" t="s">
         <v>540</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="M1" s="47" t="s">
         <v>541</v>
       </c>
-      <c r="N1" s="48" t="s">
+      <c r="N1" s="47" t="s">
         <v>542</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="O1" s="47" t="s">
         <v>543</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="P1" s="47" t="s">
         <v>544</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="47" t="s">
         <v>545</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="R1" s="47" t="s">
         <v>546</v>
       </c>
-      <c r="S1" s="49" t="s">
+      <c r="S1" s="48" t="s">
         <v>547</v>
       </c>
-      <c r="T1" s="49" t="s">
+      <c r="T1" s="48" t="s">
         <v>548</v>
       </c>
-      <c r="U1" s="50" t="s">
+      <c r="U1" s="49" t="s">
         <v>549</v>
       </c>
       <c r="V1" s="1" t="s">
@@ -6782,7 +6771,7 @@
       <c r="Z1" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="AA1" s="48" t="s">
+      <c r="AA1" s="47" t="s">
         <v>555</v>
       </c>
       <c r="AB1" s="1" t="s">
@@ -6812,7 +6801,7 @@
       <c r="AJ1" s="1" t="s">
         <v>564</v>
       </c>
-      <c r="AK1" s="51" t="s">
+      <c r="AK1" s="50" t="s">
         <v>565</v>
       </c>
       <c r="AL1" s="1" t="s">
@@ -6873,111 +6862,111 @@
         <v>584</v>
       </c>
     </row>
-    <row r="2" spans="1:56" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+    <row r="2" spans="1:56" s="56" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
         <v>585</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="52" t="s">
         <v>586</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="53" t="s">
         <v>587</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="D2" s="53" t="s">
         <v>587</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="51" t="s">
         <v>588</v>
       </c>
-      <c r="F2" s="52">
+      <c r="F2" s="51">
         <v>10</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="51" t="s">
         <v>589</v>
       </c>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="54" t="s">
         <v>590</v>
       </c>
-      <c r="I2" s="56" t="s">
+      <c r="I2" s="55" t="s">
         <v>591</v>
       </c>
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="54" t="s">
         <v>506</v>
       </c>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52">
+      <c r="K2" s="51"/>
+      <c r="L2" s="51">
         <v>9021723007</v>
       </c>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="57" t="s">
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="56" t="s">
         <v>592</v>
       </c>
-      <c r="P2" s="52" t="s">
+      <c r="P2" s="51" t="s">
         <v>593</v>
       </c>
-      <c r="Q2" s="58">
+      <c r="Q2" s="57">
         <v>5</v>
       </c>
-      <c r="R2" s="58" t="s">
+      <c r="R2" s="57" t="s">
         <v>589</v>
       </c>
-      <c r="S2" s="58" t="s">
+      <c r="S2" s="57" t="s">
         <v>594</v>
       </c>
-      <c r="T2" s="58" t="s">
+      <c r="T2" s="57" t="s">
         <v>595</v>
       </c>
-      <c r="U2" s="52" t="s">
+      <c r="U2" s="51" t="s">
         <v>596</v>
       </c>
-      <c r="V2" s="52"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="52"/>
-      <c r="Z2" s="52"/>
-      <c r="AA2" s="52"/>
-      <c r="AB2" s="52"/>
-      <c r="AC2" s="52"/>
-      <c r="AD2" s="52"/>
-      <c r="AE2" s="52"/>
-      <c r="AF2" s="52"/>
-      <c r="AG2" s="52"/>
-      <c r="AH2" s="52"/>
-      <c r="AI2" s="52"/>
-      <c r="AJ2" s="52"/>
-      <c r="AK2" s="52"/>
-      <c r="AL2" s="52"/>
-      <c r="AM2" s="52"/>
-      <c r="AN2" s="52"/>
-      <c r="AO2" s="52"/>
-      <c r="AP2" s="52"/>
-      <c r="AQ2" s="52"/>
-      <c r="AR2" s="52"/>
-      <c r="AS2" s="52"/>
-      <c r="AT2" s="52"/>
-      <c r="AU2" s="52"/>
-      <c r="AV2" s="52"/>
-      <c r="AW2" s="52"/>
-      <c r="AX2" s="52"/>
-      <c r="AY2" s="52"/>
-      <c r="AZ2" s="52"/>
-      <c r="BA2" s="52"/>
-      <c r="BB2" s="52"/>
-      <c r="BC2" s="52"/>
-      <c r="BD2" s="52"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="51"/>
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="51"/>
+      <c r="AD2" s="51"/>
+      <c r="AE2" s="51"/>
+      <c r="AF2" s="51"/>
+      <c r="AG2" s="51"/>
+      <c r="AH2" s="51"/>
+      <c r="AI2" s="51"/>
+      <c r="AJ2" s="51"/>
+      <c r="AK2" s="51"/>
+      <c r="AL2" s="51"/>
+      <c r="AM2" s="51"/>
+      <c r="AN2" s="51"/>
+      <c r="AO2" s="51"/>
+      <c r="AP2" s="51"/>
+      <c r="AQ2" s="51"/>
+      <c r="AR2" s="51"/>
+      <c r="AS2" s="51"/>
+      <c r="AT2" s="51"/>
+      <c r="AU2" s="51"/>
+      <c r="AV2" s="51"/>
+      <c r="AW2" s="51"/>
+      <c r="AX2" s="51"/>
+      <c r="AY2" s="51"/>
+      <c r="AZ2" s="51"/>
+      <c r="BA2" s="51"/>
+      <c r="BB2" s="51"/>
+      <c r="BC2" s="51"/>
+      <c r="BD2" s="51"/>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="53" t="s">
         <v>587</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="53" t="s">
         <v>587</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -7045,13 +7034,13 @@
       <c r="A4" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -7119,13 +7108,13 @@
       <c r="A5" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -7158,7 +7147,7 @@
       <c r="N5" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="O5" s="60" t="s">
+      <c r="O5" s="59" t="s">
         <v>592</v>
       </c>
       <c r="P5" s="2" t="s">
@@ -7209,13 +7198,13 @@
       <c r="A6" s="2" t="s">
         <v>605</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -7283,13 +7272,13 @@
       <c r="A7" s="2" t="s">
         <v>606</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -7363,13 +7352,13 @@
       <c r="A8" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -7409,7 +7398,7 @@
       <c r="Y8" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="Z8" s="61" t="s">
+      <c r="Z8" s="60" t="s">
         <v>611</v>
       </c>
       <c r="AA8" s="2"/>
@@ -7447,13 +7436,13 @@
       <c r="A9" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -7493,13 +7482,13 @@
       <c r="Y9" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="Z9" s="61" t="s">
+      <c r="Z9" s="60" t="s">
         <v>611</v>
       </c>
-      <c r="AA9" s="61" t="s">
+      <c r="AA9" s="60" t="s">
         <v>613</v>
       </c>
-      <c r="AB9" s="61" t="s">
+      <c r="AB9" s="60" t="s">
         <v>614</v>
       </c>
       <c r="AC9" s="2" t="s">
@@ -7539,13 +7528,13 @@
       <c r="A10" s="2" t="s">
         <v>617</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -7585,13 +7574,13 @@
       <c r="Y10" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="Z10" s="61" t="s">
+      <c r="Z10" s="60" t="s">
         <v>611</v>
       </c>
-      <c r="AA10" s="61" t="s">
+      <c r="AA10" s="60" t="s">
         <v>613</v>
       </c>
-      <c r="AB10" s="61" t="s">
+      <c r="AB10" s="60" t="s">
         <v>614</v>
       </c>
       <c r="AC10" s="2" t="s">
@@ -7631,13 +7620,13 @@
       <c r="A11" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -7677,13 +7666,13 @@
       <c r="Y11" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="Z11" s="61" t="s">
+      <c r="Z11" s="60" t="s">
         <v>611</v>
       </c>
-      <c r="AA11" s="61" t="s">
+      <c r="AA11" s="60" t="s">
         <v>613</v>
       </c>
-      <c r="AB11" s="61" t="s">
+      <c r="AB11" s="60" t="s">
         <v>614</v>
       </c>
       <c r="AC11" s="2" t="s">
@@ -7729,13 +7718,13 @@
       <c r="A12" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="B12" s="59" t="s">
+      <c r="B12" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -7775,13 +7764,13 @@
       <c r="Y12" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="Z12" s="61" t="s">
+      <c r="Z12" s="60" t="s">
         <v>611</v>
       </c>
-      <c r="AA12" s="61" t="s">
+      <c r="AA12" s="60" t="s">
         <v>613</v>
       </c>
-      <c r="AB12" s="61" t="s">
+      <c r="AB12" s="60" t="s">
         <v>614</v>
       </c>
       <c r="AC12" s="2" t="s">
@@ -7827,13 +7816,13 @@
       <c r="A13" s="2" t="s">
         <v>623</v>
       </c>
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -7873,13 +7862,13 @@
       <c r="Y13" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="Z13" s="61" t="s">
+      <c r="Z13" s="60" t="s">
         <v>611</v>
       </c>
-      <c r="AA13" s="61" t="s">
+      <c r="AA13" s="60" t="s">
         <v>613</v>
       </c>
-      <c r="AB13" s="61" t="s">
+      <c r="AB13" s="60" t="s">
         <v>614</v>
       </c>
       <c r="AC13" s="2" t="s">
@@ -7898,7 +7887,7 @@
       <c r="AH13" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="AI13" s="61" t="s">
+      <c r="AI13" s="60" t="s">
         <v>624</v>
       </c>
       <c r="AJ13" s="2"/>
@@ -7927,13 +7916,13 @@
       <c r="A14" s="2" t="s">
         <v>625</v>
       </c>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C14" s="54" t="s">
+      <c r="C14" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -7973,13 +7962,13 @@
       <c r="Y14" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="Z14" s="61" t="s">
+      <c r="Z14" s="60" t="s">
         <v>611</v>
       </c>
-      <c r="AA14" s="61" t="s">
+      <c r="AA14" s="60" t="s">
         <v>613</v>
       </c>
-      <c r="AB14" s="61" t="s">
+      <c r="AB14" s="60" t="s">
         <v>614</v>
       </c>
       <c r="AC14" s="2" t="s">
@@ -7998,7 +7987,7 @@
       <c r="AH14" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="AI14" s="61" t="s">
+      <c r="AI14" s="60" t="s">
         <v>624</v>
       </c>
       <c r="AJ14" s="2"/>
@@ -8027,13 +8016,13 @@
       <c r="A15" s="2" t="s">
         <v>626</v>
       </c>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D15" s="54" t="s">
+      <c r="D15" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -8073,13 +8062,13 @@
       <c r="Y15" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="Z15" s="61" t="s">
+      <c r="Z15" s="60" t="s">
         <v>611</v>
       </c>
-      <c r="AA15" s="61" t="s">
+      <c r="AA15" s="60" t="s">
         <v>613</v>
       </c>
-      <c r="AB15" s="61" t="s">
+      <c r="AB15" s="60" t="s">
         <v>614</v>
       </c>
       <c r="AC15" s="2" t="s">
@@ -8098,7 +8087,7 @@
       <c r="AH15" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="AI15" s="61" t="s">
+      <c r="AI15" s="60" t="s">
         <v>624</v>
       </c>
       <c r="AJ15" s="2"/>
@@ -8127,13 +8116,13 @@
       <c r="A16" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D16" s="54" t="s">
+      <c r="D16" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -8208,7 +8197,7 @@
       <c r="AT16" s="2">
         <v>411033</v>
       </c>
-      <c r="AU16" s="45" t="s">
+      <c r="AU16" s="44" t="s">
         <v>636</v>
       </c>
       <c r="AV16" s="2">
@@ -8227,125 +8216,125 @@
       <c r="BC16" s="2"/>
       <c r="BD16" s="2"/>
     </row>
-    <row r="17" spans="1:56" s="57" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="52" t="s">
+    <row r="17" spans="1:56" s="56" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="51" t="s">
         <v>638</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="E17" s="52" t="s">
+      <c r="E17" s="51" t="s">
         <v>588</v>
       </c>
-      <c r="F17" s="52">
+      <c r="F17" s="51">
         <v>5</v>
       </c>
-      <c r="G17" s="52" t="s">
+      <c r="G17" s="51" t="s">
         <v>589</v>
       </c>
-      <c r="H17" s="55" t="s">
+      <c r="H17" s="54" t="s">
         <v>590</v>
       </c>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="52"/>
-      <c r="N17" s="52"/>
-      <c r="O17" s="52"/>
-      <c r="P17" s="52"/>
-      <c r="Q17" s="52"/>
-      <c r="R17" s="52"/>
-      <c r="S17" s="52"/>
-      <c r="T17" s="52"/>
-      <c r="U17" s="52"/>
-      <c r="V17" s="52"/>
-      <c r="W17" s="55"/>
-      <c r="X17" s="52"/>
-      <c r="Y17" s="52"/>
-      <c r="Z17" s="52"/>
-      <c r="AA17" s="52"/>
-      <c r="AB17" s="52"/>
-      <c r="AC17" s="52"/>
-      <c r="AD17" s="52"/>
-      <c r="AE17" s="52"/>
-      <c r="AF17" s="52"/>
-      <c r="AG17" s="52"/>
-      <c r="AH17" s="52"/>
-      <c r="AI17" s="52"/>
-      <c r="AJ17" s="52" t="s">
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="51"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="51"/>
+      <c r="O17" s="51"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="51"/>
+      <c r="R17" s="51"/>
+      <c r="S17" s="51"/>
+      <c r="T17" s="51"/>
+      <c r="U17" s="51"/>
+      <c r="V17" s="51"/>
+      <c r="W17" s="54"/>
+      <c r="X17" s="51"/>
+      <c r="Y17" s="51"/>
+      <c r="Z17" s="51"/>
+      <c r="AA17" s="51"/>
+      <c r="AB17" s="51"/>
+      <c r="AC17" s="51"/>
+      <c r="AD17" s="51"/>
+      <c r="AE17" s="51"/>
+      <c r="AF17" s="51"/>
+      <c r="AG17" s="51"/>
+      <c r="AH17" s="51"/>
+      <c r="AI17" s="51"/>
+      <c r="AJ17" s="51" t="s">
         <v>628</v>
       </c>
-      <c r="AK17" s="52" t="s">
+      <c r="AK17" s="51" t="s">
         <v>629</v>
       </c>
-      <c r="AL17" s="52" t="s">
+      <c r="AL17" s="51" t="s">
         <v>630</v>
       </c>
-      <c r="AM17" s="52" t="s">
+      <c r="AM17" s="51" t="s">
         <v>631</v>
       </c>
-      <c r="AN17" s="52" t="s">
+      <c r="AN17" s="51" t="s">
         <v>632</v>
       </c>
-      <c r="AO17" s="52" t="s">
+      <c r="AO17" s="51" t="s">
         <v>632</v>
       </c>
-      <c r="AP17" s="52" t="s">
+      <c r="AP17" s="51" t="s">
         <v>633</v>
       </c>
-      <c r="AQ17" s="52" t="s">
+      <c r="AQ17" s="51" t="s">
         <v>634</v>
       </c>
-      <c r="AR17" s="52" t="s">
+      <c r="AR17" s="51" t="s">
         <v>635</v>
       </c>
-      <c r="AS17" s="52" t="s">
+      <c r="AS17" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="AT17" s="52">
+      <c r="AT17" s="51">
         <v>411033</v>
       </c>
-      <c r="AU17" s="62" t="s">
+      <c r="AU17" s="61" t="s">
         <v>636</v>
       </c>
-      <c r="AV17" s="52">
+      <c r="AV17" s="51">
         <v>7896543215</v>
       </c>
-      <c r="AW17" s="52">
+      <c r="AW17" s="51">
         <v>5000</v>
       </c>
-      <c r="AX17" s="52" t="s">
+      <c r="AX17" s="51" t="s">
         <v>637</v>
       </c>
-      <c r="AY17" s="52" t="s">
+      <c r="AY17" s="51" t="s">
         <v>592</v>
       </c>
-      <c r="AZ17" s="52" t="s">
+      <c r="AZ17" s="51" t="s">
         <v>592</v>
       </c>
-      <c r="BA17" s="52"/>
-      <c r="BB17" s="52"/>
-      <c r="BC17" s="52"/>
-      <c r="BD17" s="52"/>
+      <c r="BA17" s="51"/>
+      <c r="BB17" s="51"/>
+      <c r="BC17" s="51"/>
+      <c r="BD17" s="51"/>
     </row>
     <row r="18" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>639</v>
       </c>
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D18" s="54" t="s">
+      <c r="D18" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -8420,7 +8409,7 @@
       <c r="AT18" s="2">
         <v>411033</v>
       </c>
-      <c r="AU18" s="45" t="s">
+      <c r="AU18" s="44" t="s">
         <v>636</v>
       </c>
       <c r="AV18" s="2">
@@ -8447,13 +8436,13 @@
       <c r="A19" s="2" t="s">
         <v>640</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D19" s="54" t="s">
+      <c r="D19" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -8528,7 +8517,7 @@
       <c r="AT19" s="2">
         <v>411033</v>
       </c>
-      <c r="AU19" s="45" t="s">
+      <c r="AU19" s="44" t="s">
         <v>636</v>
       </c>
       <c r="AV19" s="2">
@@ -8555,13 +8544,13 @@
       <c r="A20" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D20" s="54" t="s">
+      <c r="D20" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -8636,7 +8625,7 @@
       <c r="AT20" s="2">
         <v>411033</v>
       </c>
-      <c r="AU20" s="45" t="s">
+      <c r="AU20" s="44" t="s">
         <v>636</v>
       </c>
       <c r="AV20" s="2">
@@ -8663,13 +8652,13 @@
       <c r="A21" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D21" s="54" t="s">
+      <c r="D21" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -8737,13 +8726,13 @@
       <c r="A22" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="B22" s="59" t="s">
+      <c r="B22" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D22" s="54" t="s">
+      <c r="D22" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -8811,13 +8800,13 @@
       <c r="A23" s="2" t="s">
         <v>644</v>
       </c>
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C23" s="54" t="s">
+      <c r="C23" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D23" s="54" t="s">
+      <c r="D23" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -8885,13 +8874,13 @@
       <c r="A24" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D24" s="54" t="s">
+      <c r="D24" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -8959,13 +8948,13 @@
       <c r="A25" s="2" t="s">
         <v>646</v>
       </c>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -9033,13 +9022,13 @@
       <c r="A26" s="2" t="s">
         <v>647</v>
       </c>
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C26" s="54" t="s">
+      <c r="C26" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D26" s="54" t="s">
+      <c r="D26" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -9107,13 +9096,13 @@
       <c r="A27" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C27" s="54" t="s">
+      <c r="C27" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D27" s="54" t="s">
+      <c r="D27" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -9181,13 +9170,13 @@
       <c r="A28" t="s">
         <v>649</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="58" t="s">
         <v>586</v>
       </c>
-      <c r="C28" s="54" t="s">
+      <c r="C28" s="53" t="s">
         <v>599</v>
       </c>
-      <c r="D28" s="54" t="s">
+      <c r="D28" s="53" t="s">
         <v>599</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -9220,7 +9209,7 @@
       <c r="N28" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="O28" s="60" t="s">
+      <c r="O28" s="59" t="s">
         <v>592</v>
       </c>
       <c r="P28" s="2" t="s">
@@ -9286,8 +9275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EP183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CF1" workbookViewId="0">
-      <selection activeCell="CN1" sqref="CN1"/>
+    <sheetView tabSelected="1" topLeftCell="BT14" workbookViewId="0">
+      <selection activeCell="CE16" sqref="CE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9940,21 +9929,15 @@
       <c r="BO2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP2" s="9" t="s">
-        <v>751</v>
+      <c r="BP2" s="28" t="s">
+        <v>369</v>
       </c>
       <c r="BQ2" s="28" t="s">
-        <v>369</v>
-      </c>
-      <c r="BR2" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="BS2" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="BT2" s="9" t="s">
-        <v>321</v>
-      </c>
+      <c r="BR2" s="2"/>
+      <c r="BS2" s="9"/>
+      <c r="BT2" s="9"/>
       <c r="BU2" s="9" t="s">
         <v>40</v>
       </c>
@@ -9980,11 +9963,11 @@
       <c r="CC2" s="28" t="s">
         <v>372</v>
       </c>
-      <c r="CD2" s="31"/>
+      <c r="CD2" s="9"/>
       <c r="CE2" s="28" t="s">
-        <v>752</v>
-      </c>
-      <c r="CF2" s="31"/>
+        <v>751</v>
+      </c>
+      <c r="CF2" s="9"/>
       <c r="CG2" s="28" t="s">
         <v>133</v>
       </c>
@@ -10041,22 +10024,22 @@
       <c r="CZ2" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="DA2" s="31" t="s">
+      <c r="DA2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="DB2" s="31" t="s">
+      <c r="DB2" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="DC2" s="31" t="s">
+      <c r="DC2" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="DD2" s="31" t="s">
+      <c r="DD2" s="9" t="s">
         <v>692</v>
       </c>
-      <c r="DE2" s="31" t="s">
+      <c r="DE2" s="9" t="s">
         <v>695</v>
       </c>
-      <c r="DF2" s="31" t="s">
+      <c r="DF2" s="9" t="s">
         <v>694</v>
       </c>
       <c r="DG2" s="9" t="s">
@@ -10166,7 +10149,7 @@
     </row>
     <row r="3" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>745</v>
@@ -10333,7 +10316,7 @@
       <c r="BF3" s="28" t="s">
         <v>366</v>
       </c>
-      <c r="BG3" s="28" t="s">
+      <c r="BG3" s="67" t="s">
         <v>35</v>
       </c>
       <c r="BH3" s="28"/>
@@ -10358,21 +10341,15 @@
       <c r="BO3" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP3" s="9" t="s">
-        <v>751</v>
+      <c r="BP3" s="28" t="s">
+        <v>369</v>
       </c>
       <c r="BQ3" s="28" t="s">
-        <v>369</v>
-      </c>
-      <c r="BR3" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="BS3" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="BT3" s="9" t="s">
-        <v>321</v>
-      </c>
+      <c r="BR3" s="2"/>
+      <c r="BS3" s="9"/>
+      <c r="BT3" s="9"/>
       <c r="BU3" s="9" t="s">
         <v>40</v>
       </c>
@@ -10398,11 +10375,11 @@
       <c r="CC3" s="28" t="s">
         <v>372</v>
       </c>
-      <c r="CD3" s="31"/>
+      <c r="CD3" s="9"/>
       <c r="CE3" s="28" t="s">
-        <v>754</v>
-      </c>
-      <c r="CF3" s="31"/>
+        <v>753</v>
+      </c>
+      <c r="CF3" s="9"/>
       <c r="CG3" s="28" t="s">
         <v>133</v>
       </c>
@@ -10450,9 +10427,9 @@
       <c r="CW3" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="CX3" s="31"/>
-      <c r="CY3" s="31"/>
-      <c r="CZ3" s="31"/>
+      <c r="CX3" s="9"/>
+      <c r="CY3" s="9"/>
+      <c r="CZ3" s="9"/>
       <c r="DA3" s="9"/>
       <c r="DB3" s="9"/>
       <c r="DC3" s="9" t="s">
@@ -10479,8 +10456,8 @@
       <c r="DJ3" s="9" t="s">
         <v>691</v>
       </c>
-      <c r="DK3" s="31"/>
-      <c r="DL3" s="31"/>
+      <c r="DK3" s="9"/>
+      <c r="DL3" s="9"/>
       <c r="DM3" s="9"/>
       <c r="DN3" s="9"/>
       <c r="DO3" s="9"/>
@@ -10706,21 +10683,15 @@
       <c r="BO4" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP4" s="9" t="s">
-        <v>751</v>
+      <c r="BP4" s="28" t="s">
+        <v>369</v>
       </c>
       <c r="BQ4" s="28" t="s">
-        <v>369</v>
-      </c>
-      <c r="BR4" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="BS4" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="BT4" s="9" t="s">
-        <v>321</v>
-      </c>
+      <c r="BR4" s="2"/>
+      <c r="BS4" s="9"/>
+      <c r="BT4" s="9"/>
       <c r="BU4" s="9" t="s">
         <v>40</v>
       </c>
@@ -10732,7 +10703,7 @@
         <v>167</v>
       </c>
       <c r="BY4" s="9" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="BZ4" s="9" t="s">
         <v>48</v>
@@ -10744,11 +10715,11 @@
         <v>61</v>
       </c>
       <c r="CC4" s="28"/>
-      <c r="CD4" s="31"/>
+      <c r="CD4" s="9"/>
       <c r="CE4" s="28" t="s">
-        <v>752</v>
-      </c>
-      <c r="CF4" s="31"/>
+        <v>751</v>
+      </c>
+      <c r="CF4" s="9"/>
       <c r="CG4" s="28" t="s">
         <v>133</v>
       </c>
@@ -10796,9 +10767,9 @@
       <c r="CW4" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="CX4" s="31"/>
-      <c r="CY4" s="31"/>
-      <c r="CZ4" s="31"/>
+      <c r="CX4" s="9"/>
+      <c r="CY4" s="9"/>
+      <c r="CZ4" s="9"/>
       <c r="DA4" s="9"/>
       <c r="DB4" s="9"/>
       <c r="DC4" s="9"/>
@@ -10844,7 +10815,7 @@
     </row>
     <row r="5" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>745</v>
@@ -11036,21 +11007,15 @@
       <c r="BO5" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP5" s="9" t="s">
-        <v>751</v>
+      <c r="BP5" s="28" t="s">
+        <v>369</v>
       </c>
       <c r="BQ5" s="28" t="s">
-        <v>369</v>
-      </c>
-      <c r="BR5" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="BS5" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="BT5" s="9" t="s">
-        <v>321</v>
-      </c>
+      <c r="BR5" s="2"/>
+      <c r="BS5" s="9"/>
+      <c r="BT5" s="9"/>
       <c r="BU5" s="9" t="s">
         <v>40</v>
       </c>
@@ -11062,7 +11027,7 @@
         <v>167</v>
       </c>
       <c r="BY5" s="9" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="BZ5" s="9" t="s">
         <v>48</v>
@@ -11074,11 +11039,11 @@
         <v>61</v>
       </c>
       <c r="CC5" s="28"/>
-      <c r="CD5" s="31"/>
+      <c r="CD5" s="9"/>
       <c r="CE5" s="28" t="s">
-        <v>754</v>
-      </c>
-      <c r="CF5" s="31"/>
+        <v>753</v>
+      </c>
+      <c r="CF5" s="9"/>
       <c r="CG5" s="28" t="s">
         <v>133</v>
       </c>
@@ -11126,9 +11091,9 @@
       <c r="CW5" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="CX5" s="31"/>
-      <c r="CY5" s="31"/>
-      <c r="CZ5" s="31"/>
+      <c r="CX5" s="9"/>
+      <c r="CY5" s="9"/>
+      <c r="CZ5" s="9"/>
       <c r="DA5" s="9"/>
       <c r="DB5" s="9"/>
       <c r="DC5" s="9"/>
@@ -11366,21 +11331,15 @@
       <c r="BO6" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP6" s="9" t="s">
-        <v>751</v>
+      <c r="BP6" s="28" t="s">
+        <v>369</v>
       </c>
       <c r="BQ6" s="28" t="s">
-        <v>369</v>
-      </c>
-      <c r="BR6" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="BS6" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="BT6" s="9" t="s">
-        <v>321</v>
-      </c>
+      <c r="BR6" s="2"/>
+      <c r="BS6" s="9"/>
+      <c r="BT6" s="9"/>
       <c r="BU6" s="9" t="s">
         <v>40</v>
       </c>
@@ -11404,11 +11363,11 @@
         <v>61</v>
       </c>
       <c r="CC6" s="28"/>
-      <c r="CD6" s="31"/>
+      <c r="CD6" s="9"/>
       <c r="CE6" s="28" t="s">
-        <v>752</v>
-      </c>
-      <c r="CF6" s="31"/>
+        <v>751</v>
+      </c>
+      <c r="CF6" s="9"/>
       <c r="CG6" s="28" t="s">
         <v>133</v>
       </c>
@@ -11456,9 +11415,9 @@
       <c r="CW6" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="CX6" s="31"/>
-      <c r="CY6" s="31"/>
-      <c r="CZ6" s="31"/>
+      <c r="CX6" s="9"/>
+      <c r="CY6" s="9"/>
+      <c r="CZ6" s="9"/>
       <c r="DA6" s="9"/>
       <c r="DB6" s="9"/>
       <c r="DC6" s="9"/>
@@ -11504,7 +11463,7 @@
     </row>
     <row r="7" spans="1:146" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>745</v>
@@ -11696,21 +11655,15 @@
       <c r="BO7" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP7" s="9" t="s">
-        <v>751</v>
+      <c r="BP7" s="28" t="s">
+        <v>369</v>
       </c>
       <c r="BQ7" s="28" t="s">
-        <v>369</v>
-      </c>
-      <c r="BR7" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="BS7" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="BT7" s="9" t="s">
-        <v>321</v>
-      </c>
+      <c r="BR7" s="2"/>
+      <c r="BS7" s="9"/>
+      <c r="BT7" s="9"/>
       <c r="BU7" s="9" t="s">
         <v>40</v>
       </c>
@@ -11734,11 +11687,11 @@
         <v>61</v>
       </c>
       <c r="CC7" s="28"/>
-      <c r="CD7" s="31"/>
+      <c r="CD7" s="9"/>
       <c r="CE7" s="28" t="s">
-        <v>754</v>
-      </c>
-      <c r="CF7" s="31"/>
+        <v>753</v>
+      </c>
+      <c r="CF7" s="9"/>
       <c r="CG7" s="28" t="s">
         <v>133</v>
       </c>
@@ -11786,9 +11739,9 @@
       <c r="CW7" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="CX7" s="31"/>
-      <c r="CY7" s="31"/>
-      <c r="CZ7" s="31"/>
+      <c r="CX7" s="9"/>
+      <c r="CY7" s="9"/>
+      <c r="CZ7" s="9"/>
       <c r="DA7" s="9"/>
       <c r="DB7" s="9"/>
       <c r="DC7" s="9"/>
@@ -11834,7 +11787,7 @@
     </row>
     <row r="8" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>322</v>
@@ -11868,7 +11821,7 @@
       </c>
       <c r="L8" s="9"/>
       <c r="M8" s="28" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="N8" s="28"/>
       <c r="O8" s="28" t="s">
@@ -11923,7 +11876,7 @@
         <v>36</v>
       </c>
       <c r="AF8" s="28" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="AG8" s="28" t="s">
         <v>9</v>
@@ -11962,13 +11915,13 @@
         <v>321</v>
       </c>
       <c r="AS8" s="28" t="s">
+        <v>760</v>
+      </c>
+      <c r="AT8" s="28" t="s">
         <v>761</v>
       </c>
-      <c r="AT8" s="28" t="s">
+      <c r="AU8" s="28" t="s">
         <v>762</v>
-      </c>
-      <c r="AU8" s="28" t="s">
-        <v>763</v>
       </c>
       <c r="AV8" s="28" t="s">
         <v>29</v>
@@ -12006,7 +11959,7 @@
       </c>
       <c r="BH8" s="28"/>
       <c r="BI8" s="28" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="BJ8" s="28" t="s">
         <v>167</v>
@@ -12026,25 +11979,19 @@
       <c r="BO8" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP8" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="BQ8" s="28" t="s">
+      <c r="BP8" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="BR8" s="28"/>
-      <c r="BS8" s="9" t="s">
-        <v>765</v>
-      </c>
-      <c r="BT8" s="9" t="s">
-        <v>765</v>
-      </c>
+      <c r="BQ8" s="28"/>
+      <c r="BR8" s="2"/>
+      <c r="BS8" s="9"/>
+      <c r="BT8" s="9"/>
       <c r="BU8" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BV8" s="9"/>
       <c r="BW8" s="9" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="BX8" s="9" t="s">
         <v>167</v>
@@ -12064,7 +12011,7 @@
       <c r="CC8" s="9"/>
       <c r="CD8" s="9"/>
       <c r="CE8" s="28" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="CF8" s="28"/>
       <c r="CG8" s="9" t="s">
@@ -12124,7 +12071,7 @@
       <c r="DE8" s="9"/>
       <c r="DF8" s="9"/>
       <c r="DG8" s="9"/>
-      <c r="DH8" s="35"/>
+      <c r="DH8" s="9"/>
       <c r="DI8" s="9"/>
       <c r="DJ8" s="9"/>
       <c r="DK8" s="9"/>
@@ -12162,7 +12109,7 @@
     </row>
     <row r="9" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>322</v>
@@ -12196,7 +12143,7 @@
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="28" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="N9" s="28"/>
       <c r="O9" s="28" t="s">
@@ -12251,7 +12198,7 @@
         <v>36</v>
       </c>
       <c r="AF9" s="28" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="AG9" s="28" t="s">
         <v>9</v>
@@ -12290,13 +12237,13 @@
         <v>321</v>
       </c>
       <c r="AS9" s="28" t="s">
+        <v>760</v>
+      </c>
+      <c r="AT9" s="28" t="s">
         <v>761</v>
       </c>
-      <c r="AT9" s="28" t="s">
+      <c r="AU9" s="28" t="s">
         <v>762</v>
-      </c>
-      <c r="AU9" s="28" t="s">
-        <v>763</v>
       </c>
       <c r="AV9" s="28" t="s">
         <v>29</v>
@@ -12334,7 +12281,7 @@
       </c>
       <c r="BH9" s="28"/>
       <c r="BI9" s="28" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="BJ9" s="28" t="s">
         <v>167</v>
@@ -12354,25 +12301,19 @@
       <c r="BO9" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP9" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="BQ9" s="28" t="s">
+      <c r="BP9" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="BR9" s="28"/>
-      <c r="BS9" s="9" t="s">
-        <v>765</v>
-      </c>
-      <c r="BT9" s="9" t="s">
-        <v>765</v>
-      </c>
+      <c r="BQ9" s="28"/>
+      <c r="BR9" s="2"/>
+      <c r="BS9" s="9"/>
+      <c r="BT9" s="9"/>
       <c r="BU9" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BV9" s="9"/>
       <c r="BW9" s="9" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="BX9" s="9" t="s">
         <v>167</v>
@@ -12392,7 +12333,7 @@
       <c r="CC9" s="9"/>
       <c r="CD9" s="9"/>
       <c r="CE9" s="28" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="CF9" s="28"/>
       <c r="CG9" s="9" t="s">
@@ -12452,7 +12393,7 @@
       <c r="DE9" s="9"/>
       <c r="DF9" s="9"/>
       <c r="DG9" s="9"/>
-      <c r="DH9" s="35"/>
+      <c r="DH9" s="9"/>
       <c r="DI9" s="9"/>
       <c r="DJ9" s="9"/>
       <c r="DK9" s="9"/>
@@ -12490,7 +12431,7 @@
     </row>
     <row r="10" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>322</v>
@@ -12524,7 +12465,7 @@
       </c>
       <c r="L10" s="9"/>
       <c r="M10" s="28" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="N10" s="28"/>
       <c r="O10" s="28" t="s">
@@ -12579,7 +12520,7 @@
         <v>36</v>
       </c>
       <c r="AF10" s="28" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="AG10" s="28" t="s">
         <v>9</v>
@@ -12618,13 +12559,13 @@
         <v>321</v>
       </c>
       <c r="AS10" s="28" t="s">
+        <v>768</v>
+      </c>
+      <c r="AT10" s="28" t="s">
+        <v>769</v>
+      </c>
+      <c r="AU10" s="28" t="s">
         <v>770</v>
-      </c>
-      <c r="AT10" s="28" t="s">
-        <v>771</v>
-      </c>
-      <c r="AU10" s="28" t="s">
-        <v>772</v>
       </c>
       <c r="AV10" s="28" t="s">
         <v>29</v>
@@ -12662,7 +12603,7 @@
       </c>
       <c r="BH10" s="28"/>
       <c r="BI10" s="28" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="BJ10" s="28" t="s">
         <v>167</v>
@@ -12682,25 +12623,19 @@
       <c r="BO10" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP10" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="BQ10" s="28" t="s">
+      <c r="BP10" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="BR10" s="28"/>
-      <c r="BS10" s="9" t="s">
-        <v>765</v>
-      </c>
-      <c r="BT10" s="9" t="s">
-        <v>765</v>
-      </c>
+      <c r="BQ10" s="28"/>
+      <c r="BR10" s="2"/>
+      <c r="BS10" s="9"/>
+      <c r="BT10" s="9"/>
       <c r="BU10" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BV10" s="9"/>
       <c r="BW10" s="9" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="BX10" s="9" t="s">
         <v>167</v>
@@ -12720,7 +12655,7 @@
       <c r="CC10" s="9"/>
       <c r="CD10" s="9"/>
       <c r="CE10" s="28" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="CF10" s="28"/>
       <c r="CG10" s="9" t="s">
@@ -12780,7 +12715,7 @@
       <c r="DE10" s="9"/>
       <c r="DF10" s="9"/>
       <c r="DG10" s="9"/>
-      <c r="DH10" s="35"/>
+      <c r="DH10" s="9"/>
       <c r="DI10" s="9"/>
       <c r="DJ10" s="9"/>
       <c r="DK10" s="9"/>
@@ -12818,7 +12753,7 @@
     </row>
     <row r="11" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>322</v>
@@ -12852,7 +12787,7 @@
       </c>
       <c r="L11" s="9"/>
       <c r="M11" s="28" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="N11" s="28"/>
       <c r="O11" s="28" t="s">
@@ -12907,7 +12842,7 @@
         <v>36</v>
       </c>
       <c r="AF11" s="28" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="AG11" s="28" t="s">
         <v>9</v>
@@ -12946,13 +12881,13 @@
         <v>321</v>
       </c>
       <c r="AS11" s="28" t="s">
+        <v>768</v>
+      </c>
+      <c r="AT11" s="28" t="s">
+        <v>769</v>
+      </c>
+      <c r="AU11" s="28" t="s">
         <v>770</v>
-      </c>
-      <c r="AT11" s="28" t="s">
-        <v>771</v>
-      </c>
-      <c r="AU11" s="28" t="s">
-        <v>772</v>
       </c>
       <c r="AV11" s="28" t="s">
         <v>29</v>
@@ -12990,7 +12925,7 @@
       </c>
       <c r="BH11" s="28"/>
       <c r="BI11" s="28" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="BJ11" s="28" t="s">
         <v>167</v>
@@ -13010,25 +12945,19 @@
       <c r="BO11" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP11" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="BQ11" s="28" t="s">
+      <c r="BP11" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="BR11" s="28"/>
-      <c r="BS11" s="9" t="s">
-        <v>765</v>
-      </c>
-      <c r="BT11" s="9" t="s">
-        <v>765</v>
-      </c>
+      <c r="BQ11" s="28"/>
+      <c r="BR11" s="2"/>
+      <c r="BS11" s="9"/>
+      <c r="BT11" s="9"/>
       <c r="BU11" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BV11" s="9"/>
       <c r="BW11" s="9" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="BX11" s="9" t="s">
         <v>167</v>
@@ -13048,7 +12977,7 @@
       <c r="CC11" s="9"/>
       <c r="CD11" s="9"/>
       <c r="CE11" s="28" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="CF11" s="28"/>
       <c r="CG11" s="9" t="s">
@@ -13108,7 +13037,7 @@
       <c r="DE11" s="9"/>
       <c r="DF11" s="9"/>
       <c r="DG11" s="9"/>
-      <c r="DH11" s="35"/>
+      <c r="DH11" s="9"/>
       <c r="DI11" s="9"/>
       <c r="DJ11" s="9"/>
       <c r="DK11" s="9"/>
@@ -13146,7 +13075,7 @@
     </row>
     <row r="12" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>322</v>
@@ -13180,7 +13109,7 @@
       </c>
       <c r="L12" s="9"/>
       <c r="M12" s="28" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="N12" s="28"/>
       <c r="O12" s="28" t="s">
@@ -13235,7 +13164,7 @@
         <v>36</v>
       </c>
       <c r="AF12" s="28" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="AG12" s="28" t="s">
         <v>9</v>
@@ -13274,13 +13203,13 @@
         <v>321</v>
       </c>
       <c r="AS12" s="28" t="s">
+        <v>776</v>
+      </c>
+      <c r="AT12" s="28" t="s">
+        <v>777</v>
+      </c>
+      <c r="AU12" s="28" t="s">
         <v>778</v>
-      </c>
-      <c r="AT12" s="28" t="s">
-        <v>779</v>
-      </c>
-      <c r="AU12" s="28" t="s">
-        <v>780</v>
       </c>
       <c r="AV12" s="28" t="s">
         <v>29</v>
@@ -13318,7 +13247,7 @@
       </c>
       <c r="BH12" s="28"/>
       <c r="BI12" s="28" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="BJ12" s="28" t="s">
         <v>167</v>
@@ -13338,25 +13267,19 @@
       <c r="BO12" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP12" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="BQ12" s="28" t="s">
+      <c r="BP12" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="BR12" s="28"/>
-      <c r="BS12" s="9" t="s">
-        <v>765</v>
-      </c>
-      <c r="BT12" s="9" t="s">
-        <v>765</v>
-      </c>
+      <c r="BQ12" s="28"/>
+      <c r="BR12" s="2"/>
+      <c r="BS12" s="9"/>
+      <c r="BT12" s="9"/>
       <c r="BU12" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BV12" s="9"/>
       <c r="BW12" s="9" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="BX12" s="9" t="s">
         <v>167</v>
@@ -13376,7 +13299,7 @@
       <c r="CC12" s="9"/>
       <c r="CD12" s="9"/>
       <c r="CE12" s="28" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="CF12" s="28"/>
       <c r="CG12" s="9" t="s">
@@ -13436,7 +13359,7 @@
       <c r="DE12" s="9"/>
       <c r="DF12" s="9"/>
       <c r="DG12" s="9"/>
-      <c r="DH12" s="35"/>
+      <c r="DH12" s="9"/>
       <c r="DI12" s="9"/>
       <c r="DJ12" s="9"/>
       <c r="DK12" s="9"/>
@@ -13474,7 +13397,7 @@
     </row>
     <row r="13" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>322</v>
@@ -13508,7 +13431,7 @@
       </c>
       <c r="L13" s="9"/>
       <c r="M13" s="28" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="N13" s="28"/>
       <c r="O13" s="28" t="s">
@@ -13563,7 +13486,7 @@
         <v>36</v>
       </c>
       <c r="AF13" s="28" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="AG13" s="28" t="s">
         <v>9</v>
@@ -13602,13 +13525,13 @@
         <v>321</v>
       </c>
       <c r="AS13" s="28" t="s">
+        <v>776</v>
+      </c>
+      <c r="AT13" s="28" t="s">
+        <v>777</v>
+      </c>
+      <c r="AU13" s="28" t="s">
         <v>778</v>
-      </c>
-      <c r="AT13" s="28" t="s">
-        <v>779</v>
-      </c>
-      <c r="AU13" s="28" t="s">
-        <v>780</v>
       </c>
       <c r="AV13" s="28" t="s">
         <v>29</v>
@@ -13646,7 +13569,7 @@
       </c>
       <c r="BH13" s="28"/>
       <c r="BI13" s="28" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="BJ13" s="28" t="s">
         <v>167</v>
@@ -13666,25 +13589,19 @@
       <c r="BO13" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP13" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="BQ13" s="28" t="s">
+      <c r="BP13" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="BR13" s="28"/>
-      <c r="BS13" s="9" t="s">
-        <v>765</v>
-      </c>
-      <c r="BT13" s="9" t="s">
-        <v>765</v>
-      </c>
+      <c r="BQ13" s="28"/>
+      <c r="BR13" s="2"/>
+      <c r="BS13" s="9"/>
+      <c r="BT13" s="9"/>
       <c r="BU13" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BV13" s="9"/>
       <c r="BW13" s="9" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="BX13" s="9" t="s">
         <v>167</v>
@@ -13704,7 +13621,7 @@
       <c r="CC13" s="9"/>
       <c r="CD13" s="9"/>
       <c r="CE13" s="28" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="CF13" s="28"/>
       <c r="CG13" s="9" t="s">
@@ -13764,7 +13681,7 @@
       <c r="DE13" s="9"/>
       <c r="DF13" s="9"/>
       <c r="DG13" s="9"/>
-      <c r="DH13" s="35"/>
+      <c r="DH13" s="9"/>
       <c r="DI13" s="9"/>
       <c r="DJ13" s="9"/>
       <c r="DK13" s="9"/>
@@ -13802,7 +13719,7 @@
     </row>
     <row r="14" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>322</v>
@@ -13836,7 +13753,7 @@
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="28" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="N14" s="28"/>
       <c r="O14" s="28" t="s">
@@ -13891,7 +13808,7 @@
         <v>36</v>
       </c>
       <c r="AF14" s="28" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AG14" s="28" t="s">
         <v>9</v>
@@ -13930,13 +13847,13 @@
         <v>321</v>
       </c>
       <c r="AS14" s="28" t="s">
+        <v>784</v>
+      </c>
+      <c r="AT14" s="28" t="s">
+        <v>785</v>
+      </c>
+      <c r="AU14" s="28" t="s">
         <v>786</v>
-      </c>
-      <c r="AT14" s="28" t="s">
-        <v>787</v>
-      </c>
-      <c r="AU14" s="28" t="s">
-        <v>788</v>
       </c>
       <c r="AV14" s="28" t="s">
         <v>29</v>
@@ -13974,7 +13891,7 @@
       </c>
       <c r="BH14" s="28"/>
       <c r="BI14" s="28" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="BJ14" s="28" t="s">
         <v>167</v>
@@ -13994,25 +13911,19 @@
       <c r="BO14" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP14" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="BQ14" s="28" t="s">
+      <c r="BP14" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="BR14" s="28"/>
-      <c r="BS14" s="9" t="s">
-        <v>765</v>
-      </c>
-      <c r="BT14" s="9" t="s">
-        <v>765</v>
-      </c>
+      <c r="BQ14" s="28"/>
+      <c r="BR14" s="2"/>
+      <c r="BS14" s="9"/>
+      <c r="BT14" s="9"/>
       <c r="BU14" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BV14" s="9"/>
       <c r="BW14" s="9" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="BX14" s="9" t="s">
         <v>167</v>
@@ -14032,7 +13943,7 @@
       <c r="CC14" s="9"/>
       <c r="CD14" s="9"/>
       <c r="CE14" s="28" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="CF14" s="28"/>
       <c r="CG14" s="9" t="s">
@@ -14092,7 +14003,7 @@
       <c r="DE14" s="9"/>
       <c r="DF14" s="9"/>
       <c r="DG14" s="9"/>
-      <c r="DH14" s="35"/>
+      <c r="DH14" s="9"/>
       <c r="DI14" s="9"/>
       <c r="DJ14" s="9"/>
       <c r="DK14" s="9"/>
@@ -14130,7 +14041,7 @@
     </row>
     <row r="15" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>322</v>
@@ -14164,7 +14075,7 @@
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="28" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="N15" s="28"/>
       <c r="O15" s="28" t="s">
@@ -14219,7 +14130,7 @@
         <v>36</v>
       </c>
       <c r="AF15" s="28" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="AG15" s="28" t="s">
         <v>9</v>
@@ -14258,13 +14169,13 @@
         <v>321</v>
       </c>
       <c r="AS15" s="28" t="s">
+        <v>784</v>
+      </c>
+      <c r="AT15" s="28" t="s">
+        <v>785</v>
+      </c>
+      <c r="AU15" s="28" t="s">
         <v>786</v>
-      </c>
-      <c r="AT15" s="28" t="s">
-        <v>787</v>
-      </c>
-      <c r="AU15" s="28" t="s">
-        <v>788</v>
       </c>
       <c r="AV15" s="28" t="s">
         <v>29</v>
@@ -14302,7 +14213,7 @@
       </c>
       <c r="BH15" s="28"/>
       <c r="BI15" s="28" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="BJ15" s="28" t="s">
         <v>167</v>
@@ -14322,25 +14233,19 @@
       <c r="BO15" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP15" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="BQ15" s="28" t="s">
+      <c r="BP15" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="BR15" s="28"/>
-      <c r="BS15" s="9" t="s">
-        <v>765</v>
-      </c>
-      <c r="BT15" s="9" t="s">
-        <v>765</v>
-      </c>
+      <c r="BQ15" s="28"/>
+      <c r="BR15" s="2"/>
+      <c r="BS15" s="9"/>
+      <c r="BT15" s="9"/>
       <c r="BU15" s="9" t="s">
         <v>40</v>
       </c>
       <c r="BV15" s="9"/>
       <c r="BW15" s="9" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="BX15" s="9" t="s">
         <v>167</v>
@@ -14360,7 +14265,7 @@
       <c r="CC15" s="9"/>
       <c r="CD15" s="9"/>
       <c r="CE15" s="28" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="CF15" s="28"/>
       <c r="CG15" s="9" t="s">
@@ -14420,7 +14325,7 @@
       <c r="DE15" s="9"/>
       <c r="DF15" s="9"/>
       <c r="DG15" s="9"/>
-      <c r="DH15" s="35"/>
+      <c r="DH15" s="9"/>
       <c r="DI15" s="9"/>
       <c r="DJ15" s="9"/>
       <c r="DK15" s="9"/>
@@ -14458,7 +14363,7 @@
     </row>
     <row r="16" spans="1:146" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>745</v>
@@ -14650,21 +14555,15 @@
       <c r="BO16" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP16" s="9" t="s">
-        <v>751</v>
+      <c r="BP16" s="28" t="s">
+        <v>369</v>
       </c>
       <c r="BQ16" s="28" t="s">
-        <v>369</v>
-      </c>
-      <c r="BR16" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="BS16" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="BT16" s="9" t="s">
-        <v>321</v>
-      </c>
+      <c r="BR16" s="2"/>
+      <c r="BS16" s="9"/>
+      <c r="BT16" s="9"/>
       <c r="BU16" s="9" t="s">
         <v>40</v>
       </c>
@@ -14692,7 +14591,7 @@
       </c>
       <c r="CD16" s="9"/>
       <c r="CE16" s="28" t="s">
-        <v>752</v>
+        <v>794</v>
       </c>
       <c r="CF16" s="28"/>
       <c r="CG16" s="9" t="s">
@@ -14772,7 +14671,7 @@
       <c r="DG16" s="9" t="s">
         <v>693</v>
       </c>
-      <c r="DH16" s="35" t="s">
+      <c r="DH16" s="9" t="s">
         <v>692</v>
       </c>
       <c r="DI16" s="9" t="s">
@@ -14787,55 +14686,55 @@
       <c r="DL16" s="9" t="s">
         <v>690</v>
       </c>
-      <c r="DM16" s="66" t="s">
+      <c r="DM16" s="65" t="s">
         <v>689</v>
       </c>
-      <c r="DN16" s="66" t="s">
+      <c r="DN16" s="65" t="s">
         <v>482</v>
       </c>
-      <c r="DO16" s="66" t="s">
+      <c r="DO16" s="65" t="s">
         <v>688</v>
       </c>
-      <c r="DP16" s="65" t="s">
+      <c r="DP16" s="64" t="s">
         <v>687</v>
       </c>
-      <c r="DQ16" s="65" t="s">
+      <c r="DQ16" s="64" t="s">
         <v>686</v>
       </c>
-      <c r="DR16" s="65" t="s">
+      <c r="DR16" s="64" t="s">
         <v>685</v>
       </c>
-      <c r="DS16" s="65" t="s">
+      <c r="DS16" s="64" t="s">
         <v>684</v>
       </c>
-      <c r="DT16" s="65" t="s">
+      <c r="DT16" s="64" t="s">
         <v>683</v>
       </c>
-      <c r="DU16" s="65" t="s">
+      <c r="DU16" s="64" t="s">
         <v>682</v>
       </c>
-      <c r="DV16" s="65" t="s">
+      <c r="DV16" s="64" t="s">
         <v>681</v>
       </c>
-      <c r="DW16" s="65" t="s">
+      <c r="DW16" s="64" t="s">
         <v>680</v>
       </c>
-      <c r="DX16" s="65" t="s">
+      <c r="DX16" s="64" t="s">
         <v>679</v>
       </c>
-      <c r="DY16" s="65" t="s">
+      <c r="DY16" s="64" t="s">
         <v>678</v>
       </c>
-      <c r="DZ16" s="65" t="s">
+      <c r="DZ16" s="64" t="s">
         <v>677</v>
       </c>
-      <c r="EA16" s="65" t="s">
+      <c r="EA16" s="64" t="s">
         <v>368</v>
       </c>
-      <c r="EB16" s="65" t="s">
+      <c r="EB16" s="64" t="s">
         <v>368</v>
       </c>
-      <c r="EC16" s="65" t="s">
+      <c r="EC16" s="64" t="s">
         <v>368</v>
       </c>
       <c r="ED16" s="9" t="s">
@@ -14844,37 +14743,37 @@
       <c r="EE16" s="9" t="s">
         <v>675</v>
       </c>
-      <c r="EF16" s="66" t="s">
+      <c r="EF16" s="65" t="s">
         <v>674</v>
       </c>
-      <c r="EG16" s="66" t="s">
+      <c r="EG16" s="65" t="s">
         <v>673</v>
       </c>
-      <c r="EH16" s="66" t="s">
+      <c r="EH16" s="65" t="s">
         <v>672</v>
       </c>
-      <c r="EI16" s="66" t="s">
+      <c r="EI16" s="65" t="s">
         <v>671</v>
       </c>
-      <c r="EJ16" s="66" t="s">
+      <c r="EJ16" s="65" t="s">
         <v>670</v>
       </c>
-      <c r="EK16" s="66" t="s">
+      <c r="EK16" s="65" t="s">
         <v>669</v>
       </c>
-      <c r="EL16" s="66" t="s">
+      <c r="EL16" s="65" t="s">
         <v>668</v>
       </c>
-      <c r="EM16" s="66" t="s">
+      <c r="EM16" s="65" t="s">
         <v>667</v>
       </c>
-      <c r="EN16" s="67" t="s">
+      <c r="EN16" s="66" t="s">
         <v>666</v>
       </c>
-      <c r="EO16" s="67" t="s">
+      <c r="EO16" s="66" t="s">
         <v>494</v>
       </c>
-      <c r="EP16" s="67" t="s">
+      <c r="EP16" s="66" t="s">
         <v>665</v>
       </c>
     </row>
@@ -14882,7 +14781,7 @@
       <c r="A17" s="9" t="s">
         <v>730</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="65" t="s">
         <v>697</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -15072,13 +14971,11 @@
       <c r="BO17" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="BP17" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="BQ17" s="28" t="s">
+      <c r="BP17" s="28" t="s">
         <v>371</v>
       </c>
-      <c r="BR17" s="28"/>
+      <c r="BQ17" s="28"/>
+      <c r="BR17" s="2"/>
       <c r="BS17" s="9"/>
       <c r="BT17" s="9"/>
       <c r="BU17" s="9" t="s">
@@ -15108,7 +15005,7 @@
       </c>
       <c r="CD17" s="9"/>
       <c r="CE17" s="28" t="s">
-        <v>754</v>
+        <v>795</v>
       </c>
       <c r="CF17" s="28"/>
       <c r="CG17" s="9" t="s">
@@ -15188,7 +15085,7 @@
       <c r="DG17" s="9" t="s">
         <v>693</v>
       </c>
-      <c r="DH17" s="35" t="s">
+      <c r="DH17" s="9" t="s">
         <v>692</v>
       </c>
       <c r="DI17" s="9" t="s">
@@ -15203,55 +15100,55 @@
       <c r="DL17" s="9" t="s">
         <v>690</v>
       </c>
-      <c r="DM17" s="66" t="s">
+      <c r="DM17" s="65" t="s">
         <v>689</v>
       </c>
-      <c r="DN17" s="66" t="s">
+      <c r="DN17" s="65" t="s">
         <v>482</v>
       </c>
-      <c r="DO17" s="66" t="s">
+      <c r="DO17" s="65" t="s">
         <v>688</v>
       </c>
-      <c r="DP17" s="65" t="s">
+      <c r="DP17" s="64" t="s">
         <v>687</v>
       </c>
-      <c r="DQ17" s="65" t="s">
+      <c r="DQ17" s="64" t="s">
         <v>686</v>
       </c>
-      <c r="DR17" s="65" t="s">
+      <c r="DR17" s="64" t="s">
         <v>685</v>
       </c>
-      <c r="DS17" s="65" t="s">
+      <c r="DS17" s="64" t="s">
         <v>684</v>
       </c>
-      <c r="DT17" s="65" t="s">
+      <c r="DT17" s="64" t="s">
         <v>683</v>
       </c>
-      <c r="DU17" s="65" t="s">
+      <c r="DU17" s="64" t="s">
         <v>682</v>
       </c>
-      <c r="DV17" s="65" t="s">
+      <c r="DV17" s="64" t="s">
         <v>681</v>
       </c>
-      <c r="DW17" s="65" t="s">
+      <c r="DW17" s="64" t="s">
         <v>680</v>
       </c>
-      <c r="DX17" s="65" t="s">
+      <c r="DX17" s="64" t="s">
         <v>679</v>
       </c>
-      <c r="DY17" s="65" t="s">
+      <c r="DY17" s="64" t="s">
         <v>678</v>
       </c>
-      <c r="DZ17" s="65" t="s">
+      <c r="DZ17" s="64" t="s">
         <v>677</v>
       </c>
-      <c r="EA17" s="65" t="s">
+      <c r="EA17" s="64" t="s">
         <v>368</v>
       </c>
-      <c r="EB17" s="65" t="s">
+      <c r="EB17" s="64" t="s">
         <v>368</v>
       </c>
-      <c r="EC17" s="65" t="s">
+      <c r="EC17" s="64" t="s">
         <v>368</v>
       </c>
       <c r="ED17" s="9" t="s">
@@ -15260,37 +15157,37 @@
       <c r="EE17" s="9" t="s">
         <v>675</v>
       </c>
-      <c r="EF17" s="66" t="s">
+      <c r="EF17" s="65" t="s">
         <v>674</v>
       </c>
-      <c r="EG17" s="66" t="s">
+      <c r="EG17" s="65" t="s">
         <v>673</v>
       </c>
-      <c r="EH17" s="66" t="s">
+      <c r="EH17" s="65" t="s">
         <v>672</v>
       </c>
-      <c r="EI17" s="66" t="s">
+      <c r="EI17" s="65" t="s">
         <v>671</v>
       </c>
-      <c r="EJ17" s="66" t="s">
+      <c r="EJ17" s="65" t="s">
         <v>670</v>
       </c>
-      <c r="EK17" s="66" t="s">
+      <c r="EK17" s="65" t="s">
         <v>669</v>
       </c>
-      <c r="EL17" s="66" t="s">
+      <c r="EL17" s="65" t="s">
         <v>668</v>
       </c>
-      <c r="EM17" s="66" t="s">
+      <c r="EM17" s="65" t="s">
         <v>667</v>
       </c>
-      <c r="EN17" s="67" t="s">
+      <c r="EN17" s="66" t="s">
         <v>666</v>
       </c>
-      <c r="EO17" s="67" t="s">
+      <c r="EO17" s="66" t="s">
         <v>494</v>
       </c>
-      <c r="EP17" s="67" t="s">
+      <c r="EP17" s="66" t="s">
         <v>665</v>
       </c>
     </row>
@@ -15793,8 +15690,11 @@
       <c r="CU183"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="BG3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -17983,7 +17883,7 @@
       <c r="AA8" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AB8" s="66" t="s">
+      <c r="AB8" s="65" t="s">
         <v>732</v>
       </c>
       <c r="AC8" s="9">

</xml_diff>

<commit_message>
added adaptive auth change for institution
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12948" windowHeight="6756" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12948" windowHeight="6756" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -9236,8 +9236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EP183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AU3" sqref="AU3:AU17"/>
+    <sheetView topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="BL2" sqref="BL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16487,8 +16487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ12"/>
   <sheetViews>
-    <sheetView topLeftCell="AZ1" workbookViewId="0">
-      <selection activeCell="BH2" sqref="BH2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16781,7 +16781,7 @@
         <v>402</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>202</v>
+        <v>515</v>
       </c>
       <c r="U2" s="9" t="s">
         <v>202</v>
@@ -16955,7 +16955,7 @@
         <v>402</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>202</v>
+        <v>515</v>
       </c>
       <c r="U3" s="9" t="s">
         <v>202</v>
@@ -17127,7 +17127,7 @@
         <v>402</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>202</v>
+        <v>515</v>
       </c>
       <c r="U4" s="9" t="s">
         <v>202</v>
@@ -17299,7 +17299,7 @@
         <v>402</v>
       </c>
       <c r="T5" s="9" t="s">
-        <v>202</v>
+        <v>515</v>
       </c>
       <c r="U5" s="9" t="s">
         <v>202</v>
@@ -17473,7 +17473,7 @@
         <v>402</v>
       </c>
       <c r="T6" s="9" t="s">
-        <v>202</v>
+        <v>515</v>
       </c>
       <c r="U6" s="9" t="s">
         <v>202</v>
@@ -17647,7 +17647,7 @@
         <v>402</v>
       </c>
       <c r="T7" s="9" t="s">
-        <v>202</v>
+        <v>515</v>
       </c>
       <c r="U7" s="9" t="s">
         <v>202</v>
@@ -17821,7 +17821,7 @@
         <v>402</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>202</v>
+        <v>515</v>
       </c>
       <c r="U8" s="9" t="s">
         <v>202</v>
@@ -17995,7 +17995,7 @@
         <v>402</v>
       </c>
       <c r="T9" s="9" t="s">
-        <v>202</v>
+        <v>515</v>
       </c>
       <c r="U9" s="9" t="s">
         <v>202</v>
@@ -18167,7 +18167,7 @@
         <v>402</v>
       </c>
       <c r="T10" s="9" t="s">
-        <v>202</v>
+        <v>515</v>
       </c>
       <c r="U10" s="9" t="s">
         <v>202</v>
@@ -18339,7 +18339,7 @@
         <v>402</v>
       </c>
       <c r="T11" s="9" t="s">
-        <v>202</v>
+        <v>515</v>
       </c>
       <c r="U11" s="9" t="s">
         <v>202</v>
@@ -18513,7 +18513,7 @@
         <v>402</v>
       </c>
       <c r="T12" s="9" t="s">
-        <v>202</v>
+        <v>515</v>
       </c>
       <c r="U12" s="9" t="s">
         <v>202</v>

</xml_diff>

<commit_message>
added script for add holiday configuration screen
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3867" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3879" uniqueCount="792">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -2401,6 +2401,12 @@
   </si>
   <si>
     <t>MccCode</t>
+  </si>
+  <si>
+    <t>HolidayType</t>
+  </si>
+  <si>
+    <t>Holiday [H]</t>
   </si>
 </sst>
 </file>
@@ -16506,10 +16512,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN12"/>
+  <dimension ref="A1:BO12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="BN3" sqref="BN3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16555,9 +16561,10 @@
     <col min="59" max="59" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="46" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:67" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -16756,8 +16763,11 @@
       <c r="BN1" s="1" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="2" spans="1:66" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BO1" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="2" spans="1:67" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>396</v>
       </c>
@@ -16942,8 +16952,11 @@
       <c r="BN2" s="9" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="3" spans="1:66" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BO2" s="9" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="3" spans="1:67" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>398</v>
       </c>
@@ -17126,8 +17139,11 @@
       <c r="BN3" s="9" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="4" spans="1:66" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BO3" s="9" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="4" spans="1:67" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>411</v>
       </c>
@@ -17310,8 +17326,11 @@
       <c r="BN4" s="9" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="5" spans="1:66" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BO4" s="9" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="5" spans="1:67" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>399</v>
       </c>
@@ -17496,8 +17515,11 @@
       <c r="BN5" s="9" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="6" spans="1:66" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BO5" s="9" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="6" spans="1:67" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>410</v>
       </c>
@@ -17682,8 +17704,11 @@
       <c r="BN6" s="9" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="7" spans="1:66" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BO6" s="9" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="7" spans="1:67" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>412</v>
       </c>
@@ -17868,8 +17893,11 @@
       <c r="BN7" s="9" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="8" spans="1:66" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BO7" s="9" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="8" spans="1:67" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>413</v>
       </c>
@@ -18054,8 +18082,11 @@
       <c r="BN8" s="9" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.3">
+      <c r="BO8" s="9" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="9" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>414</v>
       </c>
@@ -18238,8 +18269,11 @@
       <c r="BN9" s="9" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="10" spans="1:66" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BO9" s="9" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="10" spans="1:67" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>415</v>
       </c>
@@ -18422,8 +18456,11 @@
       <c r="BN10" s="9" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
+      <c r="BO10" s="9" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="11" spans="1:67" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>420</v>
       </c>
@@ -18608,8 +18645,11 @@
       <c r="BN11" s="9" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="12" spans="1:66" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="BO11" s="9" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="12" spans="1:67" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>516</v>
       </c>
@@ -18801,6 +18841,9 @@
       </c>
       <c r="BN12" s="9" t="s">
         <v>788</v>
+      </c>
+      <c r="BO12" s="9" t="s">
+        <v>791</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes made as per Nidhi's request
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demo/TestData/TestData.xlsx
+++ b/src/main/resources/config/demo/TestData/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5010" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5020" uniqueCount="833">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -2531,9 +2531,6 @@
   </si>
   <si>
     <t>555522</t>
-  </si>
-  <si>
-    <t>AUTHREG</t>
   </si>
 </sst>
 </file>
@@ -3722,7 +3719,7 @@
   <dimension ref="A1:BX12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4026,10 +4023,12 @@
         <v>201</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>829</v>
+        <v>689</v>
       </c>
       <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="H2" s="9" t="s">
+        <v>795</v>
+      </c>
       <c r="I2" s="28" t="s">
         <v>134</v>
       </c>
@@ -4241,7 +4240,9 @@
         <v>689</v>
       </c>
       <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="H3" s="9" t="s">
+        <v>420</v>
+      </c>
       <c r="I3" s="28" t="s">
         <v>134</v>
       </c>
@@ -4451,7 +4452,9 @@
         <v>689</v>
       </c>
       <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="H4" s="9" t="s">
+        <v>421</v>
+      </c>
       <c r="I4" s="28" t="s">
         <v>134</v>
       </c>
@@ -4661,7 +4664,9 @@
         <v>689</v>
       </c>
       <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="H5" s="9" t="s">
+        <v>422</v>
+      </c>
       <c r="I5" s="28" t="s">
         <v>134</v>
       </c>
@@ -4873,7 +4878,9 @@
         <v>689</v>
       </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
+      <c r="H6" s="9" t="s">
+        <v>423</v>
+      </c>
       <c r="I6" s="28" t="s">
         <v>134</v>
       </c>
@@ -5085,7 +5092,9 @@
         <v>689</v>
       </c>
       <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="H7" s="9" t="s">
+        <v>733</v>
+      </c>
       <c r="I7" s="28" t="s">
         <v>134</v>
       </c>
@@ -5300,7 +5309,7 @@
         <v>832</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>833</v>
+        <v>736</v>
       </c>
       <c r="I8" s="28" t="s">
         <v>728</v>
@@ -5513,7 +5522,9 @@
         <v>689</v>
       </c>
       <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+      <c r="H9" s="9" t="s">
+        <v>424</v>
+      </c>
       <c r="I9" s="28" t="s">
         <v>134</v>
       </c>
@@ -5723,7 +5734,9 @@
         <v>689</v>
       </c>
       <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="H10" s="9" t="s">
+        <v>425</v>
+      </c>
       <c r="I10" s="28" t="s">
         <v>134</v>
       </c>
@@ -5933,7 +5946,9 @@
         <v>689</v>
       </c>
       <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+      <c r="H11" s="9" t="s">
+        <v>426</v>
+      </c>
       <c r="I11" s="28" t="s">
         <v>134</v>
       </c>
@@ -6145,7 +6160,9 @@
         <v>689</v>
       </c>
       <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="H12" s="9" t="s">
+        <v>426</v>
+      </c>
       <c r="I12" s="9" t="s">
         <v>134</v>
       </c>

</xml_diff>